<commit_message>
Ajout du niveau 4 dans le fichier excel des niveaux
</commit_message>
<xml_diff>
--- a/Niveaux.xlsx
+++ b/Niveaux.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="150" windowWidth="24915" windowHeight="12075" activeTab="2"/>
+    <workbookView xWindow="120" yWindow="150" windowWidth="24915" windowHeight="12075"/>
   </bookViews>
   <sheets>
     <sheet name="Niveau 1-5" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="214" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="235" uniqueCount="11">
   <si>
     <t>J</t>
   </si>
@@ -46,6 +46,9 @@
   </si>
   <si>
     <t>P</t>
+  </si>
+  <si>
+    <t>Niveau 4</t>
   </si>
 </sst>
 </file>
@@ -869,10 +872,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="C1:H23"/>
+  <dimension ref="C1:H34"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C18" sqref="C18:H23"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L31" sqref="L31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1123,11 +1126,118 @@
         <v>3</v>
       </c>
     </row>
+    <row r="25" spans="3:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="26" spans="3:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C26" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="D26" s="8"/>
+      <c r="E26" s="8"/>
+      <c r="F26" s="8"/>
+      <c r="G26" s="9"/>
+    </row>
+    <row r="27" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C27" s="63" t="s">
+        <v>3</v>
+      </c>
+      <c r="D27" s="53" t="s">
+        <v>3</v>
+      </c>
+      <c r="E27" s="62" t="s">
+        <v>0</v>
+      </c>
+      <c r="F27" s="68" t="s">
+        <v>2</v>
+      </c>
+      <c r="G27" s="2"/>
+    </row>
+    <row r="28" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C28" s="64" t="s">
+        <v>3</v>
+      </c>
+      <c r="D28" s="52" t="s">
+        <v>3</v>
+      </c>
+      <c r="E28" s="65" t="s">
+        <v>5</v>
+      </c>
+      <c r="F28" s="52" t="s">
+        <v>3</v>
+      </c>
+      <c r="G28" s="4"/>
+    </row>
+    <row r="29" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C29" s="66" t="s">
+        <v>8</v>
+      </c>
+      <c r="D29" s="1"/>
+      <c r="E29" s="13"/>
+      <c r="F29" s="1"/>
+      <c r="G29" s="69" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="30" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C30" s="64" t="s">
+        <v>3</v>
+      </c>
+      <c r="D30" s="52" t="s">
+        <v>3</v>
+      </c>
+      <c r="E30" s="1"/>
+      <c r="F30" s="52" t="s">
+        <v>3</v>
+      </c>
+      <c r="G30" s="4"/>
+    </row>
+    <row r="31" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C31" s="70" t="s">
+        <v>2</v>
+      </c>
+      <c r="D31" s="17" t="s">
+        <v>2</v>
+      </c>
+      <c r="E31" s="52" t="s">
+        <v>3</v>
+      </c>
+      <c r="F31" s="1"/>
+      <c r="G31" s="4"/>
+    </row>
+    <row r="32" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C32" s="3"/>
+      <c r="D32" s="1"/>
+      <c r="E32" s="52" t="s">
+        <v>3</v>
+      </c>
+      <c r="F32" s="1"/>
+      <c r="G32" s="4"/>
+    </row>
+    <row r="33" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C33" s="3"/>
+      <c r="D33" s="1"/>
+      <c r="E33" s="13" t="s">
+        <v>9</v>
+      </c>
+      <c r="F33" s="1"/>
+      <c r="G33" s="4"/>
+    </row>
+    <row r="34" spans="3:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C34" s="71" t="s">
+        <v>6</v>
+      </c>
+      <c r="D34" s="5"/>
+      <c r="E34" s="67" t="s">
+        <v>3</v>
+      </c>
+      <c r="F34" s="5"/>
+      <c r="G34" s="6"/>
+    </row>
   </sheetData>
-  <mergeCells count="3">
+  <mergeCells count="4">
     <mergeCell ref="C1:G1"/>
     <mergeCell ref="C9:G9"/>
     <mergeCell ref="C17:H17"/>
+    <mergeCell ref="C26:G26"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -1150,8 +1260,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="G1:V24"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="N28" sqref="N28"/>
+    <sheetView topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="I16" sqref="I16:M23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Correction d'un bug léger sur le mot de passe secret 879121
</commit_message>
<xml_diff>
--- a/Niveaux.xlsx
+++ b/Niveaux.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="444" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="445" uniqueCount="19">
   <si>
     <t>J</t>
   </si>
@@ -428,7 +428,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="111">
+  <cellXfs count="112">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
@@ -745,6 +745,9 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1796,7 +1799,7 @@
   <dimension ref="A1:Y35"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="E7" workbookViewId="0">
-      <selection activeCell="V16" sqref="V16"/>
+      <selection activeCell="T15" sqref="T15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3035,7 +3038,9 @@
       <c r="Q32" s="96" t="s">
         <v>3</v>
       </c>
-      <c r="R32" s="6"/>
+      <c r="R32" s="111" t="s">
+        <v>2</v>
+      </c>
       <c r="S32" s="96" t="s">
         <v>3</v>
       </c>

</xml_diff>

<commit_message>
Création du niveau 7 sur Excel - Case D = Danger
</commit_message>
<xml_diff>
--- a/Niveaux.xlsx
+++ b/Niveaux.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="445" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="490" uniqueCount="21">
   <si>
     <t>J</t>
   </si>
@@ -74,12 +74,18 @@
   <si>
     <t>8 par 9</t>
   </si>
+  <si>
+    <t>D</t>
+  </si>
+  <si>
+    <t>Niveau 7</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -150,8 +156,24 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="7" tint="-0.499984740745262"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF7030A0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -182,6 +204,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="18">
     <border>
@@ -428,7 +456,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="112">
+  <cellXfs count="124">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
@@ -748,6 +776,40 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1798,8 +1860,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Y35"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E7" workbookViewId="0">
-      <selection activeCell="T15" sqref="T15"/>
+    <sheetView tabSelected="1" topLeftCell="G7" workbookViewId="0">
+      <selection activeCell="T36" sqref="T36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2404,7 +2466,7 @@
       <c r="R16" s="44"/>
       <c r="S16" s="44"/>
     </row>
-    <row r="17" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:25" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="44"/>
       <c r="B17" s="44"/>
       <c r="C17" s="44"/>
@@ -2449,7 +2511,7 @@
       <c r="R17" s="44"/>
       <c r="S17" s="44"/>
     </row>
-    <row r="18" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A18" s="44"/>
       <c r="B18" s="44"/>
       <c r="C18" s="44"/>
@@ -2484,7 +2546,7 @@
       <c r="R18" s="44"/>
       <c r="S18" s="44"/>
     </row>
-    <row r="19" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A19" s="44"/>
       <c r="B19" s="44"/>
       <c r="C19" s="44"/>
@@ -2521,7 +2583,7 @@
       <c r="R19" s="44"/>
       <c r="S19" s="44"/>
     </row>
-    <row r="20" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A20" s="44"/>
       <c r="B20" s="44"/>
       <c r="C20" s="44"/>
@@ -2556,7 +2618,7 @@
       <c r="R20" s="44"/>
       <c r="S20" s="44"/>
     </row>
-    <row r="21" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:25" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="44"/>
       <c r="B21" s="44"/>
       <c r="C21" s="44"/>
@@ -2590,8 +2652,21 @@
       </c>
       <c r="R21" s="44"/>
       <c r="S21" s="44"/>
-    </row>
-    <row r="22" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="U21" s="60" t="s">
+        <v>3</v>
+      </c>
+      <c r="V21" s="60" t="s">
+        <v>3</v>
+      </c>
+      <c r="W21" s="115"/>
+      <c r="X21" s="60" t="s">
+        <v>3</v>
+      </c>
+      <c r="Y21" s="60" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="22" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A22" s="44"/>
       <c r="B22" s="44"/>
       <c r="C22" s="44"/>
@@ -2623,8 +2698,21 @@
       </c>
       <c r="R22" s="44"/>
       <c r="S22" s="44"/>
-    </row>
-    <row r="23" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="U22" s="60" t="s">
+        <v>3</v>
+      </c>
+      <c r="V22" s="118" t="s">
+        <v>19</v>
+      </c>
+      <c r="W22" s="117" t="s">
+        <v>6</v>
+      </c>
+      <c r="X22" s="9"/>
+      <c r="Y22" s="60" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="23" spans="1:25" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="44"/>
       <c r="B23" s="44"/>
       <c r="C23" s="44"/>
@@ -2658,8 +2746,21 @@
       </c>
       <c r="R23" s="44"/>
       <c r="S23" s="44"/>
-    </row>
-    <row r="24" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="U23" s="60" t="s">
+        <v>3</v>
+      </c>
+      <c r="V23" s="119" t="s">
+        <v>19</v>
+      </c>
+      <c r="W23" s="120" t="s">
+        <v>19</v>
+      </c>
+      <c r="X23" s="12"/>
+      <c r="Y23" s="60" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="24" spans="1:25" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A24" s="44"/>
       <c r="B24" s="44"/>
       <c r="C24" s="44"/>
@@ -2711,8 +2812,16 @@
       <c r="U24" s="60" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="25" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="V24" s="10"/>
+      <c r="W24" s="16" t="s">
+        <v>2</v>
+      </c>
+      <c r="X24" s="12"/>
+      <c r="Y24" s="60" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="25" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A25" s="44"/>
       <c r="B25" s="44"/>
       <c r="C25" s="44"/>
@@ -2760,8 +2869,18 @@
       <c r="U25" s="60" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="26" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="V25" s="10"/>
+      <c r="W25" s="120" t="s">
+        <v>19</v>
+      </c>
+      <c r="X25" s="121" t="s">
+        <v>19</v>
+      </c>
+      <c r="Y25" s="60" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="26" spans="1:25" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A26" s="44"/>
       <c r="B26" s="44"/>
       <c r="C26" s="44"/>
@@ -2805,8 +2924,16 @@
       <c r="U26" s="60" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="27" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="V26" s="10"/>
+      <c r="W26" s="16" t="s">
+        <v>2</v>
+      </c>
+      <c r="X26" s="12"/>
+      <c r="Y26" s="60" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="27" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A27" s="44"/>
       <c r="B27" s="44"/>
       <c r="C27" s="44"/>
@@ -2856,8 +2983,16 @@
       <c r="U27" s="60" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="28" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="V27" s="10"/>
+      <c r="W27" s="120" t="s">
+        <v>19</v>
+      </c>
+      <c r="X27" s="12"/>
+      <c r="Y27" s="60" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="28" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A28" s="44"/>
       <c r="B28" s="44"/>
       <c r="C28" s="44"/>
@@ -2891,8 +3026,16 @@
       <c r="U28" s="60" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="29" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="V28" s="119" t="s">
+        <v>19</v>
+      </c>
+      <c r="W28" s="11"/>
+      <c r="X28" s="77"/>
+      <c r="Y28" s="60" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="29" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A29" s="44"/>
       <c r="B29" s="44"/>
       <c r="C29" s="44"/>
@@ -2928,8 +3071,18 @@
       <c r="U29" s="60" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="30" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="V29" s="119" t="s">
+        <v>19</v>
+      </c>
+      <c r="W29" s="11"/>
+      <c r="X29" s="121" t="s">
+        <v>19</v>
+      </c>
+      <c r="Y29" s="60" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="30" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A30" s="44"/>
       <c r="B30" s="44"/>
       <c r="C30" s="44"/>
@@ -2967,8 +3120,18 @@
       <c r="U30" s="60" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="31" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="V30" s="119" t="s">
+        <v>19</v>
+      </c>
+      <c r="W30" s="51"/>
+      <c r="X30" s="121" t="s">
+        <v>19</v>
+      </c>
+      <c r="Y30" s="60" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="31" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A31" s="44"/>
       <c r="B31" s="44"/>
       <c r="C31" s="44"/>
@@ -3002,11 +3165,24 @@
       <c r="S31" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="T31" s="76" t="s">
+      <c r="T31" s="112" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="32" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="U31" s="113"/>
+      <c r="V31" s="114" t="s">
+        <v>0</v>
+      </c>
+      <c r="W31" s="16" t="s">
+        <v>2</v>
+      </c>
+      <c r="X31" s="121" t="s">
+        <v>19</v>
+      </c>
+      <c r="Y31" s="60" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="32" spans="1:25" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A32" s="44"/>
       <c r="B32" s="44"/>
       <c r="C32" s="44"/>
@@ -3050,8 +3226,18 @@
       <c r="U32" s="60" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="33" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="V32" s="70" t="s">
+        <v>2</v>
+      </c>
+      <c r="W32" s="116"/>
+      <c r="X32" s="121" t="s">
+        <v>19</v>
+      </c>
+      <c r="Y32" s="60" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="33" spans="1:25" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A33" s="44"/>
       <c r="B33" s="44"/>
       <c r="C33" s="44"/>
@@ -3095,8 +3281,18 @@
       <c r="U33" s="60" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="34" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="V33" s="13"/>
+      <c r="W33" s="122" t="s">
+        <v>19</v>
+      </c>
+      <c r="X33" s="123" t="s">
+        <v>19</v>
+      </c>
+      <c r="Y33" s="60" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="34" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A34" s="44"/>
       <c r="B34" s="44"/>
       <c r="C34" s="44"/>
@@ -3118,8 +3314,23 @@
       <c r="Q34" s="110"/>
       <c r="R34" s="44"/>
       <c r="S34" s="44"/>
-    </row>
-    <row r="35" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="U34" s="60" t="s">
+        <v>3</v>
+      </c>
+      <c r="V34" s="60" t="s">
+        <v>3</v>
+      </c>
+      <c r="W34" s="60" t="s">
+        <v>3</v>
+      </c>
+      <c r="X34" s="60" t="s">
+        <v>3</v>
+      </c>
+      <c r="Y34" s="60" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="35" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A35" s="44"/>
       <c r="B35" s="44"/>
       <c r="C35" s="44"/>
@@ -3139,9 +3350,15 @@
       <c r="Q35" s="44"/>
       <c r="R35" s="44"/>
       <c r="S35" s="44"/>
+      <c r="V35" s="109" t="s">
+        <v>20</v>
+      </c>
+      <c r="W35" s="109"/>
+      <c r="X35" s="109"/>
     </row>
   </sheetData>
-  <mergeCells count="5">
+  <mergeCells count="6">
+    <mergeCell ref="V35:X35"/>
     <mergeCell ref="O1:Q1"/>
     <mergeCell ref="F16:H16"/>
     <mergeCell ref="J7:L7"/>

</xml_diff>

<commit_message>
Création et implémentation du niveau 7. TO DO : coder le rechargement du niveau lorsque l'on marche sur une case D
</commit_message>
<xml_diff>
--- a/Niveaux.xlsx
+++ b/Niveaux.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="150" windowWidth="24915" windowHeight="12075" activeTab="2"/>
+    <workbookView xWindow="120" yWindow="150" windowWidth="24915" windowHeight="12075" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Niveau 1-5" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="490" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="514" uniqueCount="22">
   <si>
     <t>J</t>
   </si>
@@ -79,6 +79,9 @@
   </si>
   <si>
     <t>Niveau 7</t>
+  </si>
+  <si>
+    <t>12 par 3</t>
   </si>
 </sst>
 </file>
@@ -211,7 +214,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="18">
+  <borders count="19">
     <border>
       <left/>
       <right/>
@@ -452,11 +455,20 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="124">
+  <cellXfs count="125">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
@@ -810,6 +822,9 @@
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1632,10 +1647,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="C2:M11"/>
+  <dimension ref="C2:M26"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="N17" sqref="N17"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I17" sqref="I17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1848,9 +1863,125 @@
         <v>3</v>
       </c>
     </row>
+    <row r="14" spans="3:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C14" s="124" t="s">
+        <v>20</v>
+      </c>
+      <c r="D14" s="124"/>
+      <c r="E14" s="124"/>
+    </row>
+    <row r="15" spans="3:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C15" s="118" t="s">
+        <v>19</v>
+      </c>
+      <c r="D15" s="117" t="s">
+        <v>6</v>
+      </c>
+      <c r="E15" s="9"/>
+    </row>
+    <row r="16" spans="3:13" x14ac:dyDescent="0.25">
+      <c r="C16" s="119" t="s">
+        <v>19</v>
+      </c>
+      <c r="D16" s="120" t="s">
+        <v>19</v>
+      </c>
+      <c r="E16" s="12"/>
+      <c r="G16" s="85" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="17" spans="3:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C17" s="10"/>
+      <c r="D17" s="16" t="s">
+        <v>2</v>
+      </c>
+      <c r="E17" s="12"/>
+      <c r="G17" s="86" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="18" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C18" s="10"/>
+      <c r="D18" s="120" t="s">
+        <v>19</v>
+      </c>
+      <c r="E18" s="121" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="19" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C19" s="10"/>
+      <c r="D19" s="16" t="s">
+        <v>2</v>
+      </c>
+      <c r="E19" s="12"/>
+    </row>
+    <row r="20" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C20" s="10"/>
+      <c r="D20" s="120" t="s">
+        <v>19</v>
+      </c>
+      <c r="E20" s="12"/>
+    </row>
+    <row r="21" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C21" s="119" t="s">
+        <v>19</v>
+      </c>
+      <c r="D21" s="11"/>
+      <c r="E21" s="77"/>
+    </row>
+    <row r="22" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C22" s="119" t="s">
+        <v>19</v>
+      </c>
+      <c r="D22" s="11"/>
+      <c r="E22" s="121" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="23" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C23" s="119" t="s">
+        <v>19</v>
+      </c>
+      <c r="D23" s="51"/>
+      <c r="E23" s="121" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="24" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C24" s="114" t="s">
+        <v>0</v>
+      </c>
+      <c r="D24" s="16" t="s">
+        <v>2</v>
+      </c>
+      <c r="E24" s="121" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="25" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C25" s="70" t="s">
+        <v>2</v>
+      </c>
+      <c r="D25" s="116"/>
+      <c r="E25" s="121" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="26" spans="3:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C26" s="13"/>
+      <c r="D26" s="122" t="s">
+        <v>19</v>
+      </c>
+      <c r="E26" s="123" t="s">
+        <v>19</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="1">
+  <mergeCells count="2">
     <mergeCell ref="C3:K3"/>
+    <mergeCell ref="C14:E14"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1860,8 +1991,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Y35"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G7" workbookViewId="0">
-      <selection activeCell="T36" sqref="T36"/>
+    <sheetView topLeftCell="G4" workbookViewId="0">
+      <selection activeCell="V22" sqref="V22:X33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Implémentation des portes, blocs, messages (anglais et français) et du bouton dans le niveau 8
</commit_message>
<xml_diff>
--- a/Niveaux.xlsx
+++ b/Niveaux.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="514" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="663" uniqueCount="24">
   <si>
     <t>J</t>
   </si>
@@ -83,12 +83,18 @@
   <si>
     <t>12 par 3</t>
   </si>
+  <si>
+    <t>Niveau 8</t>
+  </si>
+  <si>
+    <t>8 par 7</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="11" x14ac:knownFonts="1">
+  <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -175,6 +181,13 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFC00000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="7">
     <fill>
@@ -214,7 +227,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="19">
+  <borders count="18">
     <border>
       <left/>
       <right/>
@@ -455,20 +468,11 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="125">
+  <cellXfs count="133">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
@@ -759,6 +763,39 @@
     <xf numFmtId="0" fontId="7" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -775,56 +812,47 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1136,13 +1164,13 @@
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="3:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C1" s="102" t="s">
+      <c r="C1" s="113" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="103"/>
-      <c r="E1" s="103"/>
-      <c r="F1" s="103"/>
-      <c r="G1" s="104"/>
+      <c r="D1" s="114"/>
+      <c r="E1" s="114"/>
+      <c r="F1" s="114"/>
+      <c r="G1" s="115"/>
     </row>
     <row r="2" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C2" s="35" t="s">
@@ -1211,13 +1239,13 @@
     </row>
     <row r="8" spans="3:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="9" spans="3:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C9" s="102" t="s">
+      <c r="C9" s="113" t="s">
         <v>4</v>
       </c>
-      <c r="D9" s="103"/>
-      <c r="E9" s="103"/>
-      <c r="F9" s="103"/>
-      <c r="G9" s="104"/>
+      <c r="D9" s="114"/>
+      <c r="E9" s="114"/>
+      <c r="F9" s="114"/>
+      <c r="G9" s="115"/>
     </row>
     <row r="10" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C10" s="34" t="s">
@@ -1288,14 +1316,14 @@
     </row>
     <row r="16" spans="3:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="17" spans="3:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C17" s="105" t="s">
+      <c r="C17" s="116" t="s">
         <v>7</v>
       </c>
-      <c r="D17" s="106"/>
-      <c r="E17" s="106"/>
-      <c r="F17" s="106"/>
-      <c r="G17" s="106"/>
-      <c r="H17" s="107"/>
+      <c r="D17" s="117"/>
+      <c r="E17" s="117"/>
+      <c r="F17" s="117"/>
+      <c r="G17" s="117"/>
+      <c r="H17" s="118"/>
     </row>
     <row r="18" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C18" s="21"/>
@@ -1401,13 +1429,13 @@
     </row>
     <row r="25" spans="3:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="26" spans="3:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C26" s="102" t="s">
+      <c r="C26" s="113" t="s">
         <v>10</v>
       </c>
-      <c r="D26" s="103"/>
-      <c r="E26" s="103"/>
-      <c r="F26" s="103"/>
-      <c r="G26" s="104"/>
+      <c r="D26" s="114"/>
+      <c r="E26" s="114"/>
+      <c r="F26" s="114"/>
+      <c r="G26" s="115"/>
     </row>
     <row r="27" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C27" s="63" t="s">
@@ -1513,13 +1541,13 @@
     </row>
     <row r="36" spans="3:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="37" spans="3:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C37" s="102" t="s">
+      <c r="C37" s="113" t="s">
         <v>11</v>
       </c>
-      <c r="D37" s="103"/>
-      <c r="E37" s="103"/>
-      <c r="F37" s="103"/>
-      <c r="G37" s="104"/>
+      <c r="D37" s="114"/>
+      <c r="E37" s="114"/>
+      <c r="F37" s="114"/>
+      <c r="G37" s="115"/>
     </row>
     <row r="38" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C38" s="83" t="s">
@@ -1647,27 +1675,27 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="C2:M26"/>
+  <dimension ref="C2:M37"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I17" sqref="I17"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="K44" sqref="K44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="2" spans="3:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="3" spans="3:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C3" s="102" t="s">
+      <c r="C3" s="113" t="s">
         <v>17</v>
       </c>
-      <c r="D3" s="103"/>
-      <c r="E3" s="103"/>
-      <c r="F3" s="103"/>
-      <c r="G3" s="103"/>
-      <c r="H3" s="103"/>
-      <c r="I3" s="103"/>
-      <c r="J3" s="103"/>
-      <c r="K3" s="104"/>
+      <c r="D3" s="114"/>
+      <c r="E3" s="114"/>
+      <c r="F3" s="114"/>
+      <c r="G3" s="114"/>
+      <c r="H3" s="114"/>
+      <c r="I3" s="114"/>
+      <c r="J3" s="114"/>
+      <c r="K3" s="115"/>
     </row>
     <row r="4" spans="3:13" x14ac:dyDescent="0.25">
       <c r="C4" s="87" t="s">
@@ -1863,27 +1891,28 @@
         <v>3</v>
       </c>
     </row>
+    <row r="13" spans="3:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="14" spans="3:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C14" s="124" t="s">
+      <c r="C14" s="129" t="s">
         <v>20</v>
       </c>
-      <c r="D14" s="124"/>
-      <c r="E14" s="124"/>
+      <c r="D14" s="130"/>
+      <c r="E14" s="131"/>
     </row>
     <row r="15" spans="3:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C15" s="118" t="s">
-        <v>19</v>
-      </c>
-      <c r="D15" s="117" t="s">
+      <c r="C15" s="107" t="s">
+        <v>19</v>
+      </c>
+      <c r="D15" s="106" t="s">
         <v>6</v>
       </c>
       <c r="E15" s="9"/>
     </row>
     <row r="16" spans="3:13" x14ac:dyDescent="0.25">
-      <c r="C16" s="119" t="s">
-        <v>19</v>
-      </c>
-      <c r="D16" s="120" t="s">
+      <c r="C16" s="108" t="s">
+        <v>19</v>
+      </c>
+      <c r="D16" s="109" t="s">
         <v>19</v>
       </c>
       <c r="E16" s="12"/>
@@ -1891,7 +1920,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="17" spans="3:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="3:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C17" s="10"/>
       <c r="D17" s="16" t="s">
         <v>2</v>
@@ -1901,87 +1930,246 @@
         <v>21</v>
       </c>
     </row>
-    <row r="18" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="18" spans="3:11" x14ac:dyDescent="0.25">
       <c r="C18" s="10"/>
-      <c r="D18" s="120" t="s">
-        <v>19</v>
-      </c>
-      <c r="E18" s="121" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="19" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="D18" s="109" t="s">
+        <v>19</v>
+      </c>
+      <c r="E18" s="110" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="19" spans="3:11" x14ac:dyDescent="0.25">
       <c r="C19" s="10"/>
       <c r="D19" s="16" t="s">
         <v>2</v>
       </c>
       <c r="E19" s="12"/>
     </row>
-    <row r="20" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="20" spans="3:11" x14ac:dyDescent="0.25">
       <c r="C20" s="10"/>
-      <c r="D20" s="120" t="s">
+      <c r="D20" s="109" t="s">
         <v>19</v>
       </c>
       <c r="E20" s="12"/>
     </row>
-    <row r="21" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C21" s="119" t="s">
+    <row r="21" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="C21" s="108" t="s">
         <v>19</v>
       </c>
       <c r="D21" s="11"/>
       <c r="E21" s="77"/>
     </row>
-    <row r="22" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C22" s="119" t="s">
+    <row r="22" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="C22" s="108" t="s">
         <v>19</v>
       </c>
       <c r="D22" s="11"/>
-      <c r="E22" s="121" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="23" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C23" s="119" t="s">
+      <c r="E22" s="110" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="23" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="C23" s="108" t="s">
         <v>19</v>
       </c>
       <c r="D23" s="51"/>
-      <c r="E23" s="121" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="24" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C24" s="114" t="s">
+      <c r="E23" s="110" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="24" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="C24" s="104" t="s">
         <v>0</v>
       </c>
       <c r="D24" s="16" t="s">
         <v>2</v>
       </c>
-      <c r="E24" s="121" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="25" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="E24" s="110" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="25" spans="3:11" x14ac:dyDescent="0.25">
       <c r="C25" s="70" t="s">
         <v>2</v>
       </c>
-      <c r="D25" s="116"/>
-      <c r="E25" s="121" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="26" spans="3:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D25" s="105"/>
+      <c r="E25" s="110" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="26" spans="3:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C26" s="13"/>
-      <c r="D26" s="122" t="s">
-        <v>19</v>
-      </c>
-      <c r="E26" s="123" t="s">
-        <v>19</v>
+      <c r="D26" s="111" t="s">
+        <v>19</v>
+      </c>
+      <c r="E26" s="112" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="28" spans="3:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="29" spans="3:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C29" s="129" t="s">
+        <v>22</v>
+      </c>
+      <c r="D29" s="130"/>
+      <c r="E29" s="130"/>
+      <c r="F29" s="130"/>
+      <c r="G29" s="130"/>
+      <c r="H29" s="130"/>
+      <c r="I29" s="131"/>
+    </row>
+    <row r="30" spans="3:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C30" s="124"/>
+      <c r="D30" s="8"/>
+      <c r="E30" s="126" t="s">
+        <v>19</v>
+      </c>
+      <c r="F30" s="126" t="s">
+        <v>19</v>
+      </c>
+      <c r="G30" s="8"/>
+      <c r="H30" s="8"/>
+      <c r="I30" s="9"/>
+    </row>
+    <row r="31" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="C31" s="10"/>
+      <c r="D31" s="11"/>
+      <c r="E31" s="11"/>
+      <c r="F31" s="16" t="s">
+        <v>2</v>
+      </c>
+      <c r="G31" s="11"/>
+      <c r="H31" s="65" t="s">
+        <v>5</v>
+      </c>
+      <c r="I31" s="12"/>
+      <c r="K31" s="85" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="32" spans="3:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C32" s="66" t="s">
+        <v>8</v>
+      </c>
+      <c r="D32" s="109" t="s">
+        <v>19</v>
+      </c>
+      <c r="E32" s="11"/>
+      <c r="F32" s="109" t="s">
+        <v>19</v>
+      </c>
+      <c r="G32" s="109" t="s">
+        <v>19</v>
+      </c>
+      <c r="H32" s="109" t="s">
+        <v>19</v>
+      </c>
+      <c r="I32" s="110" t="s">
+        <v>19</v>
+      </c>
+      <c r="K32" s="86" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="33" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C33" s="108" t="s">
+        <v>19</v>
+      </c>
+      <c r="D33" s="109" t="s">
+        <v>19</v>
+      </c>
+      <c r="E33" s="11"/>
+      <c r="F33" s="109" t="s">
+        <v>19</v>
+      </c>
+      <c r="G33" s="109" t="s">
+        <v>19</v>
+      </c>
+      <c r="H33" s="109" t="s">
+        <v>19</v>
+      </c>
+      <c r="I33" s="110" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="34" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C34" s="10"/>
+      <c r="D34" s="16" t="s">
+        <v>2</v>
+      </c>
+      <c r="E34" s="11"/>
+      <c r="F34" s="109"/>
+      <c r="G34" s="109"/>
+      <c r="H34" s="109"/>
+      <c r="I34" s="110" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="35" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C35" s="10"/>
+      <c r="D35" s="109" t="s">
+        <v>19</v>
+      </c>
+      <c r="E35" s="109" t="s">
+        <v>19</v>
+      </c>
+      <c r="F35" s="109" t="s">
+        <v>19</v>
+      </c>
+      <c r="G35" s="109" t="s">
+        <v>19</v>
+      </c>
+      <c r="H35" s="11"/>
+      <c r="I35" s="110" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="36" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C36" s="10"/>
+      <c r="D36" s="11"/>
+      <c r="E36" s="11"/>
+      <c r="F36" s="16" t="s">
+        <v>2</v>
+      </c>
+      <c r="G36" s="109" t="s">
+        <v>19</v>
+      </c>
+      <c r="H36" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="I36" s="110" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="37" spans="3:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C37" s="127" t="s">
+        <v>19</v>
+      </c>
+      <c r="D37" s="111" t="s">
+        <v>19</v>
+      </c>
+      <c r="E37" s="109" t="s">
+        <v>19</v>
+      </c>
+      <c r="F37" s="125" t="s">
+        <v>0</v>
+      </c>
+      <c r="G37" s="109" t="s">
+        <v>19</v>
+      </c>
+      <c r="H37" s="132" t="s">
+        <v>2</v>
+      </c>
+      <c r="I37" s="15" t="s">
+        <v>6</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="2">
+  <mergeCells count="3">
     <mergeCell ref="C3:K3"/>
     <mergeCell ref="C14:E14"/>
+    <mergeCell ref="C29:I29"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1989,27 +2177,27 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Y35"/>
+  <dimension ref="A1:AA35"/>
   <sheetViews>
-    <sheetView topLeftCell="G4" workbookViewId="0">
-      <selection activeCell="V22" sqref="V22:X33"/>
+    <sheetView topLeftCell="J1" workbookViewId="0">
+      <selection activeCell="T13" sqref="T13:Z20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="O1" s="108" t="s">
+    <row r="1" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="O1" s="120" t="s">
         <v>4</v>
       </c>
-      <c r="P1" s="108"/>
-      <c r="Q1" s="108"/>
-      <c r="U1" s="108" t="s">
+      <c r="P1" s="120"/>
+      <c r="Q1" s="120"/>
+      <c r="U1" s="120" t="s">
         <v>1</v>
       </c>
-      <c r="V1" s="108"/>
-      <c r="W1" s="108"/>
-    </row>
-    <row r="2" spans="1:25" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="V1" s="120"/>
+      <c r="W1" s="120"/>
+    </row>
+    <row r="2" spans="1:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="M2" s="58" t="s">
         <v>3</v>
       </c>
@@ -2049,8 +2237,14 @@
       <c r="Y2" s="58" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="3" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Z2" s="59" t="s">
+        <v>3</v>
+      </c>
+      <c r="AA2" s="59" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:27" x14ac:dyDescent="0.25">
       <c r="M3" s="58" t="s">
         <v>3</v>
       </c>
@@ -2078,8 +2272,14 @@
       <c r="Y3" s="58" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="4" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Z3" s="59" t="s">
+        <v>3</v>
+      </c>
+      <c r="AA3" s="59" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A4" s="44"/>
       <c r="B4" s="44"/>
       <c r="C4" s="44"/>
@@ -2123,8 +2323,14 @@
       <c r="Y4" s="59" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="5" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Z4" s="59" t="s">
+        <v>3</v>
+      </c>
+      <c r="AA4" s="59" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A5" s="44"/>
       <c r="B5" s="44"/>
       <c r="C5" s="44"/>
@@ -2160,8 +2366,14 @@
       <c r="Y5" s="58" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="6" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Z5" s="59" t="s">
+        <v>3</v>
+      </c>
+      <c r="AA5" s="59" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A6" s="44"/>
       <c r="B6" s="44"/>
       <c r="C6" s="44"/>
@@ -2205,8 +2417,14 @@
       <c r="Y6" s="58" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="7" spans="1:25" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="Z6" s="59" t="s">
+        <v>3</v>
+      </c>
+      <c r="AA6" s="59" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="44"/>
       <c r="B7" s="44"/>
       <c r="C7" s="44"/>
@@ -2216,11 +2434,11 @@
       <c r="G7" s="44"/>
       <c r="H7" s="44"/>
       <c r="I7" s="44"/>
-      <c r="J7" s="109" t="s">
+      <c r="J7" s="119" t="s">
         <v>7</v>
       </c>
-      <c r="K7" s="109"/>
-      <c r="L7" s="109"/>
+      <c r="K7" s="119"/>
+      <c r="L7" s="119"/>
       <c r="M7" s="58" t="s">
         <v>3</v>
       </c>
@@ -2252,8 +2470,14 @@
       <c r="Y7" s="58" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="8" spans="1:25" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="Z7" s="59" t="s">
+        <v>3</v>
+      </c>
+      <c r="AA7" s="59" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="8" spans="1:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="44"/>
       <c r="B8" s="44"/>
       <c r="C8" s="44"/>
@@ -2309,8 +2533,14 @@
       <c r="Y8" s="59" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="9" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Z8" s="59" t="s">
+        <v>3</v>
+      </c>
+      <c r="AA8" s="59" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="9" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A9" s="44"/>
       <c r="B9" s="44"/>
       <c r="C9" s="44"/>
@@ -2360,8 +2590,14 @@
       <c r="Y9" s="58" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="10" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Z9" s="59" t="s">
+        <v>3</v>
+      </c>
+      <c r="AA9" s="59" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="10" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A10" s="44"/>
       <c r="B10" s="44"/>
       <c r="C10" s="44"/>
@@ -2389,13 +2625,41 @@
       <c r="P10" s="89" t="s">
         <v>3</v>
       </c>
-      <c r="Q10" s="60" t="s">
-        <v>3</v>
-      </c>
-      <c r="R10" s="44"/>
-      <c r="S10" s="44"/>
-    </row>
-    <row r="11" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Q10" s="59" t="s">
+        <v>3</v>
+      </c>
+      <c r="R10" s="59" t="s">
+        <v>3</v>
+      </c>
+      <c r="S10" s="59" t="s">
+        <v>3</v>
+      </c>
+      <c r="T10" s="59" t="s">
+        <v>3</v>
+      </c>
+      <c r="U10" s="59" t="s">
+        <v>3</v>
+      </c>
+      <c r="V10" s="59" t="s">
+        <v>3</v>
+      </c>
+      <c r="W10" s="59" t="s">
+        <v>3</v>
+      </c>
+      <c r="X10" s="59" t="s">
+        <v>3</v>
+      </c>
+      <c r="Y10" s="59" t="s">
+        <v>3</v>
+      </c>
+      <c r="Z10" s="59" t="s">
+        <v>3</v>
+      </c>
+      <c r="AA10" s="59" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="11" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A11" s="44"/>
       <c r="B11" s="44"/>
       <c r="C11" s="44"/>
@@ -2420,13 +2684,41 @@
       <c r="P11" s="89" t="s">
         <v>3</v>
       </c>
-      <c r="Q11" s="60" t="s">
-        <v>3</v>
-      </c>
-      <c r="R11" s="44"/>
-      <c r="S11" s="44"/>
-    </row>
-    <row r="12" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Q11" s="59" t="s">
+        <v>3</v>
+      </c>
+      <c r="R11" s="59" t="s">
+        <v>3</v>
+      </c>
+      <c r="S11" s="59" t="s">
+        <v>3</v>
+      </c>
+      <c r="T11" s="59" t="s">
+        <v>3</v>
+      </c>
+      <c r="U11" s="59" t="s">
+        <v>3</v>
+      </c>
+      <c r="V11" s="59" t="s">
+        <v>3</v>
+      </c>
+      <c r="W11" s="59" t="s">
+        <v>3</v>
+      </c>
+      <c r="X11" s="59" t="s">
+        <v>3</v>
+      </c>
+      <c r="Y11" s="59" t="s">
+        <v>3</v>
+      </c>
+      <c r="Z11" s="59" t="s">
+        <v>3</v>
+      </c>
+      <c r="AA11" s="59" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="12" spans="1:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="44"/>
       <c r="B12" s="44"/>
       <c r="C12" s="44"/>
@@ -2449,13 +2741,41 @@
       <c r="P12" s="89" t="s">
         <v>3</v>
       </c>
-      <c r="Q12" s="60" t="s">
-        <v>3</v>
-      </c>
-      <c r="R12" s="44"/>
-      <c r="S12" s="44"/>
-    </row>
-    <row r="13" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Q12" s="59" t="s">
+        <v>3</v>
+      </c>
+      <c r="R12" s="59" t="s">
+        <v>3</v>
+      </c>
+      <c r="S12" s="59" t="s">
+        <v>3</v>
+      </c>
+      <c r="T12" s="59" t="s">
+        <v>3</v>
+      </c>
+      <c r="U12" s="59" t="s">
+        <v>3</v>
+      </c>
+      <c r="V12" s="59" t="s">
+        <v>3</v>
+      </c>
+      <c r="W12" s="59" t="s">
+        <v>3</v>
+      </c>
+      <c r="X12" s="59" t="s">
+        <v>3</v>
+      </c>
+      <c r="Y12" s="59" t="s">
+        <v>3</v>
+      </c>
+      <c r="Z12" s="59" t="s">
+        <v>3</v>
+      </c>
+      <c r="AA12" s="59" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="13" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A13" s="44"/>
       <c r="B13" s="44"/>
       <c r="C13" s="44"/>
@@ -2484,13 +2804,31 @@
       <c r="P13" s="89" t="s">
         <v>3</v>
       </c>
-      <c r="Q13" s="60" t="s">
-        <v>3</v>
-      </c>
-      <c r="R13" s="44"/>
-      <c r="S13" s="44"/>
-    </row>
-    <row r="14" spans="1:25" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="Q13" s="59" t="s">
+        <v>3</v>
+      </c>
+      <c r="R13" s="59" t="s">
+        <v>3</v>
+      </c>
+      <c r="S13" s="59" t="s">
+        <v>3</v>
+      </c>
+      <c r="T13" s="124"/>
+      <c r="U13" s="8"/>
+      <c r="V13" s="126" t="s">
+        <v>19</v>
+      </c>
+      <c r="W13" s="126" t="s">
+        <v>19</v>
+      </c>
+      <c r="X13" s="8"/>
+      <c r="Y13" s="8"/>
+      <c r="Z13" s="9"/>
+      <c r="AA13" s="59" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="14" spans="1:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="44"/>
       <c r="B14" s="44"/>
       <c r="C14" s="44"/>
@@ -2521,13 +2859,31 @@
       <c r="P14" s="90" t="s">
         <v>3</v>
       </c>
-      <c r="Q14" s="60" t="s">
-        <v>3</v>
-      </c>
-      <c r="R14" s="44"/>
-      <c r="S14" s="44"/>
-    </row>
-    <row r="15" spans="1:25" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="Q14" s="59" t="s">
+        <v>3</v>
+      </c>
+      <c r="R14" s="59" t="s">
+        <v>3</v>
+      </c>
+      <c r="S14" s="59" t="s">
+        <v>3</v>
+      </c>
+      <c r="T14" s="10"/>
+      <c r="U14" s="11"/>
+      <c r="V14" s="11"/>
+      <c r="W14" s="16" t="s">
+        <v>2</v>
+      </c>
+      <c r="X14" s="11"/>
+      <c r="Y14" s="65" t="s">
+        <v>5</v>
+      </c>
+      <c r="Z14" s="12"/>
+      <c r="AA14" s="59" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="15" spans="1:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="44"/>
       <c r="B15" s="44"/>
       <c r="C15" s="44"/>
@@ -2556,23 +2912,49 @@
       <c r="P15" s="60" t="s">
         <v>3</v>
       </c>
-      <c r="Q15" s="60" t="s">
-        <v>3</v>
-      </c>
-      <c r="R15" s="44"/>
-      <c r="S15" s="44"/>
-    </row>
-    <row r="16" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Q15" s="59" t="s">
+        <v>3</v>
+      </c>
+      <c r="R15" s="59" t="s">
+        <v>3</v>
+      </c>
+      <c r="S15" s="59" t="s">
+        <v>3</v>
+      </c>
+      <c r="T15" s="66" t="s">
+        <v>8</v>
+      </c>
+      <c r="U15" s="109" t="s">
+        <v>19</v>
+      </c>
+      <c r="V15" s="11"/>
+      <c r="W15" s="109" t="s">
+        <v>19</v>
+      </c>
+      <c r="X15" s="109" t="s">
+        <v>19</v>
+      </c>
+      <c r="Y15" s="109" t="s">
+        <v>19</v>
+      </c>
+      <c r="Z15" s="110" t="s">
+        <v>19</v>
+      </c>
+      <c r="AA15" s="59" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="16" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A16" s="44"/>
       <c r="B16" s="44"/>
       <c r="C16" s="44"/>
       <c r="D16" s="44"/>
       <c r="E16" s="44"/>
-      <c r="F16" s="109" t="s">
+      <c r="F16" s="119" t="s">
         <v>11</v>
       </c>
-      <c r="G16" s="109"/>
-      <c r="H16" s="109"/>
+      <c r="G16" s="119"/>
+      <c r="H16" s="119"/>
       <c r="I16" s="44"/>
       <c r="J16" s="44"/>
       <c r="K16" s="60" t="s">
@@ -2591,13 +2973,39 @@
         <v>2</v>
       </c>
       <c r="P16" s="9"/>
-      <c r="Q16" s="60" t="s">
-        <v>3</v>
-      </c>
-      <c r="R16" s="44"/>
-      <c r="S16" s="44"/>
-    </row>
-    <row r="17" spans="1:25" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="Q16" s="59" t="s">
+        <v>3</v>
+      </c>
+      <c r="R16" s="59" t="s">
+        <v>3</v>
+      </c>
+      <c r="S16" s="59" t="s">
+        <v>3</v>
+      </c>
+      <c r="T16" s="108" t="s">
+        <v>19</v>
+      </c>
+      <c r="U16" s="109" t="s">
+        <v>19</v>
+      </c>
+      <c r="V16" s="11"/>
+      <c r="W16" s="109" t="s">
+        <v>19</v>
+      </c>
+      <c r="X16" s="109" t="s">
+        <v>19</v>
+      </c>
+      <c r="Y16" s="109" t="s">
+        <v>19</v>
+      </c>
+      <c r="Z16" s="110" t="s">
+        <v>19</v>
+      </c>
+      <c r="AA16" s="59" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="17" spans="1:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="44"/>
       <c r="B17" s="44"/>
       <c r="C17" s="44"/>
@@ -2636,13 +3044,31 @@
         <v>3</v>
       </c>
       <c r="P17" s="12"/>
-      <c r="Q17" s="60" t="s">
-        <v>3</v>
-      </c>
-      <c r="R17" s="44"/>
-      <c r="S17" s="44"/>
-    </row>
-    <row r="18" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Q17" s="59" t="s">
+        <v>3</v>
+      </c>
+      <c r="R17" s="59" t="s">
+        <v>3</v>
+      </c>
+      <c r="S17" s="59" t="s">
+        <v>3</v>
+      </c>
+      <c r="T17" s="10"/>
+      <c r="U17" s="16" t="s">
+        <v>2</v>
+      </c>
+      <c r="V17" s="11"/>
+      <c r="W17" s="109"/>
+      <c r="X17" s="109"/>
+      <c r="Y17" s="109"/>
+      <c r="Z17" s="110" t="s">
+        <v>19</v>
+      </c>
+      <c r="AA17" s="59" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="18" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A18" s="44"/>
       <c r="B18" s="44"/>
       <c r="C18" s="44"/>
@@ -2671,13 +3097,37 @@
       <c r="P18" s="69" t="s">
         <v>2</v>
       </c>
-      <c r="Q18" s="60" t="s">
-        <v>3</v>
-      </c>
-      <c r="R18" s="44"/>
-      <c r="S18" s="44"/>
-    </row>
-    <row r="19" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Q18" s="59" t="s">
+        <v>3</v>
+      </c>
+      <c r="R18" s="59" t="s">
+        <v>3</v>
+      </c>
+      <c r="S18" s="59" t="s">
+        <v>3</v>
+      </c>
+      <c r="T18" s="10"/>
+      <c r="U18" s="109" t="s">
+        <v>19</v>
+      </c>
+      <c r="V18" s="109" t="s">
+        <v>19</v>
+      </c>
+      <c r="W18" s="109" t="s">
+        <v>19</v>
+      </c>
+      <c r="X18" s="109" t="s">
+        <v>19</v>
+      </c>
+      <c r="Y18" s="11"/>
+      <c r="Z18" s="110" t="s">
+        <v>19</v>
+      </c>
+      <c r="AA18" s="59" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="19" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A19" s="44"/>
       <c r="B19" s="44"/>
       <c r="C19" s="44"/>
@@ -2708,13 +3158,35 @@
         <v>3</v>
       </c>
       <c r="P19" s="12"/>
-      <c r="Q19" s="60" t="s">
-        <v>3</v>
-      </c>
-      <c r="R19" s="44"/>
-      <c r="S19" s="44"/>
-    </row>
-    <row r="20" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Q19" s="59" t="s">
+        <v>3</v>
+      </c>
+      <c r="R19" s="59" t="s">
+        <v>3</v>
+      </c>
+      <c r="S19" s="59" t="s">
+        <v>3</v>
+      </c>
+      <c r="T19" s="10"/>
+      <c r="U19" s="11"/>
+      <c r="V19" s="11"/>
+      <c r="W19" s="16" t="s">
+        <v>2</v>
+      </c>
+      <c r="X19" s="109" t="s">
+        <v>19</v>
+      </c>
+      <c r="Y19" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="Z19" s="110" t="s">
+        <v>19</v>
+      </c>
+      <c r="AA19" s="59" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="20" spans="1:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="44"/>
       <c r="B20" s="44"/>
       <c r="C20" s="44"/>
@@ -2743,13 +3215,38 @@
       </c>
       <c r="O20" s="11"/>
       <c r="P20" s="12"/>
-      <c r="Q20" s="60" t="s">
-        <v>3</v>
-      </c>
-      <c r="R20" s="44"/>
-      <c r="S20" s="44"/>
-    </row>
-    <row r="21" spans="1:25" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="Q20" s="59" t="s">
+        <v>3</v>
+      </c>
+      <c r="R20" s="59" t="s">
+        <v>3</v>
+      </c>
+      <c r="S20" s="59" t="s">
+        <v>3</v>
+      </c>
+      <c r="T20" s="127" t="s">
+        <v>19</v>
+      </c>
+      <c r="U20" s="111" t="s">
+        <v>19</v>
+      </c>
+      <c r="V20" s="109" t="s">
+        <v>19</v>
+      </c>
+      <c r="W20" s="125" t="s">
+        <v>0</v>
+      </c>
+      <c r="X20" s="109" t="s">
+        <v>19</v>
+      </c>
+      <c r="Y20" s="132" t="s">
+        <v>2</v>
+      </c>
+      <c r="Z20" s="15" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="21" spans="1:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="44"/>
       <c r="B21" s="44"/>
       <c r="C21" s="44"/>
@@ -2778,26 +3275,33 @@
       </c>
       <c r="O21" s="11"/>
       <c r="P21" s="12"/>
-      <c r="Q21" s="60" t="s">
-        <v>3</v>
-      </c>
-      <c r="R21" s="44"/>
-      <c r="S21" s="44"/>
-      <c r="U21" s="60" t="s">
-        <v>3</v>
-      </c>
-      <c r="V21" s="60" t="s">
-        <v>3</v>
-      </c>
-      <c r="W21" s="115"/>
-      <c r="X21" s="60" t="s">
-        <v>3</v>
-      </c>
-      <c r="Y21" s="60" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="22" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Q21" s="59" t="s">
+        <v>3</v>
+      </c>
+      <c r="R21" s="59" t="s">
+        <v>3</v>
+      </c>
+      <c r="S21" s="59" t="s">
+        <v>3</v>
+      </c>
+      <c r="T21" s="59" t="s">
+        <v>3</v>
+      </c>
+      <c r="U21" s="59" t="s">
+        <v>3</v>
+      </c>
+      <c r="V21" s="59" t="s">
+        <v>3</v>
+      </c>
+      <c r="W21" s="122"/>
+      <c r="X21" s="59" t="s">
+        <v>3</v>
+      </c>
+      <c r="Y21" s="59" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="22" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A22" s="44"/>
       <c r="B22" s="44"/>
       <c r="C22" s="44"/>
@@ -2824,26 +3328,33 @@
       </c>
       <c r="O22" s="11"/>
       <c r="P22" s="12"/>
-      <c r="Q22" s="60" t="s">
-        <v>3</v>
-      </c>
-      <c r="R22" s="44"/>
-      <c r="S22" s="44"/>
-      <c r="U22" s="60" t="s">
-        <v>3</v>
-      </c>
-      <c r="V22" s="118" t="s">
-        <v>19</v>
-      </c>
-      <c r="W22" s="117" t="s">
+      <c r="Q22" s="59" t="s">
+        <v>3</v>
+      </c>
+      <c r="R22" s="59" t="s">
+        <v>3</v>
+      </c>
+      <c r="S22" s="59" t="s">
+        <v>3</v>
+      </c>
+      <c r="T22" s="59" t="s">
+        <v>3</v>
+      </c>
+      <c r="U22" s="59" t="s">
+        <v>3</v>
+      </c>
+      <c r="V22" s="107" t="s">
+        <v>19</v>
+      </c>
+      <c r="W22" s="123" t="s">
         <v>6</v>
       </c>
       <c r="X22" s="9"/>
-      <c r="Y22" s="60" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="23" spans="1:25" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="Y22" s="59" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="23" spans="1:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="44"/>
       <c r="B23" s="44"/>
       <c r="C23" s="44"/>
@@ -2872,26 +3383,33 @@
       </c>
       <c r="O23" s="14"/>
       <c r="P23" s="15"/>
-      <c r="Q23" s="60" t="s">
-        <v>3</v>
-      </c>
-      <c r="R23" s="44"/>
-      <c r="S23" s="44"/>
-      <c r="U23" s="60" t="s">
-        <v>3</v>
-      </c>
-      <c r="V23" s="119" t="s">
-        <v>19</v>
-      </c>
-      <c r="W23" s="120" t="s">
+      <c r="Q23" s="59" t="s">
+        <v>3</v>
+      </c>
+      <c r="R23" s="59" t="s">
+        <v>3</v>
+      </c>
+      <c r="S23" s="59" t="s">
+        <v>3</v>
+      </c>
+      <c r="T23" s="59" t="s">
+        <v>3</v>
+      </c>
+      <c r="U23" s="59" t="s">
+        <v>3</v>
+      </c>
+      <c r="V23" s="108" t="s">
+        <v>19</v>
+      </c>
+      <c r="W23" s="109" t="s">
         <v>19</v>
       </c>
       <c r="X23" s="12"/>
-      <c r="Y23" s="60" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="24" spans="1:25" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="Y23" s="59" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="24" spans="1:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A24" s="44"/>
       <c r="B24" s="44"/>
       <c r="C24" s="44"/>
@@ -2928,19 +3446,19 @@
       <c r="P24" s="60" t="s">
         <v>3</v>
       </c>
-      <c r="Q24" s="60" t="s">
-        <v>3</v>
-      </c>
-      <c r="R24" s="60" t="s">
-        <v>3</v>
-      </c>
-      <c r="S24" s="60" t="s">
-        <v>3</v>
-      </c>
-      <c r="T24" s="60" t="s">
-        <v>3</v>
-      </c>
-      <c r="U24" s="60" t="s">
+      <c r="Q24" s="59" t="s">
+        <v>3</v>
+      </c>
+      <c r="R24" s="59" t="s">
+        <v>3</v>
+      </c>
+      <c r="S24" s="59" t="s">
+        <v>3</v>
+      </c>
+      <c r="T24" s="59" t="s">
+        <v>3</v>
+      </c>
+      <c r="U24" s="59" t="s">
         <v>3</v>
       </c>
       <c r="V24" s="10"/>
@@ -2948,11 +3466,11 @@
         <v>2</v>
       </c>
       <c r="X24" s="12"/>
-      <c r="Y24" s="60" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="25" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Y24" s="59" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="25" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A25" s="44"/>
       <c r="B25" s="44"/>
       <c r="C25" s="44"/>
@@ -2997,21 +3515,21 @@
       <c r="T25" s="101" t="s">
         <v>3</v>
       </c>
-      <c r="U25" s="60" t="s">
+      <c r="U25" s="59" t="s">
         <v>3</v>
       </c>
       <c r="V25" s="10"/>
-      <c r="W25" s="120" t="s">
-        <v>19</v>
-      </c>
-      <c r="X25" s="121" t="s">
-        <v>19</v>
-      </c>
-      <c r="Y25" s="60" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="26" spans="1:25" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="W25" s="109" t="s">
+        <v>19</v>
+      </c>
+      <c r="X25" s="110" t="s">
+        <v>19</v>
+      </c>
+      <c r="Y25" s="59" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="26" spans="1:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A26" s="44"/>
       <c r="B26" s="44"/>
       <c r="C26" s="44"/>
@@ -3052,7 +3570,7 @@
       <c r="T26" s="98" t="s">
         <v>3</v>
       </c>
-      <c r="U26" s="60" t="s">
+      <c r="U26" s="59" t="s">
         <v>3</v>
       </c>
       <c r="V26" s="10"/>
@@ -3060,11 +3578,11 @@
         <v>2</v>
       </c>
       <c r="X26" s="12"/>
-      <c r="Y26" s="60" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="27" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Y26" s="59" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="27" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A27" s="44"/>
       <c r="B27" s="44"/>
       <c r="C27" s="44"/>
@@ -3111,19 +3629,19 @@
       <c r="T27" s="98" t="s">
         <v>3</v>
       </c>
-      <c r="U27" s="60" t="s">
+      <c r="U27" s="59" t="s">
         <v>3</v>
       </c>
       <c r="V27" s="10"/>
-      <c r="W27" s="120" t="s">
+      <c r="W27" s="109" t="s">
         <v>19</v>
       </c>
       <c r="X27" s="12"/>
-      <c r="Y27" s="60" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="28" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Y27" s="59" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="28" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A28" s="44"/>
       <c r="B28" s="44"/>
       <c r="C28" s="44"/>
@@ -3154,19 +3672,19 @@
       <c r="T28" s="98" t="s">
         <v>3</v>
       </c>
-      <c r="U28" s="60" t="s">
-        <v>3</v>
-      </c>
-      <c r="V28" s="119" t="s">
+      <c r="U28" s="59" t="s">
+        <v>3</v>
+      </c>
+      <c r="V28" s="108" t="s">
         <v>19</v>
       </c>
       <c r="W28" s="11"/>
       <c r="X28" s="77"/>
-      <c r="Y28" s="60" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="29" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Y28" s="59" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="29" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A29" s="44"/>
       <c r="B29" s="44"/>
       <c r="C29" s="44"/>
@@ -3199,21 +3717,21 @@
       <c r="T29" s="98" t="s">
         <v>3</v>
       </c>
-      <c r="U29" s="60" t="s">
-        <v>3</v>
-      </c>
-      <c r="V29" s="119" t="s">
+      <c r="U29" s="59" t="s">
+        <v>3</v>
+      </c>
+      <c r="V29" s="108" t="s">
         <v>19</v>
       </c>
       <c r="W29" s="11"/>
-      <c r="X29" s="121" t="s">
-        <v>19</v>
-      </c>
-      <c r="Y29" s="60" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="30" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="X29" s="110" t="s">
+        <v>19</v>
+      </c>
+      <c r="Y29" s="59" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="30" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A30" s="44"/>
       <c r="B30" s="44"/>
       <c r="C30" s="44"/>
@@ -3248,21 +3766,21 @@
       <c r="T30" s="98" t="s">
         <v>3</v>
       </c>
-      <c r="U30" s="60" t="s">
-        <v>3</v>
-      </c>
-      <c r="V30" s="119" t="s">
+      <c r="U30" s="59" t="s">
+        <v>3</v>
+      </c>
+      <c r="V30" s="108" t="s">
         <v>19</v>
       </c>
       <c r="W30" s="51"/>
-      <c r="X30" s="121" t="s">
-        <v>19</v>
-      </c>
-      <c r="Y30" s="60" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="31" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="X30" s="110" t="s">
+        <v>19</v>
+      </c>
+      <c r="Y30" s="59" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="31" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A31" s="44"/>
       <c r="B31" s="44"/>
       <c r="C31" s="44"/>
@@ -3296,24 +3814,24 @@
       <c r="S31" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="T31" s="112" t="s">
+      <c r="T31" s="103" t="s">
         <v>6</v>
       </c>
-      <c r="U31" s="113"/>
-      <c r="V31" s="114" t="s">
+      <c r="U31" s="128"/>
+      <c r="V31" s="104" t="s">
         <v>0</v>
       </c>
       <c r="W31" s="16" t="s">
         <v>2</v>
       </c>
-      <c r="X31" s="121" t="s">
-        <v>19</v>
-      </c>
-      <c r="Y31" s="60" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="32" spans="1:25" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="X31" s="110" t="s">
+        <v>19</v>
+      </c>
+      <c r="Y31" s="59" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="32" spans="1:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A32" s="44"/>
       <c r="B32" s="44"/>
       <c r="C32" s="44"/>
@@ -3345,7 +3863,7 @@
       <c r="Q32" s="96" t="s">
         <v>3</v>
       </c>
-      <c r="R32" s="111" t="s">
+      <c r="R32" s="102" t="s">
         <v>2</v>
       </c>
       <c r="S32" s="96" t="s">
@@ -3354,17 +3872,17 @@
       <c r="T32" s="97" t="s">
         <v>3</v>
       </c>
-      <c r="U32" s="60" t="s">
+      <c r="U32" s="59" t="s">
         <v>3</v>
       </c>
       <c r="V32" s="70" t="s">
         <v>2</v>
       </c>
-      <c r="W32" s="116"/>
-      <c r="X32" s="121" t="s">
-        <v>19</v>
-      </c>
-      <c r="Y32" s="60" t="s">
+      <c r="W32" s="105"/>
+      <c r="X32" s="110" t="s">
+        <v>19</v>
+      </c>
+      <c r="Y32" s="59" t="s">
         <v>3</v>
       </c>
     </row>
@@ -3385,41 +3903,41 @@
       <c r="L33" s="60" t="s">
         <v>3</v>
       </c>
-      <c r="M33" s="60" t="s">
-        <v>3</v>
-      </c>
-      <c r="N33" s="60" t="s">
-        <v>3</v>
-      </c>
-      <c r="O33" s="60" t="s">
-        <v>3</v>
-      </c>
-      <c r="P33" s="60" t="s">
-        <v>3</v>
-      </c>
-      <c r="Q33" s="60" t="s">
-        <v>3</v>
-      </c>
-      <c r="R33" s="60" t="s">
-        <v>3</v>
-      </c>
-      <c r="S33" s="60" t="s">
-        <v>3</v>
-      </c>
-      <c r="T33" s="60" t="s">
-        <v>3</v>
-      </c>
-      <c r="U33" s="60" t="s">
+      <c r="M33" s="59" t="s">
+        <v>3</v>
+      </c>
+      <c r="N33" s="59" t="s">
+        <v>3</v>
+      </c>
+      <c r="O33" s="59" t="s">
+        <v>3</v>
+      </c>
+      <c r="P33" s="59" t="s">
+        <v>3</v>
+      </c>
+      <c r="Q33" s="59" t="s">
+        <v>3</v>
+      </c>
+      <c r="R33" s="59" t="s">
+        <v>3</v>
+      </c>
+      <c r="S33" s="59" t="s">
+        <v>3</v>
+      </c>
+      <c r="T33" s="59" t="s">
+        <v>3</v>
+      </c>
+      <c r="U33" s="59" t="s">
         <v>3</v>
       </c>
       <c r="V33" s="13"/>
-      <c r="W33" s="122" t="s">
-        <v>19</v>
-      </c>
-      <c r="X33" s="123" t="s">
-        <v>19</v>
-      </c>
-      <c r="Y33" s="60" t="s">
+      <c r="W33" s="111" t="s">
+        <v>19</v>
+      </c>
+      <c r="X33" s="112" t="s">
+        <v>19</v>
+      </c>
+      <c r="Y33" s="59" t="s">
         <v>3</v>
       </c>
     </row>
@@ -3438,26 +3956,26 @@
       <c r="L34" s="44"/>
       <c r="M34" s="44"/>
       <c r="N34" s="44"/>
-      <c r="O34" s="110" t="s">
+      <c r="O34" s="121" t="s">
         <v>17</v>
       </c>
-      <c r="P34" s="110"/>
-      <c r="Q34" s="110"/>
+      <c r="P34" s="121"/>
+      <c r="Q34" s="121"/>
       <c r="R34" s="44"/>
       <c r="S34" s="44"/>
-      <c r="U34" s="60" t="s">
-        <v>3</v>
-      </c>
-      <c r="V34" s="60" t="s">
-        <v>3</v>
-      </c>
-      <c r="W34" s="60" t="s">
-        <v>3</v>
-      </c>
-      <c r="X34" s="60" t="s">
-        <v>3</v>
-      </c>
-      <c r="Y34" s="60" t="s">
+      <c r="U34" s="59" t="s">
+        <v>3</v>
+      </c>
+      <c r="V34" s="59" t="s">
+        <v>3</v>
+      </c>
+      <c r="W34" s="59" t="s">
+        <v>3</v>
+      </c>
+      <c r="X34" s="59" t="s">
+        <v>3</v>
+      </c>
+      <c r="Y34" s="59" t="s">
         <v>3</v>
       </c>
     </row>
@@ -3481,11 +3999,11 @@
       <c r="Q35" s="44"/>
       <c r="R35" s="44"/>
       <c r="S35" s="44"/>
-      <c r="V35" s="109" t="s">
+      <c r="V35" s="119" t="s">
         <v>20</v>
       </c>
-      <c r="W35" s="109"/>
-      <c r="X35" s="109"/>
+      <c r="W35" s="119"/>
+      <c r="X35" s="119"/>
     </row>
   </sheetData>
   <mergeCells count="6">

</xml_diff>

<commit_message>
Niveau 9 entièrement implémenté
</commit_message>
<xml_diff>
--- a/Niveaux.xlsx
+++ b/Niveaux.xlsx
@@ -4,19 +4,20 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="150" windowWidth="24915" windowHeight="12075" activeTab="1"/>
+    <workbookView xWindow="120" yWindow="150" windowWidth="24915" windowHeight="12075" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Niveau 1-5" sheetId="1" r:id="rId1"/>
     <sheet name="Niveau 6-10" sheetId="2" r:id="rId2"/>
     <sheet name="Tous_les_niveaux" sheetId="3" r:id="rId3"/>
+    <sheet name="Carte des niveaux" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="663" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="677" uniqueCount="26">
   <si>
     <t>J</t>
   </si>
@@ -88,6 +89,12 @@
   </si>
   <si>
     <t>8 par 7</t>
+  </si>
+  <si>
+    <t>m</t>
+  </si>
+  <si>
+    <t>Niveau 9</t>
   </si>
 </sst>
 </file>
@@ -227,7 +234,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="18">
+  <borders count="19">
     <border>
       <left/>
       <right/>
@@ -468,11 +475,26 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="133">
+  <cellXfs count="142">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
@@ -796,6 +818,31 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -813,6 +860,15 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -823,35 +879,26 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1164,13 +1211,13 @@
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="3:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C1" s="113" t="s">
+      <c r="C1" s="122" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="114"/>
-      <c r="E1" s="114"/>
-      <c r="F1" s="114"/>
-      <c r="G1" s="115"/>
+      <c r="D1" s="123"/>
+      <c r="E1" s="123"/>
+      <c r="F1" s="123"/>
+      <c r="G1" s="124"/>
     </row>
     <row r="2" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C2" s="35" t="s">
@@ -1239,13 +1286,13 @@
     </row>
     <row r="8" spans="3:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="9" spans="3:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C9" s="113" t="s">
+      <c r="C9" s="122" t="s">
         <v>4</v>
       </c>
-      <c r="D9" s="114"/>
-      <c r="E9" s="114"/>
-      <c r="F9" s="114"/>
-      <c r="G9" s="115"/>
+      <c r="D9" s="123"/>
+      <c r="E9" s="123"/>
+      <c r="F9" s="123"/>
+      <c r="G9" s="124"/>
     </row>
     <row r="10" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C10" s="34" t="s">
@@ -1316,14 +1363,14 @@
     </row>
     <row r="16" spans="3:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="17" spans="3:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C17" s="116" t="s">
+      <c r="C17" s="125" t="s">
         <v>7</v>
       </c>
-      <c r="D17" s="117"/>
-      <c r="E17" s="117"/>
-      <c r="F17" s="117"/>
-      <c r="G17" s="117"/>
-      <c r="H17" s="118"/>
+      <c r="D17" s="126"/>
+      <c r="E17" s="126"/>
+      <c r="F17" s="126"/>
+      <c r="G17" s="126"/>
+      <c r="H17" s="127"/>
     </row>
     <row r="18" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C18" s="21"/>
@@ -1429,13 +1476,13 @@
     </row>
     <row r="25" spans="3:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="26" spans="3:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C26" s="113" t="s">
+      <c r="C26" s="122" t="s">
         <v>10</v>
       </c>
-      <c r="D26" s="114"/>
-      <c r="E26" s="114"/>
-      <c r="F26" s="114"/>
-      <c r="G26" s="115"/>
+      <c r="D26" s="123"/>
+      <c r="E26" s="123"/>
+      <c r="F26" s="123"/>
+      <c r="G26" s="124"/>
     </row>
     <row r="27" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C27" s="63" t="s">
@@ -1541,13 +1588,13 @@
     </row>
     <row r="36" spans="3:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="37" spans="3:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C37" s="113" t="s">
+      <c r="C37" s="122" t="s">
         <v>11</v>
       </c>
-      <c r="D37" s="114"/>
-      <c r="E37" s="114"/>
-      <c r="F37" s="114"/>
-      <c r="G37" s="115"/>
+      <c r="D37" s="123"/>
+      <c r="E37" s="123"/>
+      <c r="F37" s="123"/>
+      <c r="G37" s="124"/>
     </row>
     <row r="38" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C38" s="83" t="s">
@@ -1677,7 +1724,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="C2:M37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+    <sheetView topLeftCell="A10" workbookViewId="0">
       <selection activeCell="K44" sqref="K44"/>
     </sheetView>
   </sheetViews>
@@ -1685,17 +1732,17 @@
   <sheetData>
     <row r="2" spans="3:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="3" spans="3:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C3" s="113" t="s">
+      <c r="C3" s="122" t="s">
         <v>17</v>
       </c>
-      <c r="D3" s="114"/>
-      <c r="E3" s="114"/>
-      <c r="F3" s="114"/>
-      <c r="G3" s="114"/>
-      <c r="H3" s="114"/>
-      <c r="I3" s="114"/>
-      <c r="J3" s="114"/>
-      <c r="K3" s="115"/>
+      <c r="D3" s="123"/>
+      <c r="E3" s="123"/>
+      <c r="F3" s="123"/>
+      <c r="G3" s="123"/>
+      <c r="H3" s="123"/>
+      <c r="I3" s="123"/>
+      <c r="J3" s="123"/>
+      <c r="K3" s="124"/>
     </row>
     <row r="4" spans="3:13" x14ac:dyDescent="0.25">
       <c r="C4" s="87" t="s">
@@ -1893,11 +1940,11 @@
     </row>
     <row r="13" spans="3:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="14" spans="3:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C14" s="129" t="s">
+      <c r="C14" s="128" t="s">
         <v>20</v>
       </c>
-      <c r="D14" s="130"/>
-      <c r="E14" s="131"/>
+      <c r="D14" s="129"/>
+      <c r="E14" s="130"/>
     </row>
     <row r="15" spans="3:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C15" s="107" t="s">
@@ -2009,23 +2056,23 @@
     </row>
     <row r="28" spans="3:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="29" spans="3:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C29" s="129" t="s">
+      <c r="C29" s="128" t="s">
         <v>22</v>
       </c>
-      <c r="D29" s="130"/>
-      <c r="E29" s="130"/>
-      <c r="F29" s="130"/>
-      <c r="G29" s="130"/>
-      <c r="H29" s="130"/>
-      <c r="I29" s="131"/>
+      <c r="D29" s="129"/>
+      <c r="E29" s="129"/>
+      <c r="F29" s="129"/>
+      <c r="G29" s="129"/>
+      <c r="H29" s="129"/>
+      <c r="I29" s="130"/>
     </row>
     <row r="30" spans="3:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C30" s="124"/>
+      <c r="C30" s="115"/>
       <c r="D30" s="8"/>
-      <c r="E30" s="126" t="s">
-        <v>19</v>
-      </c>
-      <c r="F30" s="126" t="s">
+      <c r="E30" s="117" t="s">
+        <v>19</v>
+      </c>
+      <c r="F30" s="117" t="s">
         <v>19</v>
       </c>
       <c r="G30" s="8"/>
@@ -2143,7 +2190,7 @@
       </c>
     </row>
     <row r="37" spans="3:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C37" s="127" t="s">
+      <c r="C37" s="118" t="s">
         <v>19</v>
       </c>
       <c r="D37" s="111" t="s">
@@ -2152,13 +2199,13 @@
       <c r="E37" s="109" t="s">
         <v>19</v>
       </c>
-      <c r="F37" s="125" t="s">
+      <c r="F37" s="116" t="s">
         <v>0</v>
       </c>
       <c r="G37" s="109" t="s">
         <v>19</v>
       </c>
-      <c r="H37" s="132" t="s">
+      <c r="H37" s="120" t="s">
         <v>2</v>
       </c>
       <c r="I37" s="15" t="s">
@@ -2177,25 +2224,25 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AA35"/>
+  <dimension ref="A1:AF35"/>
   <sheetViews>
-    <sheetView topLeftCell="J1" workbookViewId="0">
-      <selection activeCell="T13" sqref="T13:Z20"/>
+    <sheetView tabSelected="1" topLeftCell="P1" workbookViewId="0">
+      <selection activeCell="AG16" sqref="AG16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="O1" s="120" t="s">
+      <c r="O1" s="132" t="s">
         <v>4</v>
       </c>
-      <c r="P1" s="120"/>
-      <c r="Q1" s="120"/>
-      <c r="U1" s="120" t="s">
+      <c r="P1" s="132"/>
+      <c r="Q1" s="132"/>
+      <c r="U1" s="132" t="s">
         <v>1</v>
       </c>
-      <c r="V1" s="120"/>
-      <c r="W1" s="120"/>
+      <c r="V1" s="132"/>
+      <c r="W1" s="132"/>
     </row>
     <row r="2" spans="1:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="M2" s="58" t="s">
@@ -2434,11 +2481,11 @@
       <c r="G7" s="44"/>
       <c r="H7" s="44"/>
       <c r="I7" s="44"/>
-      <c r="J7" s="119" t="s">
+      <c r="J7" s="131" t="s">
         <v>7</v>
       </c>
-      <c r="K7" s="119"/>
-      <c r="L7" s="119"/>
+      <c r="K7" s="131"/>
+      <c r="L7" s="131"/>
       <c r="M7" s="58" t="s">
         <v>3</v>
       </c>
@@ -2659,7 +2706,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="11" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="44"/>
       <c r="B11" s="44"/>
       <c r="C11" s="44"/>
@@ -2756,15 +2803,11 @@
       <c r="U12" s="59" t="s">
         <v>3</v>
       </c>
-      <c r="V12" s="59" t="s">
-        <v>3</v>
-      </c>
-      <c r="W12" s="59" t="s">
-        <v>3</v>
-      </c>
-      <c r="X12" s="59" t="s">
-        <v>3</v>
-      </c>
+      <c r="V12" s="136" t="s">
+        <v>22</v>
+      </c>
+      <c r="W12" s="137"/>
+      <c r="X12" s="138"/>
       <c r="Y12" s="59" t="s">
         <v>3</v>
       </c>
@@ -2813,12 +2856,12 @@
       <c r="S13" s="59" t="s">
         <v>3</v>
       </c>
-      <c r="T13" s="124"/>
+      <c r="T13" s="115"/>
       <c r="U13" s="8"/>
-      <c r="V13" s="126" t="s">
-        <v>19</v>
-      </c>
-      <c r="W13" s="126" t="s">
+      <c r="V13" s="117" t="s">
+        <v>19</v>
+      </c>
+      <c r="W13" s="117" t="s">
         <v>19</v>
       </c>
       <c r="X13" s="8"/>
@@ -2950,11 +2993,11 @@
       <c r="C16" s="44"/>
       <c r="D16" s="44"/>
       <c r="E16" s="44"/>
-      <c r="F16" s="119" t="s">
+      <c r="F16" s="131" t="s">
         <v>11</v>
       </c>
-      <c r="G16" s="119"/>
-      <c r="H16" s="119"/>
+      <c r="G16" s="131"/>
+      <c r="H16" s="131"/>
       <c r="I16" s="44"/>
       <c r="J16" s="44"/>
       <c r="K16" s="60" t="s">
@@ -3005,7 +3048,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="17" spans="1:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:32" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="44"/>
       <c r="B17" s="44"/>
       <c r="C17" s="44"/>
@@ -3068,7 +3111,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="18" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A18" s="44"/>
       <c r="B18" s="44"/>
       <c r="C18" s="44"/>
@@ -3127,7 +3170,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="19" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A19" s="44"/>
       <c r="B19" s="44"/>
       <c r="C19" s="44"/>
@@ -3186,7 +3229,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="20" spans="1:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:32" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="44"/>
       <c r="B20" s="44"/>
       <c r="C20" s="44"/>
@@ -3224,29 +3267,29 @@
       <c r="S20" s="59" t="s">
         <v>3</v>
       </c>
-      <c r="T20" s="127" t="s">
+      <c r="T20" s="118" t="s">
         <v>19</v>
       </c>
       <c r="U20" s="111" t="s">
         <v>19</v>
       </c>
-      <c r="V20" s="109" t="s">
-        <v>19</v>
-      </c>
-      <c r="W20" s="125" t="s">
+      <c r="V20" s="111" t="s">
+        <v>19</v>
+      </c>
+      <c r="W20" s="116" t="s">
         <v>0</v>
       </c>
-      <c r="X20" s="109" t="s">
-        <v>19</v>
-      </c>
-      <c r="Y20" s="132" t="s">
+      <c r="X20" s="111" t="s">
+        <v>19</v>
+      </c>
+      <c r="Y20" s="120" t="s">
         <v>2</v>
       </c>
-      <c r="Z20" s="15" t="s">
+      <c r="Z20" s="134" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="21" spans="1:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:32" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="44"/>
       <c r="B21" s="44"/>
       <c r="C21" s="44"/>
@@ -3293,15 +3336,21 @@
       <c r="V21" s="59" t="s">
         <v>3</v>
       </c>
-      <c r="W21" s="122"/>
+      <c r="W21" s="113"/>
       <c r="X21" s="59" t="s">
         <v>3</v>
       </c>
       <c r="Y21" s="59" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="22" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="Z21" s="135"/>
+      <c r="AB21" s="122" t="s">
+        <v>25</v>
+      </c>
+      <c r="AC21" s="123"/>
+      <c r="AD21" s="124"/>
+    </row>
+    <row r="22" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A22" s="44"/>
       <c r="B22" s="44"/>
       <c r="C22" s="44"/>
@@ -3346,15 +3395,30 @@
       <c r="V22" s="107" t="s">
         <v>19</v>
       </c>
-      <c r="W22" s="123" t="s">
+      <c r="W22" s="114" t="s">
         <v>6</v>
       </c>
       <c r="X22" s="9"/>
       <c r="Y22" s="59" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="23" spans="1:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="Z22" s="139" t="s">
+        <v>0</v>
+      </c>
+      <c r="AA22" s="117" t="s">
+        <v>19</v>
+      </c>
+      <c r="AB22" s="8"/>
+      <c r="AC22" s="8"/>
+      <c r="AD22" s="8"/>
+      <c r="AE22" s="117" t="s">
+        <v>19</v>
+      </c>
+      <c r="AF22" s="141" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="23" spans="1:32" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="44"/>
       <c r="B23" s="44"/>
       <c r="C23" s="44"/>
@@ -3408,8 +3472,19 @@
       <c r="Y23" s="59" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="24" spans="1:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="Z23" s="10"/>
+      <c r="AA23" s="11"/>
+      <c r="AB23" s="109" t="s">
+        <v>19</v>
+      </c>
+      <c r="AC23" s="11"/>
+      <c r="AD23" s="109" t="s">
+        <v>19</v>
+      </c>
+      <c r="AE23" s="11"/>
+      <c r="AF23" s="5"/>
+    </row>
+    <row r="24" spans="1:32" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A24" s="44"/>
       <c r="B24" s="44"/>
       <c r="C24" s="44"/>
@@ -3469,8 +3544,21 @@
       <c r="Y24" s="59" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="25" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="Z24" s="108" t="s">
+        <v>19</v>
+      </c>
+      <c r="AA24" s="11"/>
+      <c r="AB24" s="11"/>
+      <c r="AC24" s="109" t="s">
+        <v>19</v>
+      </c>
+      <c r="AD24" s="11"/>
+      <c r="AE24" s="11"/>
+      <c r="AF24" s="110" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="25" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A25" s="44"/>
       <c r="B25" s="44"/>
       <c r="C25" s="44"/>
@@ -3528,8 +3616,19 @@
       <c r="Y25" s="59" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="26" spans="1:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="Z25" s="10"/>
+      <c r="AA25" s="109" t="s">
+        <v>19</v>
+      </c>
+      <c r="AB25" s="11"/>
+      <c r="AC25" s="11"/>
+      <c r="AD25" s="11"/>
+      <c r="AE25" s="109" t="s">
+        <v>19</v>
+      </c>
+      <c r="AF25" s="5"/>
+    </row>
+    <row r="26" spans="1:32" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A26" s="44"/>
       <c r="B26" s="44"/>
       <c r="C26" s="44"/>
@@ -3581,8 +3680,23 @@
       <c r="Y26" s="59" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="27" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="Z26" s="71" t="s">
+        <v>6</v>
+      </c>
+      <c r="AA26" s="14"/>
+      <c r="AB26" s="111" t="s">
+        <v>19</v>
+      </c>
+      <c r="AC26" s="111" t="s">
+        <v>19</v>
+      </c>
+      <c r="AD26" s="111" t="s">
+        <v>19</v>
+      </c>
+      <c r="AE26" s="14"/>
+      <c r="AF26" s="7"/>
+    </row>
+    <row r="27" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A27" s="44"/>
       <c r="B27" s="44"/>
       <c r="C27" s="44"/>
@@ -3641,7 +3755,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="28" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A28" s="44"/>
       <c r="B28" s="44"/>
       <c r="C28" s="44"/>
@@ -3684,7 +3798,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="29" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A29" s="44"/>
       <c r="B29" s="44"/>
       <c r="C29" s="44"/>
@@ -3731,7 +3845,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="30" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A30" s="44"/>
       <c r="B30" s="44"/>
       <c r="C30" s="44"/>
@@ -3780,7 +3894,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="31" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A31" s="44"/>
       <c r="B31" s="44"/>
       <c r="C31" s="44"/>
@@ -3817,7 +3931,7 @@
       <c r="T31" s="103" t="s">
         <v>6</v>
       </c>
-      <c r="U31" s="128"/>
+      <c r="U31" s="119"/>
       <c r="V31" s="104" t="s">
         <v>0</v>
       </c>
@@ -3831,7 +3945,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="32" spans="1:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:32" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A32" s="44"/>
       <c r="B32" s="44"/>
       <c r="C32" s="44"/>
@@ -3956,11 +4070,11 @@
       <c r="L34" s="44"/>
       <c r="M34" s="44"/>
       <c r="N34" s="44"/>
-      <c r="O34" s="121" t="s">
+      <c r="O34" s="133" t="s">
         <v>17</v>
       </c>
-      <c r="P34" s="121"/>
-      <c r="Q34" s="121"/>
+      <c r="P34" s="133"/>
+      <c r="Q34" s="133"/>
       <c r="R34" s="44"/>
       <c r="S34" s="44"/>
       <c r="U34" s="59" t="s">
@@ -3999,22 +4113,323 @@
       <c r="Q35" s="44"/>
       <c r="R35" s="44"/>
       <c r="S35" s="44"/>
-      <c r="V35" s="119" t="s">
+      <c r="V35" s="131" t="s">
         <v>20</v>
       </c>
-      <c r="W35" s="119"/>
-      <c r="X35" s="119"/>
+      <c r="W35" s="131"/>
+      <c r="X35" s="131"/>
     </row>
   </sheetData>
-  <mergeCells count="6">
+  <mergeCells count="8">
+    <mergeCell ref="AB21:AD21"/>
     <mergeCell ref="V35:X35"/>
     <mergeCell ref="O1:Q1"/>
     <mergeCell ref="F16:H16"/>
     <mergeCell ref="J7:L7"/>
     <mergeCell ref="O34:Q34"/>
     <mergeCell ref="U1:W1"/>
+    <mergeCell ref="V12:X12"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="F2:Q20"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="O22" sqref="O22"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="2" spans="6:17" x14ac:dyDescent="0.25">
+      <c r="F2" s="121"/>
+      <c r="G2" s="121"/>
+      <c r="H2" s="121"/>
+      <c r="I2" s="121"/>
+      <c r="J2" s="121"/>
+      <c r="K2" s="121"/>
+      <c r="L2" s="121"/>
+      <c r="M2" s="121"/>
+      <c r="N2" s="121"/>
+      <c r="O2" s="121"/>
+      <c r="P2" s="121"/>
+      <c r="Q2" s="121"/>
+    </row>
+    <row r="3" spans="6:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F3" s="121"/>
+      <c r="G3" s="121"/>
+      <c r="H3" s="121"/>
+      <c r="I3" s="121"/>
+      <c r="J3" s="121"/>
+      <c r="K3" s="121"/>
+      <c r="L3" s="121"/>
+      <c r="M3" s="121"/>
+      <c r="N3" s="121"/>
+      <c r="O3" s="121"/>
+      <c r="P3" s="121"/>
+      <c r="Q3" s="121"/>
+    </row>
+    <row r="4" spans="6:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F4" s="121"/>
+      <c r="G4" s="121"/>
+      <c r="H4" s="140">
+        <v>2</v>
+      </c>
+      <c r="I4" s="140">
+        <v>1</v>
+      </c>
+      <c r="J4" s="121"/>
+      <c r="K4" s="121"/>
+      <c r="L4" s="121"/>
+      <c r="M4" s="121"/>
+      <c r="N4" s="121"/>
+      <c r="O4" s="121"/>
+      <c r="P4" s="121"/>
+      <c r="Q4" s="121"/>
+    </row>
+    <row r="5" spans="6:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F5" s="121"/>
+      <c r="G5" s="121"/>
+      <c r="H5" s="140">
+        <v>3</v>
+      </c>
+      <c r="I5" s="121"/>
+      <c r="J5" s="121"/>
+      <c r="K5" s="121"/>
+      <c r="L5" s="121"/>
+      <c r="M5" s="121"/>
+      <c r="N5" s="121"/>
+      <c r="O5" s="121"/>
+      <c r="P5" s="121"/>
+      <c r="Q5" s="121"/>
+    </row>
+    <row r="6" spans="6:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F6" s="121"/>
+      <c r="G6" s="121"/>
+      <c r="H6" s="140">
+        <v>4</v>
+      </c>
+      <c r="I6" s="140">
+        <v>8</v>
+      </c>
+      <c r="J6" s="121"/>
+      <c r="K6" s="121"/>
+      <c r="L6" s="121"/>
+      <c r="M6" s="121"/>
+      <c r="N6" s="121"/>
+      <c r="O6" s="121"/>
+      <c r="P6" s="121"/>
+      <c r="Q6" s="121"/>
+    </row>
+    <row r="7" spans="6:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F7" s="121"/>
+      <c r="G7" s="140">
+        <v>5</v>
+      </c>
+      <c r="H7" s="140">
+        <v>6</v>
+      </c>
+      <c r="I7" s="140">
+        <v>7</v>
+      </c>
+      <c r="J7" s="140">
+        <v>9</v>
+      </c>
+      <c r="K7" s="121"/>
+      <c r="L7" s="121"/>
+      <c r="M7" s="121"/>
+      <c r="N7" s="121"/>
+      <c r="O7" s="121"/>
+      <c r="P7" s="121"/>
+      <c r="Q7" s="121"/>
+    </row>
+    <row r="8" spans="6:17" x14ac:dyDescent="0.25">
+      <c r="F8" s="121"/>
+      <c r="G8" s="121"/>
+      <c r="H8" s="121"/>
+      <c r="I8" s="121"/>
+      <c r="J8" s="121"/>
+      <c r="K8" s="121"/>
+      <c r="L8" s="121"/>
+      <c r="M8" s="121"/>
+      <c r="N8" s="121"/>
+      <c r="O8" s="121"/>
+      <c r="P8" s="121"/>
+      <c r="Q8" s="121"/>
+    </row>
+    <row r="9" spans="6:17" x14ac:dyDescent="0.25">
+      <c r="F9" s="121"/>
+      <c r="G9" s="121"/>
+      <c r="H9" s="121"/>
+      <c r="I9" s="121"/>
+      <c r="J9" s="121"/>
+      <c r="K9" s="121"/>
+      <c r="L9" s="121"/>
+      <c r="M9" s="121"/>
+      <c r="N9" s="121"/>
+      <c r="O9" s="121"/>
+      <c r="P9" s="121"/>
+      <c r="Q9" s="121"/>
+    </row>
+    <row r="10" spans="6:17" x14ac:dyDescent="0.25">
+      <c r="F10" s="121"/>
+      <c r="G10" s="121"/>
+      <c r="H10" s="121"/>
+      <c r="I10" s="121"/>
+      <c r="J10" s="121"/>
+      <c r="K10" s="121"/>
+      <c r="L10" s="121"/>
+      <c r="M10" s="121"/>
+      <c r="N10" s="121"/>
+      <c r="O10" s="121"/>
+      <c r="P10" s="121"/>
+      <c r="Q10" s="121"/>
+    </row>
+    <row r="11" spans="6:17" x14ac:dyDescent="0.25">
+      <c r="F11" s="121"/>
+      <c r="G11" s="121"/>
+      <c r="H11" s="121"/>
+      <c r="I11" s="121"/>
+      <c r="J11" s="121"/>
+      <c r="K11" s="121"/>
+      <c r="L11" s="121"/>
+      <c r="M11" s="121"/>
+      <c r="N11" s="121"/>
+      <c r="O11" s="121"/>
+      <c r="P11" s="121"/>
+      <c r="Q11" s="121"/>
+    </row>
+    <row r="12" spans="6:17" x14ac:dyDescent="0.25">
+      <c r="F12" s="121"/>
+      <c r="G12" s="121"/>
+      <c r="H12" s="121"/>
+      <c r="I12" s="121"/>
+      <c r="J12" s="121"/>
+      <c r="K12" s="121"/>
+      <c r="L12" s="121"/>
+      <c r="M12" s="121"/>
+      <c r="N12" s="121"/>
+      <c r="O12" s="121"/>
+      <c r="P12" s="121"/>
+      <c r="Q12" s="121"/>
+    </row>
+    <row r="13" spans="6:17" x14ac:dyDescent="0.25">
+      <c r="F13" s="121"/>
+      <c r="G13" s="121"/>
+      <c r="H13" s="121"/>
+      <c r="I13" s="121"/>
+      <c r="J13" s="121"/>
+      <c r="K13" s="121"/>
+      <c r="L13" s="121"/>
+      <c r="M13" s="121"/>
+      <c r="N13" s="121"/>
+      <c r="O13" s="121"/>
+      <c r="P13" s="121"/>
+      <c r="Q13" s="121"/>
+    </row>
+    <row r="14" spans="6:17" x14ac:dyDescent="0.25">
+      <c r="F14" s="121"/>
+      <c r="G14" s="121"/>
+      <c r="H14" s="121"/>
+      <c r="I14" s="121"/>
+      <c r="J14" s="121"/>
+      <c r="K14" s="121"/>
+      <c r="L14" s="121"/>
+      <c r="M14" s="121"/>
+      <c r="N14" s="121"/>
+      <c r="O14" s="121"/>
+      <c r="P14" s="121"/>
+      <c r="Q14" s="121"/>
+    </row>
+    <row r="15" spans="6:17" x14ac:dyDescent="0.25">
+      <c r="F15" s="121"/>
+      <c r="G15" s="121"/>
+      <c r="H15" s="121"/>
+      <c r="I15" s="121"/>
+      <c r="J15" s="121"/>
+      <c r="K15" s="121"/>
+      <c r="L15" s="121"/>
+      <c r="M15" s="121"/>
+      <c r="N15" s="121"/>
+      <c r="O15" s="121"/>
+      <c r="P15" s="121"/>
+      <c r="Q15" s="121"/>
+    </row>
+    <row r="16" spans="6:17" x14ac:dyDescent="0.25">
+      <c r="F16" s="121"/>
+      <c r="G16" s="121"/>
+      <c r="H16" s="121"/>
+      <c r="I16" s="121"/>
+      <c r="J16" s="121"/>
+      <c r="K16" s="121"/>
+      <c r="L16" s="121"/>
+      <c r="M16" s="121"/>
+      <c r="N16" s="121"/>
+      <c r="O16" s="121"/>
+      <c r="P16" s="121"/>
+      <c r="Q16" s="121"/>
+    </row>
+    <row r="17" spans="6:17" x14ac:dyDescent="0.25">
+      <c r="F17" s="121"/>
+      <c r="G17" s="121"/>
+      <c r="H17" s="121"/>
+      <c r="I17" s="121"/>
+      <c r="J17" s="121"/>
+      <c r="K17" s="121"/>
+      <c r="L17" s="121"/>
+      <c r="M17" s="121"/>
+      <c r="N17" s="121"/>
+      <c r="O17" s="121"/>
+      <c r="P17" s="121"/>
+      <c r="Q17" s="121"/>
+    </row>
+    <row r="18" spans="6:17" x14ac:dyDescent="0.25">
+      <c r="F18" s="121"/>
+      <c r="G18" s="121"/>
+      <c r="H18" s="121"/>
+      <c r="I18" s="121"/>
+      <c r="J18" s="121"/>
+      <c r="K18" s="121"/>
+      <c r="L18" s="121"/>
+      <c r="M18" s="121"/>
+      <c r="N18" s="121"/>
+      <c r="O18" s="121"/>
+      <c r="P18" s="121"/>
+      <c r="Q18" s="121"/>
+    </row>
+    <row r="19" spans="6:17" x14ac:dyDescent="0.25">
+      <c r="F19" s="121"/>
+      <c r="G19" s="121"/>
+      <c r="H19" s="121"/>
+      <c r="I19" s="121"/>
+      <c r="J19" s="121"/>
+      <c r="K19" s="121"/>
+      <c r="L19" s="121"/>
+      <c r="M19" s="121"/>
+      <c r="N19" s="121"/>
+      <c r="O19" s="121"/>
+      <c r="P19" s="121"/>
+      <c r="Q19" s="121"/>
+    </row>
+    <row r="20" spans="6:17" x14ac:dyDescent="0.25">
+      <c r="F20" s="121"/>
+      <c r="G20" s="121"/>
+      <c r="H20" s="121"/>
+      <c r="I20" s="121"/>
+      <c r="J20" s="121"/>
+      <c r="K20" s="121"/>
+      <c r="L20" s="121"/>
+      <c r="M20" s="121"/>
+      <c r="N20" s="121"/>
+      <c r="O20" s="121"/>
+      <c r="P20" s="121"/>
+      <c r="Q20" s="121"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
TO DO : régler le bug d'affichage de la manivelle au niveau 9 quand le niveau vient d'être reconfiguré suite à l'activation de la manivelle
</commit_message>
<xml_diff>
--- a/Niveaux.xlsx
+++ b/Niveaux.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="150" windowWidth="24915" windowHeight="12075" activeTab="2"/>
+    <workbookView xWindow="120" yWindow="150" windowWidth="24915" windowHeight="12075" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Niveau 1-5" sheetId="1" r:id="rId1"/>
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="677" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="712" uniqueCount="27">
   <si>
     <t>J</t>
   </si>
@@ -95,6 +95,9 @@
   </si>
   <si>
     <t>Niveau 9</t>
+  </si>
+  <si>
+    <t>Configuration 2 du niveau 9</t>
   </si>
 </sst>
 </file>
@@ -1722,10 +1725,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="C2:M37"/>
+  <dimension ref="C2:M54"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="K44" sqref="K44"/>
+    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="K42" sqref="K42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2212,11 +2215,191 @@
         <v>6</v>
       </c>
     </row>
+    <row r="40" spans="3:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="41" spans="3:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C41" s="122" t="s">
+        <v>25</v>
+      </c>
+      <c r="D41" s="123"/>
+      <c r="E41" s="123"/>
+      <c r="F41" s="123"/>
+      <c r="G41" s="123"/>
+      <c r="H41" s="123"/>
+      <c r="I41" s="124"/>
+    </row>
+    <row r="42" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C42" s="139" t="s">
+        <v>0</v>
+      </c>
+      <c r="D42" s="117" t="s">
+        <v>19</v>
+      </c>
+      <c r="E42" s="8"/>
+      <c r="F42" s="8"/>
+      <c r="G42" s="8"/>
+      <c r="H42" s="117" t="s">
+        <v>19</v>
+      </c>
+      <c r="I42" s="141" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="43" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C43" s="10"/>
+      <c r="D43" s="11"/>
+      <c r="E43" s="109" t="s">
+        <v>19</v>
+      </c>
+      <c r="F43" s="11"/>
+      <c r="G43" s="109" t="s">
+        <v>19</v>
+      </c>
+      <c r="H43" s="11"/>
+      <c r="I43" s="5"/>
+    </row>
+    <row r="44" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C44" s="108" t="s">
+        <v>19</v>
+      </c>
+      <c r="D44" s="16" t="s">
+        <v>2</v>
+      </c>
+      <c r="E44" s="11"/>
+      <c r="F44" s="109" t="s">
+        <v>19</v>
+      </c>
+      <c r="G44" s="11"/>
+      <c r="H44" s="11"/>
+      <c r="I44" s="110" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="45" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C45" s="10"/>
+      <c r="D45" s="109" t="s">
+        <v>19</v>
+      </c>
+      <c r="E45" s="11"/>
+      <c r="F45" s="11"/>
+      <c r="G45" s="11"/>
+      <c r="H45" s="109" t="s">
+        <v>19</v>
+      </c>
+      <c r="I45" s="5"/>
+    </row>
+    <row r="46" spans="3:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C46" s="71" t="s">
+        <v>6</v>
+      </c>
+      <c r="D46" s="14"/>
+      <c r="E46" s="111" t="s">
+        <v>19</v>
+      </c>
+      <c r="F46" s="111" t="s">
+        <v>19</v>
+      </c>
+      <c r="G46" s="111" t="s">
+        <v>19</v>
+      </c>
+      <c r="H46" s="14"/>
+      <c r="I46" s="7"/>
+    </row>
+    <row r="48" spans="3:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="49" spans="3:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C49" s="122" t="s">
+        <v>26</v>
+      </c>
+      <c r="D49" s="123"/>
+      <c r="E49" s="123"/>
+      <c r="F49" s="123"/>
+      <c r="G49" s="123"/>
+      <c r="H49" s="123"/>
+      <c r="I49" s="124"/>
+    </row>
+    <row r="50" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C50" s="139" t="s">
+        <v>0</v>
+      </c>
+      <c r="D50" s="117" t="s">
+        <v>19</v>
+      </c>
+      <c r="E50" s="8"/>
+      <c r="F50" s="8"/>
+      <c r="G50" s="8"/>
+      <c r="H50" s="117" t="s">
+        <v>19</v>
+      </c>
+      <c r="I50" s="141" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="51" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C51" s="10"/>
+      <c r="D51" s="109" t="s">
+        <v>19</v>
+      </c>
+      <c r="E51" s="109"/>
+      <c r="F51" s="109" t="s">
+        <v>19</v>
+      </c>
+      <c r="G51" s="109"/>
+      <c r="H51" s="109" t="s">
+        <v>19</v>
+      </c>
+      <c r="I51" s="5"/>
+    </row>
+    <row r="52" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C52" s="108"/>
+      <c r="D52" s="16" t="s">
+        <v>2</v>
+      </c>
+      <c r="E52" s="11"/>
+      <c r="F52" s="109" t="s">
+        <v>19</v>
+      </c>
+      <c r="G52" s="11"/>
+      <c r="H52" s="109" t="s">
+        <v>19</v>
+      </c>
+      <c r="I52" s="110"/>
+    </row>
+    <row r="53" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C53" s="10"/>
+      <c r="D53" s="109" t="s">
+        <v>19</v>
+      </c>
+      <c r="E53" s="11"/>
+      <c r="F53" s="109" t="s">
+        <v>19</v>
+      </c>
+      <c r="G53" s="11"/>
+      <c r="H53" s="109" t="s">
+        <v>19</v>
+      </c>
+      <c r="I53" s="5"/>
+    </row>
+    <row r="54" spans="3:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C54" s="71" t="s">
+        <v>6</v>
+      </c>
+      <c r="D54" s="111" t="s">
+        <v>19</v>
+      </c>
+      <c r="E54" s="111"/>
+      <c r="F54" s="111" t="s">
+        <v>19</v>
+      </c>
+      <c r="G54" s="111"/>
+      <c r="H54" s="14"/>
+      <c r="I54" s="7"/>
+    </row>
   </sheetData>
-  <mergeCells count="3">
+  <mergeCells count="5">
     <mergeCell ref="C3:K3"/>
     <mergeCell ref="C14:E14"/>
     <mergeCell ref="C29:I29"/>
+    <mergeCell ref="C41:I41"/>
+    <mergeCell ref="C49:I49"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2226,8 +2409,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AF35"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="P1" workbookViewId="0">
-      <selection activeCell="AG16" sqref="AG16"/>
+    <sheetView topLeftCell="P1" workbookViewId="0">
+      <selection activeCell="Z22" sqref="Z22:AF26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3547,7 +3730,9 @@
       <c r="Z24" s="108" t="s">
         <v>19</v>
       </c>
-      <c r="AA24" s="11"/>
+      <c r="AA24" s="16" t="s">
+        <v>2</v>
+      </c>
       <c r="AB24" s="11"/>
       <c r="AC24" s="109" t="s">
         <v>19</v>

</xml_diff>

<commit_message>
Fin du niveau 9
</commit_message>
<xml_diff>
--- a/Niveaux.xlsx
+++ b/Niveaux.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="150" windowWidth="24915" windowHeight="12075" activeTab="1"/>
+    <workbookView xWindow="120" yWindow="150" windowWidth="24915" windowHeight="12075" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Niveau 1-5" sheetId="1" r:id="rId1"/>
@@ -497,7 +497,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="142">
+  <cellXfs count="143">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
@@ -902,6 +902,9 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1727,7 +1730,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="C2:M54"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
+    <sheetView topLeftCell="A28" workbookViewId="0">
       <selection activeCell="K42" sqref="K42"/>
     </sheetView>
   </sheetViews>
@@ -2410,7 +2413,7 @@
   <dimension ref="A1:AF35"/>
   <sheetViews>
     <sheetView topLeftCell="P1" workbookViewId="0">
-      <selection activeCell="Z22" sqref="Z22:AF26"/>
+      <selection activeCell="AD17" sqref="AD17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3865,7 +3868,7 @@
       <c r="Y26" s="59" t="s">
         <v>3</v>
       </c>
-      <c r="Z26" s="71" t="s">
+      <c r="Z26" s="142" t="s">
         <v>6</v>
       </c>
       <c r="AA26" s="14"/>
@@ -3939,6 +3942,7 @@
       <c r="Y27" s="59" t="s">
         <v>3</v>
       </c>
+      <c r="Z27" s="135"/>
     </row>
     <row r="28" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A28" s="44"/>
@@ -3982,6 +3986,7 @@
       <c r="Y28" s="59" t="s">
         <v>3</v>
       </c>
+      <c r="Z28" s="135"/>
     </row>
     <row r="29" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A29" s="44"/>
@@ -4324,8 +4329,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="F2:Q20"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="O22" sqref="O22"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L17" sqref="L17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4432,12 +4437,14 @@
       <c r="P7" s="121"/>
       <c r="Q7" s="121"/>
     </row>
-    <row r="8" spans="6:17" x14ac:dyDescent="0.25">
+    <row r="8" spans="6:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="F8" s="121"/>
       <c r="G8" s="121"/>
       <c r="H8" s="121"/>
       <c r="I8" s="121"/>
-      <c r="J8" s="121"/>
+      <c r="J8" s="140">
+        <v>10</v>
+      </c>
       <c r="K8" s="121"/>
       <c r="L8" s="121"/>
       <c r="M8" s="121"/>

</xml_diff>

<commit_message>
Début implémentation du niveau 10
</commit_message>
<xml_diff>
--- a/Niveaux.xlsx
+++ b/Niveaux.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="150" windowWidth="24915" windowHeight="12075" activeTab="3"/>
+    <workbookView xWindow="120" yWindow="150" windowWidth="24915" windowHeight="12075" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Niveau 1-5" sheetId="1" r:id="rId1"/>
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="712" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="876" uniqueCount="29">
   <si>
     <t>J</t>
   </si>
@@ -98,6 +98,12 @@
   </si>
   <si>
     <t>Configuration 2 du niveau 9</t>
+  </si>
+  <si>
+    <t>Niveau 10</t>
+  </si>
+  <si>
+    <t>Configuration 2 du niveau 10</t>
   </si>
 </sst>
 </file>
@@ -497,7 +503,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="143">
+  <cellXfs count="152">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
@@ -905,6 +911,31 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1728,10 +1759,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="C2:M54"/>
+  <dimension ref="C2:M78"/>
   <sheetViews>
-    <sheetView topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="K42" sqref="K42"/>
+    <sheetView tabSelected="1" topLeftCell="A52" workbookViewId="0">
+      <selection activeCell="Q78" sqref="Q78"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2308,7 +2339,7 @@
       <c r="I46" s="7"/>
     </row>
     <row r="48" spans="3:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="49" spans="3:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="49" spans="3:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C49" s="122" t="s">
         <v>26</v>
       </c>
@@ -2319,7 +2350,7 @@
       <c r="H49" s="123"/>
       <c r="I49" s="124"/>
     </row>
-    <row r="50" spans="3:9" x14ac:dyDescent="0.25">
+    <row r="50" spans="3:13" x14ac:dyDescent="0.25">
       <c r="C50" s="139" t="s">
         <v>0</v>
       </c>
@@ -2336,7 +2367,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="51" spans="3:9" x14ac:dyDescent="0.25">
+    <row r="51" spans="3:13" x14ac:dyDescent="0.25">
       <c r="C51" s="10"/>
       <c r="D51" s="109" t="s">
         <v>19</v>
@@ -2351,7 +2382,7 @@
       </c>
       <c r="I51" s="5"/>
     </row>
-    <row r="52" spans="3:9" x14ac:dyDescent="0.25">
+    <row r="52" spans="3:13" x14ac:dyDescent="0.25">
       <c r="C52" s="108"/>
       <c r="D52" s="16" t="s">
         <v>2</v>
@@ -2366,7 +2397,7 @@
       </c>
       <c r="I52" s="110"/>
     </row>
-    <row r="53" spans="3:9" x14ac:dyDescent="0.25">
+    <row r="53" spans="3:13" x14ac:dyDescent="0.25">
       <c r="C53" s="10"/>
       <c r="D53" s="109" t="s">
         <v>19</v>
@@ -2381,7 +2412,7 @@
       </c>
       <c r="I53" s="5"/>
     </row>
-    <row r="54" spans="3:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="54" spans="3:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C54" s="71" t="s">
         <v>6</v>
       </c>
@@ -2396,8 +2427,490 @@
       <c r="H54" s="14"/>
       <c r="I54" s="7"/>
     </row>
+    <row r="56" spans="3:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="57" spans="3:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C57" s="128" t="s">
+        <v>27</v>
+      </c>
+      <c r="D57" s="129"/>
+      <c r="E57" s="129"/>
+      <c r="F57" s="129"/>
+      <c r="G57" s="129"/>
+      <c r="H57" s="129"/>
+      <c r="I57" s="129"/>
+      <c r="J57" s="129"/>
+      <c r="K57" s="129"/>
+      <c r="L57" s="129"/>
+      <c r="M57" s="130"/>
+    </row>
+    <row r="58" spans="3:13" x14ac:dyDescent="0.25">
+      <c r="C58" s="139" t="s">
+        <v>0</v>
+      </c>
+      <c r="D58" s="117" t="s">
+        <v>19</v>
+      </c>
+      <c r="E58" s="8"/>
+      <c r="F58" s="8"/>
+      <c r="G58" s="8"/>
+      <c r="H58" s="8"/>
+      <c r="I58" s="8"/>
+      <c r="J58" s="2"/>
+      <c r="K58" s="2"/>
+      <c r="L58" s="117" t="s">
+        <v>19</v>
+      </c>
+      <c r="M58" s="146" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="59" spans="3:13" x14ac:dyDescent="0.25">
+      <c r="C59" s="10"/>
+      <c r="D59" s="109" t="s">
+        <v>19</v>
+      </c>
+      <c r="E59" s="11"/>
+      <c r="F59" s="109" t="s">
+        <v>19</v>
+      </c>
+      <c r="G59" s="109" t="s">
+        <v>19</v>
+      </c>
+      <c r="H59" s="109" t="s">
+        <v>19</v>
+      </c>
+      <c r="I59" s="109" t="s">
+        <v>19</v>
+      </c>
+      <c r="J59" s="109" t="s">
+        <v>19</v>
+      </c>
+      <c r="K59" s="1"/>
+      <c r="L59" s="109" t="s">
+        <v>19</v>
+      </c>
+      <c r="M59" s="110" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="60" spans="3:13" x14ac:dyDescent="0.25">
+      <c r="C60" s="10"/>
+      <c r="D60" s="109" t="s">
+        <v>19</v>
+      </c>
+      <c r="E60" s="11"/>
+      <c r="F60" s="109" t="s">
+        <v>19</v>
+      </c>
+      <c r="G60" s="11"/>
+      <c r="H60" s="11"/>
+      <c r="I60" s="11"/>
+      <c r="J60" s="109" t="s">
+        <v>19</v>
+      </c>
+      <c r="K60" s="1"/>
+      <c r="L60" s="109" t="s">
+        <v>19</v>
+      </c>
+      <c r="M60" s="110" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="61" spans="3:13" x14ac:dyDescent="0.25">
+      <c r="C61" s="10"/>
+      <c r="D61" s="109" t="s">
+        <v>19</v>
+      </c>
+      <c r="E61" s="11"/>
+      <c r="F61" s="109" t="s">
+        <v>19</v>
+      </c>
+      <c r="G61" s="11"/>
+      <c r="H61" s="109" t="s">
+        <v>19</v>
+      </c>
+      <c r="I61" s="11"/>
+      <c r="J61" s="109" t="s">
+        <v>19</v>
+      </c>
+      <c r="K61" s="1"/>
+      <c r="L61" s="109" t="s">
+        <v>19</v>
+      </c>
+      <c r="M61" s="110" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="62" spans="3:13" x14ac:dyDescent="0.25">
+      <c r="C62" s="10"/>
+      <c r="D62" s="109" t="s">
+        <v>19</v>
+      </c>
+      <c r="E62" s="11"/>
+      <c r="F62" s="109" t="s">
+        <v>19</v>
+      </c>
+      <c r="G62" s="65" t="s">
+        <v>24</v>
+      </c>
+      <c r="H62" s="109" t="s">
+        <v>19</v>
+      </c>
+      <c r="I62" s="11"/>
+      <c r="J62" s="109" t="s">
+        <v>19</v>
+      </c>
+      <c r="K62" s="145" t="s">
+        <v>2</v>
+      </c>
+      <c r="L62" s="109" t="s">
+        <v>19</v>
+      </c>
+      <c r="M62" s="147" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="63" spans="3:13" x14ac:dyDescent="0.25">
+      <c r="C63" s="144" t="s">
+        <v>2</v>
+      </c>
+      <c r="D63" s="109" t="s">
+        <v>19</v>
+      </c>
+      <c r="E63" s="11"/>
+      <c r="F63" s="109" t="s">
+        <v>19</v>
+      </c>
+      <c r="G63" s="109" t="s">
+        <v>19</v>
+      </c>
+      <c r="H63" s="109" t="s">
+        <v>19</v>
+      </c>
+      <c r="I63" s="11"/>
+      <c r="J63" s="109" t="s">
+        <v>19</v>
+      </c>
+      <c r="K63" s="1"/>
+      <c r="L63" s="109" t="s">
+        <v>19</v>
+      </c>
+      <c r="M63" s="110" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="64" spans="3:13" x14ac:dyDescent="0.25">
+      <c r="C64" s="10"/>
+      <c r="D64" s="109" t="s">
+        <v>19</v>
+      </c>
+      <c r="E64" s="11"/>
+      <c r="F64" s="11"/>
+      <c r="G64" s="11"/>
+      <c r="H64" s="11"/>
+      <c r="I64" s="11"/>
+      <c r="J64" s="109" t="s">
+        <v>19</v>
+      </c>
+      <c r="K64" s="1"/>
+      <c r="L64" s="109" t="s">
+        <v>19</v>
+      </c>
+      <c r="M64" s="110" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="65" spans="3:13" x14ac:dyDescent="0.25">
+      <c r="C65" s="10"/>
+      <c r="D65" s="109" t="s">
+        <v>19</v>
+      </c>
+      <c r="E65" s="109" t="s">
+        <v>19</v>
+      </c>
+      <c r="F65" s="109" t="s">
+        <v>19</v>
+      </c>
+      <c r="G65" s="109" t="s">
+        <v>19</v>
+      </c>
+      <c r="H65" s="109" t="s">
+        <v>19</v>
+      </c>
+      <c r="I65" s="109" t="s">
+        <v>19</v>
+      </c>
+      <c r="J65" s="109" t="s">
+        <v>19</v>
+      </c>
+      <c r="K65" s="1"/>
+      <c r="L65" s="109" t="s">
+        <v>19</v>
+      </c>
+      <c r="M65" s="110" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="66" spans="3:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C66" s="13"/>
+      <c r="D66" s="14"/>
+      <c r="E66" s="14"/>
+      <c r="F66" s="14"/>
+      <c r="G66" s="120" t="s">
+        <v>2</v>
+      </c>
+      <c r="H66" s="14"/>
+      <c r="I66" s="14"/>
+      <c r="J66" s="6"/>
+      <c r="K66" s="6"/>
+      <c r="L66" s="111" t="s">
+        <v>19</v>
+      </c>
+      <c r="M66" s="112" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="68" spans="3:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="69" spans="3:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C69" s="148" t="s">
+        <v>28</v>
+      </c>
+      <c r="D69" s="149"/>
+      <c r="E69" s="149"/>
+      <c r="F69" s="149"/>
+      <c r="G69" s="149"/>
+      <c r="H69" s="149"/>
+      <c r="I69" s="149"/>
+      <c r="J69" s="149"/>
+      <c r="K69" s="149"/>
+      <c r="L69" s="149"/>
+      <c r="M69" s="150"/>
+    </row>
+    <row r="70" spans="3:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C70" s="139" t="s">
+        <v>0</v>
+      </c>
+      <c r="D70" s="117" t="s">
+        <v>19</v>
+      </c>
+      <c r="E70" s="117" t="s">
+        <v>19</v>
+      </c>
+      <c r="F70" s="117" t="s">
+        <v>19</v>
+      </c>
+      <c r="G70" s="117" t="s">
+        <v>19</v>
+      </c>
+      <c r="H70" s="117" t="s">
+        <v>19</v>
+      </c>
+      <c r="I70" s="8"/>
+      <c r="J70" s="117" t="s">
+        <v>19</v>
+      </c>
+      <c r="K70" s="2"/>
+      <c r="L70" s="117"/>
+      <c r="M70" s="146" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="71" spans="3:13" x14ac:dyDescent="0.25">
+      <c r="C71" s="108" t="s">
+        <v>19</v>
+      </c>
+      <c r="D71" s="109" t="s">
+        <v>19</v>
+      </c>
+      <c r="E71" s="11"/>
+      <c r="F71" s="109"/>
+      <c r="G71" s="109"/>
+      <c r="H71" s="109" t="s">
+        <v>19</v>
+      </c>
+      <c r="I71" s="109"/>
+      <c r="J71" s="117" t="s">
+        <v>19</v>
+      </c>
+      <c r="K71" s="65" t="s">
+        <v>5</v>
+      </c>
+      <c r="L71" s="109"/>
+      <c r="M71" s="110" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="72" spans="3:13" x14ac:dyDescent="0.25">
+      <c r="C72" s="10"/>
+      <c r="D72" s="109"/>
+      <c r="E72" s="11"/>
+      <c r="F72" s="109" t="s">
+        <v>19</v>
+      </c>
+      <c r="G72" s="11"/>
+      <c r="H72" s="109" t="s">
+        <v>19</v>
+      </c>
+      <c r="I72" s="11"/>
+      <c r="J72" s="109"/>
+      <c r="K72" s="1"/>
+      <c r="L72" s="109"/>
+      <c r="M72" s="110" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="73" spans="3:13" x14ac:dyDescent="0.25">
+      <c r="C73" s="10"/>
+      <c r="D73" s="109" t="s">
+        <v>19</v>
+      </c>
+      <c r="E73" s="109" t="s">
+        <v>19</v>
+      </c>
+      <c r="F73" s="109" t="s">
+        <v>19</v>
+      </c>
+      <c r="G73" s="11"/>
+      <c r="H73" s="109" t="s">
+        <v>19</v>
+      </c>
+      <c r="I73" s="11"/>
+      <c r="J73" s="109" t="s">
+        <v>19</v>
+      </c>
+      <c r="K73" s="1"/>
+      <c r="L73" s="109"/>
+      <c r="M73" s="110" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="74" spans="3:13" x14ac:dyDescent="0.25">
+      <c r="C74" s="10"/>
+      <c r="D74" s="109" t="s">
+        <v>19</v>
+      </c>
+      <c r="E74" s="11"/>
+      <c r="F74" s="109" t="s">
+        <v>19</v>
+      </c>
+      <c r="G74" s="65" t="s">
+        <v>24</v>
+      </c>
+      <c r="H74" s="109" t="s">
+        <v>19</v>
+      </c>
+      <c r="I74" s="11"/>
+      <c r="J74" s="109" t="s">
+        <v>19</v>
+      </c>
+      <c r="K74" s="145" t="s">
+        <v>2</v>
+      </c>
+      <c r="L74" s="109"/>
+      <c r="M74" s="147" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="75" spans="3:13" x14ac:dyDescent="0.25">
+      <c r="C75" s="144" t="s">
+        <v>2</v>
+      </c>
+      <c r="D75" s="109" t="s">
+        <v>19</v>
+      </c>
+      <c r="E75" s="11"/>
+      <c r="F75" s="109" t="s">
+        <v>19</v>
+      </c>
+      <c r="G75" s="109" t="s">
+        <v>19</v>
+      </c>
+      <c r="H75" s="109" t="s">
+        <v>19</v>
+      </c>
+      <c r="I75" s="11"/>
+      <c r="J75" s="109" t="s">
+        <v>19</v>
+      </c>
+      <c r="K75" s="1"/>
+      <c r="L75" s="109"/>
+      <c r="M75" s="110" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="76" spans="3:13" x14ac:dyDescent="0.25">
+      <c r="C76" s="10"/>
+      <c r="D76" s="109" t="s">
+        <v>19</v>
+      </c>
+      <c r="E76" s="11"/>
+      <c r="F76" s="11"/>
+      <c r="G76" s="11"/>
+      <c r="H76" s="11"/>
+      <c r="I76" s="11"/>
+      <c r="J76" s="109" t="s">
+        <v>19</v>
+      </c>
+      <c r="K76" s="1"/>
+      <c r="L76" s="109"/>
+      <c r="M76" s="110" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="77" spans="3:13" x14ac:dyDescent="0.25">
+      <c r="C77" s="10"/>
+      <c r="D77" s="109" t="s">
+        <v>19</v>
+      </c>
+      <c r="E77" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="F77" s="109" t="s">
+        <v>19</v>
+      </c>
+      <c r="G77" s="109" t="s">
+        <v>19</v>
+      </c>
+      <c r="H77" s="109" t="s">
+        <v>19</v>
+      </c>
+      <c r="I77" s="109"/>
+      <c r="J77" s="109" t="s">
+        <v>19</v>
+      </c>
+      <c r="K77" s="1"/>
+      <c r="L77" s="109" t="s">
+        <v>19</v>
+      </c>
+      <c r="M77" s="110" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="78" spans="3:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C78" s="13"/>
+      <c r="D78" s="14"/>
+      <c r="E78" s="14"/>
+      <c r="F78" s="14"/>
+      <c r="G78" s="120" t="s">
+        <v>2</v>
+      </c>
+      <c r="H78" s="14"/>
+      <c r="I78" s="14"/>
+      <c r="J78" s="111" t="s">
+        <v>19</v>
+      </c>
+      <c r="K78" s="6"/>
+      <c r="L78" s="151" t="s">
+        <v>8</v>
+      </c>
+      <c r="M78" s="112" t="s">
+        <v>19</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="5">
+  <mergeCells count="7">
+    <mergeCell ref="C57:M57"/>
+    <mergeCell ref="C69:M69"/>
     <mergeCell ref="C3:K3"/>
     <mergeCell ref="C14:E14"/>
     <mergeCell ref="C29:I29"/>
@@ -2410,15 +2923,15 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AF35"/>
+  <dimension ref="A1:AJ36"/>
   <sheetViews>
-    <sheetView topLeftCell="P1" workbookViewId="0">
-      <selection activeCell="AD17" sqref="AD17"/>
+    <sheetView topLeftCell="U7" workbookViewId="0">
+      <selection activeCell="Z28" sqref="Z28:AJ36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:34" x14ac:dyDescent="0.25">
       <c r="O1" s="132" t="s">
         <v>4</v>
       </c>
@@ -2430,7 +2943,7 @@
       <c r="V1" s="132"/>
       <c r="W1" s="132"/>
     </row>
-    <row r="2" spans="1:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:34" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="M2" s="58" t="s">
         <v>3</v>
       </c>
@@ -2477,7 +2990,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:34" x14ac:dyDescent="0.25">
       <c r="M3" s="58" t="s">
         <v>3</v>
       </c>
@@ -2512,7 +3025,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A4" s="44"/>
       <c r="B4" s="44"/>
       <c r="C4" s="44"/>
@@ -2563,7 +3076,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A5" s="44"/>
       <c r="B5" s="44"/>
       <c r="C5" s="44"/>
@@ -2606,7 +3119,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A6" s="44"/>
       <c r="B6" s="44"/>
       <c r="C6" s="44"/>
@@ -2657,7 +3170,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="7" spans="1:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:34" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="44"/>
       <c r="B7" s="44"/>
       <c r="C7" s="44"/>
@@ -2710,7 +3223,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="8" spans="1:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:34" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="44"/>
       <c r="B8" s="44"/>
       <c r="C8" s="44"/>
@@ -2773,7 +3286,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="9" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A9" s="44"/>
       <c r="B9" s="44"/>
       <c r="C9" s="44"/>
@@ -2830,7 +3343,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="10" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A10" s="44"/>
       <c r="B10" s="44"/>
       <c r="C10" s="44"/>
@@ -2892,7 +3405,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="11" spans="1:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:34" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="44"/>
       <c r="B11" s="44"/>
       <c r="C11" s="44"/>
@@ -2951,7 +3464,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="12" spans="1:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:34" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="44"/>
       <c r="B12" s="44"/>
       <c r="C12" s="44"/>
@@ -3004,7 +3517,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="13" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A13" s="44"/>
       <c r="B13" s="44"/>
       <c r="C13" s="44"/>
@@ -3057,7 +3570,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="14" spans="1:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:34" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="44"/>
       <c r="B14" s="44"/>
       <c r="C14" s="44"/>
@@ -3112,7 +3625,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="15" spans="1:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:34" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="44"/>
       <c r="B15" s="44"/>
       <c r="C15" s="44"/>
@@ -3173,7 +3686,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="16" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A16" s="44"/>
       <c r="B16" s="44"/>
       <c r="C16" s="44"/>
@@ -3233,8 +3746,9 @@
       <c r="AA16" s="59" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="17" spans="1:32" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="AH16" s="143"/>
+    </row>
+    <row r="17" spans="1:36" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="44"/>
       <c r="B17" s="44"/>
       <c r="C17" s="44"/>
@@ -3297,7 +3811,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="18" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A18" s="44"/>
       <c r="B18" s="44"/>
       <c r="C18" s="44"/>
@@ -3356,7 +3870,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="19" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A19" s="44"/>
       <c r="B19" s="44"/>
       <c r="C19" s="44"/>
@@ -3415,7 +3929,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="20" spans="1:32" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:36" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="44"/>
       <c r="B20" s="44"/>
       <c r="C20" s="44"/>
@@ -3475,7 +3989,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="21" spans="1:32" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:36" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="44"/>
       <c r="B21" s="44"/>
       <c r="C21" s="44"/>
@@ -3536,7 +4050,7 @@
       <c r="AC21" s="123"/>
       <c r="AD21" s="124"/>
     </row>
-    <row r="22" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A22" s="44"/>
       <c r="B22" s="44"/>
       <c r="C22" s="44"/>
@@ -3604,7 +4118,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="23" spans="1:32" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:36" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="44"/>
       <c r="B23" s="44"/>
       <c r="C23" s="44"/>
@@ -3670,7 +4184,7 @@
       <c r="AE23" s="11"/>
       <c r="AF23" s="5"/>
     </row>
-    <row r="24" spans="1:32" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:36" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A24" s="44"/>
       <c r="B24" s="44"/>
       <c r="C24" s="44"/>
@@ -3746,7 +4260,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="25" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A25" s="44"/>
       <c r="B25" s="44"/>
       <c r="C25" s="44"/>
@@ -3816,7 +4330,7 @@
       </c>
       <c r="AF25" s="5"/>
     </row>
-    <row r="26" spans="1:32" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:36" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A26" s="44"/>
       <c r="B26" s="44"/>
       <c r="C26" s="44"/>
@@ -3884,7 +4398,7 @@
       <c r="AE26" s="14"/>
       <c r="AF26" s="7"/>
     </row>
-    <row r="27" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:36" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A27" s="44"/>
       <c r="B27" s="44"/>
       <c r="C27" s="44"/>
@@ -3944,7 +4458,7 @@
       </c>
       <c r="Z27" s="135"/>
     </row>
-    <row r="28" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A28" s="44"/>
       <c r="B28" s="44"/>
       <c r="C28" s="44"/>
@@ -3986,9 +4500,27 @@
       <c r="Y28" s="59" t="s">
         <v>3</v>
       </c>
-      <c r="Z28" s="135"/>
-    </row>
-    <row r="29" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="Z28" s="139" t="s">
+        <v>0</v>
+      </c>
+      <c r="AA28" s="117" t="s">
+        <v>19</v>
+      </c>
+      <c r="AB28" s="8"/>
+      <c r="AC28" s="8"/>
+      <c r="AD28" s="8"/>
+      <c r="AE28" s="8"/>
+      <c r="AF28" s="8"/>
+      <c r="AG28" s="2"/>
+      <c r="AH28" s="2"/>
+      <c r="AI28" s="117" t="s">
+        <v>19</v>
+      </c>
+      <c r="AJ28" s="146" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="29" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A29" s="44"/>
       <c r="B29" s="44"/>
       <c r="C29" s="44"/>
@@ -4034,8 +4566,35 @@
       <c r="Y29" s="59" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="30" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="Z29" s="10"/>
+      <c r="AA29" s="109" t="s">
+        <v>19</v>
+      </c>
+      <c r="AB29" s="11"/>
+      <c r="AC29" s="109" t="s">
+        <v>19</v>
+      </c>
+      <c r="AD29" s="109" t="s">
+        <v>19</v>
+      </c>
+      <c r="AE29" s="109" t="s">
+        <v>19</v>
+      </c>
+      <c r="AF29" s="109" t="s">
+        <v>19</v>
+      </c>
+      <c r="AG29" s="109" t="s">
+        <v>19</v>
+      </c>
+      <c r="AH29" s="1"/>
+      <c r="AI29" s="109" t="s">
+        <v>19</v>
+      </c>
+      <c r="AJ29" s="110" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="30" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A30" s="44"/>
       <c r="B30" s="44"/>
       <c r="C30" s="44"/>
@@ -4083,8 +4642,29 @@
       <c r="Y30" s="59" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="31" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="Z30" s="10"/>
+      <c r="AA30" s="109" t="s">
+        <v>19</v>
+      </c>
+      <c r="AB30" s="11"/>
+      <c r="AC30" s="109" t="s">
+        <v>19</v>
+      </c>
+      <c r="AD30" s="11"/>
+      <c r="AE30" s="11"/>
+      <c r="AF30" s="11"/>
+      <c r="AG30" s="109" t="s">
+        <v>19</v>
+      </c>
+      <c r="AH30" s="1"/>
+      <c r="AI30" s="109" t="s">
+        <v>19</v>
+      </c>
+      <c r="AJ30" s="110" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="31" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A31" s="44"/>
       <c r="B31" s="44"/>
       <c r="C31" s="44"/>
@@ -4134,8 +4714,31 @@
       <c r="Y31" s="59" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="32" spans="1:32" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="Z31" s="10"/>
+      <c r="AA31" s="109" t="s">
+        <v>19</v>
+      </c>
+      <c r="AB31" s="11"/>
+      <c r="AC31" s="109" t="s">
+        <v>19</v>
+      </c>
+      <c r="AD31" s="11"/>
+      <c r="AE31" s="109" t="s">
+        <v>19</v>
+      </c>
+      <c r="AF31" s="11"/>
+      <c r="AG31" s="109" t="s">
+        <v>19</v>
+      </c>
+      <c r="AH31" s="1"/>
+      <c r="AI31" s="109" t="s">
+        <v>19</v>
+      </c>
+      <c r="AJ31" s="110" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="32" spans="1:36" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A32" s="44"/>
       <c r="B32" s="44"/>
       <c r="C32" s="44"/>
@@ -4189,8 +4792,35 @@
       <c r="Y32" s="59" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="33" spans="1:25" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="Z32" s="10"/>
+      <c r="AA32" s="109" t="s">
+        <v>19</v>
+      </c>
+      <c r="AB32" s="11"/>
+      <c r="AC32" s="109" t="s">
+        <v>19</v>
+      </c>
+      <c r="AD32" s="65" t="s">
+        <v>24</v>
+      </c>
+      <c r="AE32" s="109" t="s">
+        <v>19</v>
+      </c>
+      <c r="AF32" s="11"/>
+      <c r="AG32" s="109" t="s">
+        <v>19</v>
+      </c>
+      <c r="AH32" s="145" t="s">
+        <v>2</v>
+      </c>
+      <c r="AI32" s="109" t="s">
+        <v>19</v>
+      </c>
+      <c r="AJ32" s="147" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="33" spans="1:36" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A33" s="44"/>
       <c r="B33" s="44"/>
       <c r="C33" s="44"/>
@@ -4244,8 +4874,35 @@
       <c r="Y33" s="59" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="34" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Z33" s="144" t="s">
+        <v>2</v>
+      </c>
+      <c r="AA33" s="109" t="s">
+        <v>19</v>
+      </c>
+      <c r="AB33" s="11"/>
+      <c r="AC33" s="109" t="s">
+        <v>19</v>
+      </c>
+      <c r="AD33" s="109" t="s">
+        <v>19</v>
+      </c>
+      <c r="AE33" s="109" t="s">
+        <v>19</v>
+      </c>
+      <c r="AF33" s="11"/>
+      <c r="AG33" s="109" t="s">
+        <v>19</v>
+      </c>
+      <c r="AH33" s="1"/>
+      <c r="AI33" s="109" t="s">
+        <v>19</v>
+      </c>
+      <c r="AJ33" s="110" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="34" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A34" s="44"/>
       <c r="B34" s="44"/>
       <c r="C34" s="44"/>
@@ -4282,8 +4939,27 @@
       <c r="Y34" s="59" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="35" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="Z34" s="10"/>
+      <c r="AA34" s="109" t="s">
+        <v>19</v>
+      </c>
+      <c r="AB34" s="11"/>
+      <c r="AC34" s="11"/>
+      <c r="AD34" s="11"/>
+      <c r="AE34" s="11"/>
+      <c r="AF34" s="11"/>
+      <c r="AG34" s="109" t="s">
+        <v>19</v>
+      </c>
+      <c r="AH34" s="1"/>
+      <c r="AI34" s="109" t="s">
+        <v>19</v>
+      </c>
+      <c r="AJ34" s="110" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="35" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A35" s="44"/>
       <c r="B35" s="44"/>
       <c r="C35" s="44"/>
@@ -4308,6 +4984,54 @@
       </c>
       <c r="W35" s="131"/>
       <c r="X35" s="131"/>
+      <c r="Z35" s="10"/>
+      <c r="AA35" s="109" t="s">
+        <v>19</v>
+      </c>
+      <c r="AB35" s="109" t="s">
+        <v>19</v>
+      </c>
+      <c r="AC35" s="109" t="s">
+        <v>19</v>
+      </c>
+      <c r="AD35" s="109" t="s">
+        <v>19</v>
+      </c>
+      <c r="AE35" s="109" t="s">
+        <v>19</v>
+      </c>
+      <c r="AF35" s="109" t="s">
+        <v>19</v>
+      </c>
+      <c r="AG35" s="109" t="s">
+        <v>19</v>
+      </c>
+      <c r="AH35" s="1"/>
+      <c r="AI35" s="109" t="s">
+        <v>19</v>
+      </c>
+      <c r="AJ35" s="110" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="36" spans="1:36" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="Z36" s="13"/>
+      <c r="AA36" s="14"/>
+      <c r="AB36" s="14"/>
+      <c r="AC36" s="14"/>
+      <c r="AD36" s="120" t="s">
+        <v>2</v>
+      </c>
+      <c r="AE36" s="14"/>
+      <c r="AF36" s="14"/>
+      <c r="AG36" s="6"/>
+      <c r="AH36" s="6"/>
+      <c r="AI36" s="111" t="s">
+        <v>19</v>
+      </c>
+      <c r="AJ36" s="112" t="s">
+        <v>19</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="8">
@@ -4329,7 +5053,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="F2:Q20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="L17" sqref="L17"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Correction du bug du débloquage des niveaux
</commit_message>
<xml_diff>
--- a/Niveaux.xlsx
+++ b/Niveaux.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="150" windowWidth="24915" windowHeight="12075" activeTab="1"/>
+    <workbookView xWindow="120" yWindow="150" windowWidth="24915" windowHeight="12075" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Niveau 1-5" sheetId="1" r:id="rId1"/>
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="876" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="927" uniqueCount="34">
   <si>
     <t>J</t>
   </si>
@@ -104,6 +104,21 @@
   </si>
   <si>
     <t>Configuration 2 du niveau 10</t>
+  </si>
+  <si>
+    <t>m1</t>
+  </si>
+  <si>
+    <t>P2</t>
+  </si>
+  <si>
+    <t>b2</t>
+  </si>
+  <si>
+    <t>5 par 7</t>
+  </si>
+  <si>
+    <t>8 par 11</t>
   </si>
 </sst>
 </file>
@@ -205,7 +220,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="7">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -242,6 +257,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="1"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="19">
     <border>
@@ -503,7 +524,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="152">
+  <cellXfs count="153">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
@@ -938,6 +959,7 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1759,10 +1781,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="C2:M78"/>
+  <dimension ref="C2:O78"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A52" workbookViewId="0">
-      <selection activeCell="Q78" sqref="Q78"/>
+    <sheetView topLeftCell="A46" workbookViewId="0">
+      <selection activeCell="Q62" sqref="Q62"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2156,7 +2178,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="33" spans="3:9" x14ac:dyDescent="0.25">
+    <row r="33" spans="3:11" x14ac:dyDescent="0.25">
       <c r="C33" s="108" t="s">
         <v>19</v>
       </c>
@@ -2177,7 +2199,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="34" spans="3:9" x14ac:dyDescent="0.25">
+    <row r="34" spans="3:11" x14ac:dyDescent="0.25">
       <c r="C34" s="10"/>
       <c r="D34" s="16" t="s">
         <v>2</v>
@@ -2190,7 +2212,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="35" spans="3:9" x14ac:dyDescent="0.25">
+    <row r="35" spans="3:11" x14ac:dyDescent="0.25">
       <c r="C35" s="10"/>
       <c r="D35" s="109" t="s">
         <v>19</v>
@@ -2209,7 +2231,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="36" spans="3:9" x14ac:dyDescent="0.25">
+    <row r="36" spans="3:11" x14ac:dyDescent="0.25">
       <c r="C36" s="10"/>
       <c r="D36" s="11"/>
       <c r="E36" s="11"/>
@@ -2226,7 +2248,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="37" spans="3:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="37" spans="3:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C37" s="118" t="s">
         <v>19</v>
       </c>
@@ -2249,8 +2271,8 @@
         <v>6</v>
       </c>
     </row>
-    <row r="40" spans="3:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="41" spans="3:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="40" spans="3:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="41" spans="3:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C41" s="122" t="s">
         <v>25</v>
       </c>
@@ -2261,7 +2283,7 @@
       <c r="H41" s="123"/>
       <c r="I41" s="124"/>
     </row>
-    <row r="42" spans="3:9" x14ac:dyDescent="0.25">
+    <row r="42" spans="3:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C42" s="139" t="s">
         <v>0</v>
       </c>
@@ -2278,7 +2300,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="43" spans="3:9" x14ac:dyDescent="0.25">
+    <row r="43" spans="3:11" x14ac:dyDescent="0.25">
       <c r="C43" s="10"/>
       <c r="D43" s="11"/>
       <c r="E43" s="109" t="s">
@@ -2290,8 +2312,11 @@
       </c>
       <c r="H43" s="11"/>
       <c r="I43" s="5"/>
-    </row>
-    <row r="44" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="K43" s="85" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="44" spans="3:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C44" s="108" t="s">
         <v>19</v>
       </c>
@@ -2307,8 +2332,11 @@
       <c r="I44" s="110" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="45" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="K44" s="86" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="45" spans="3:11" x14ac:dyDescent="0.25">
       <c r="C45" s="10"/>
       <c r="D45" s="109" t="s">
         <v>19</v>
@@ -2321,7 +2349,7 @@
       </c>
       <c r="I45" s="5"/>
     </row>
-    <row r="46" spans="3:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="46" spans="3:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C46" s="71" t="s">
         <v>6</v>
       </c>
@@ -2338,8 +2366,8 @@
       <c r="H46" s="14"/>
       <c r="I46" s="7"/>
     </row>
-    <row r="48" spans="3:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="49" spans="3:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="48" spans="3:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="49" spans="3:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C49" s="122" t="s">
         <v>26</v>
       </c>
@@ -2350,7 +2378,7 @@
       <c r="H49" s="123"/>
       <c r="I49" s="124"/>
     </row>
-    <row r="50" spans="3:13" x14ac:dyDescent="0.25">
+    <row r="50" spans="3:15" x14ac:dyDescent="0.25">
       <c r="C50" s="139" t="s">
         <v>0</v>
       </c>
@@ -2367,7 +2395,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="51" spans="3:13" x14ac:dyDescent="0.25">
+    <row r="51" spans="3:15" x14ac:dyDescent="0.25">
       <c r="C51" s="10"/>
       <c r="D51" s="109" t="s">
         <v>19</v>
@@ -2382,7 +2410,7 @@
       </c>
       <c r="I51" s="5"/>
     </row>
-    <row r="52" spans="3:13" x14ac:dyDescent="0.25">
+    <row r="52" spans="3:15" x14ac:dyDescent="0.25">
       <c r="C52" s="108"/>
       <c r="D52" s="16" t="s">
         <v>2</v>
@@ -2397,7 +2425,7 @@
       </c>
       <c r="I52" s="110"/>
     </row>
-    <row r="53" spans="3:13" x14ac:dyDescent="0.25">
+    <row r="53" spans="3:15" x14ac:dyDescent="0.25">
       <c r="C53" s="10"/>
       <c r="D53" s="109" t="s">
         <v>19</v>
@@ -2412,7 +2440,7 @@
       </c>
       <c r="I53" s="5"/>
     </row>
-    <row r="54" spans="3:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="54" spans="3:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C54" s="71" t="s">
         <v>6</v>
       </c>
@@ -2427,8 +2455,8 @@
       <c r="H54" s="14"/>
       <c r="I54" s="7"/>
     </row>
-    <row r="56" spans="3:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="57" spans="3:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="56" spans="3:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="57" spans="3:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C57" s="128" t="s">
         <v>27</v>
       </c>
@@ -2443,7 +2471,7 @@
       <c r="L57" s="129"/>
       <c r="M57" s="130"/>
     </row>
-    <row r="58" spans="3:13" x14ac:dyDescent="0.25">
+    <row r="58" spans="3:15" x14ac:dyDescent="0.25">
       <c r="C58" s="139" t="s">
         <v>0</v>
       </c>
@@ -2464,7 +2492,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="59" spans="3:13" x14ac:dyDescent="0.25">
+    <row r="59" spans="3:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C59" s="10"/>
       <c r="D59" s="109" t="s">
         <v>19</v>
@@ -2493,7 +2521,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="60" spans="3:13" x14ac:dyDescent="0.25">
+    <row r="60" spans="3:15" x14ac:dyDescent="0.25">
       <c r="C60" s="10"/>
       <c r="D60" s="109" t="s">
         <v>19</v>
@@ -2515,8 +2543,11 @@
       <c r="M60" s="110" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="61" spans="3:13" x14ac:dyDescent="0.25">
+      <c r="O60" s="85" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="61" spans="3:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C61" s="10"/>
       <c r="D61" s="109" t="s">
         <v>19</v>
@@ -2540,8 +2571,11 @@
       <c r="M61" s="110" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="62" spans="3:13" x14ac:dyDescent="0.25">
+      <c r="O61" s="86" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="62" spans="3:15" x14ac:dyDescent="0.25">
       <c r="C62" s="10"/>
       <c r="D62" s="109" t="s">
         <v>19</v>
@@ -2570,7 +2604,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="63" spans="3:13" x14ac:dyDescent="0.25">
+    <row r="63" spans="3:15" x14ac:dyDescent="0.25">
       <c r="C63" s="144" t="s">
         <v>2</v>
       </c>
@@ -2599,7 +2633,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="64" spans="3:13" x14ac:dyDescent="0.25">
+    <row r="64" spans="3:15" x14ac:dyDescent="0.25">
       <c r="C64" s="10"/>
       <c r="D64" s="109" t="s">
         <v>19</v>
@@ -2670,7 +2704,12 @@
         <v>19</v>
       </c>
     </row>
-    <row r="68" spans="3:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="67" spans="3:13" x14ac:dyDescent="0.25">
+      <c r="H67" s="152"/>
+    </row>
+    <row r="68" spans="3:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="H68" s="152"/>
+    </row>
     <row r="69" spans="3:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C69" s="148" t="s">
         <v>28</v>
@@ -2686,7 +2725,7 @@
       <c r="L69" s="149"/>
       <c r="M69" s="150"/>
     </row>
-    <row r="70" spans="3:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="70" spans="3:13" x14ac:dyDescent="0.25">
       <c r="C70" s="139" t="s">
         <v>0</v>
       </c>
@@ -2706,9 +2745,7 @@
         <v>19</v>
       </c>
       <c r="I70" s="8"/>
-      <c r="J70" s="117" t="s">
-        <v>19</v>
-      </c>
+      <c r="J70" s="8"/>
       <c r="K70" s="2"/>
       <c r="L70" s="117"/>
       <c r="M70" s="146" t="s">
@@ -2729,7 +2766,7 @@
         <v>19</v>
       </c>
       <c r="I71" s="109"/>
-      <c r="J71" s="117" t="s">
+      <c r="J71" s="109" t="s">
         <v>19</v>
       </c>
       <c r="K71" s="65" t="s">
@@ -2789,7 +2826,9 @@
       <c r="D74" s="109" t="s">
         <v>19</v>
       </c>
-      <c r="E74" s="11"/>
+      <c r="E74" s="65" t="s">
+        <v>31</v>
+      </c>
       <c r="F74" s="109" t="s">
         <v>19</v>
       </c>
@@ -2806,7 +2845,9 @@
       <c r="K74" s="145" t="s">
         <v>2</v>
       </c>
-      <c r="L74" s="109"/>
+      <c r="L74" s="11" t="s">
+        <v>30</v>
+      </c>
       <c r="M74" s="147" t="s">
         <v>6</v>
       </c>
@@ -2848,9 +2889,7 @@
       <c r="G76" s="11"/>
       <c r="H76" s="11"/>
       <c r="I76" s="11"/>
-      <c r="J76" s="109" t="s">
-        <v>19</v>
-      </c>
+      <c r="J76" s="11"/>
       <c r="K76" s="1"/>
       <c r="L76" s="109"/>
       <c r="M76" s="110" t="s">
@@ -2862,9 +2901,7 @@
       <c r="D77" s="109" t="s">
         <v>19</v>
       </c>
-      <c r="E77" s="11" t="s">
-        <v>9</v>
-      </c>
+      <c r="E77" s="11"/>
       <c r="F77" s="109" t="s">
         <v>19</v>
       </c>
@@ -2901,7 +2938,7 @@
       </c>
       <c r="K78" s="6"/>
       <c r="L78" s="151" t="s">
-        <v>8</v>
+        <v>29</v>
       </c>
       <c r="M78" s="112" t="s">
         <v>19</v>
@@ -2923,10 +2960,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AJ36"/>
+  <dimension ref="A1:AK37"/>
   <sheetViews>
-    <sheetView topLeftCell="U7" workbookViewId="0">
-      <selection activeCell="Z28" sqref="Z28:AJ36"/>
+    <sheetView topLeftCell="U10" workbookViewId="0">
+      <selection activeCell="AI41" sqref="AI41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3748,7 +3785,7 @@
       </c>
       <c r="AH16" s="143"/>
     </row>
-    <row r="17" spans="1:36" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:37" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="44"/>
       <c r="B17" s="44"/>
       <c r="C17" s="44"/>
@@ -3811,7 +3848,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="18" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A18" s="44"/>
       <c r="B18" s="44"/>
       <c r="C18" s="44"/>
@@ -3870,7 +3907,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="19" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A19" s="44"/>
       <c r="B19" s="44"/>
       <c r="C19" s="44"/>
@@ -3929,7 +3966,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="20" spans="1:36" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:37" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="44"/>
       <c r="B20" s="44"/>
       <c r="C20" s="44"/>
@@ -3988,8 +4025,29 @@
       <c r="Z20" s="134" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="21" spans="1:36" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="AA20" s="59" t="s">
+        <v>3</v>
+      </c>
+      <c r="AB20" s="59" t="s">
+        <v>3</v>
+      </c>
+      <c r="AC20" s="59" t="s">
+        <v>3</v>
+      </c>
+      <c r="AD20" s="59" t="s">
+        <v>3</v>
+      </c>
+      <c r="AE20" s="59" t="s">
+        <v>3</v>
+      </c>
+      <c r="AF20" s="59" t="s">
+        <v>3</v>
+      </c>
+      <c r="AG20" s="59" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="21" spans="1:37" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="44"/>
       <c r="B21" s="44"/>
       <c r="C21" s="44"/>
@@ -4044,13 +4102,25 @@
         <v>3</v>
       </c>
       <c r="Z21" s="135"/>
+      <c r="AA21" s="59" t="s">
+        <v>3</v>
+      </c>
       <c r="AB21" s="122" t="s">
         <v>25</v>
       </c>
       <c r="AC21" s="123"/>
       <c r="AD21" s="124"/>
-    </row>
-    <row r="22" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="AE21" s="59" t="s">
+        <v>3</v>
+      </c>
+      <c r="AF21" s="59" t="s">
+        <v>3</v>
+      </c>
+      <c r="AG21" s="59" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="22" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A22" s="44"/>
       <c r="B22" s="44"/>
       <c r="C22" s="44"/>
@@ -4117,8 +4187,11 @@
       <c r="AF22" s="141" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="23" spans="1:36" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="AG22" s="59" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="23" spans="1:37" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="44"/>
       <c r="B23" s="44"/>
       <c r="C23" s="44"/>
@@ -4183,8 +4256,11 @@
       </c>
       <c r="AE23" s="11"/>
       <c r="AF23" s="5"/>
-    </row>
-    <row r="24" spans="1:36" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="AG23" s="59" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="24" spans="1:37" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A24" s="44"/>
       <c r="B24" s="44"/>
       <c r="C24" s="44"/>
@@ -4259,8 +4335,11 @@
       <c r="AF24" s="110" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="25" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="AG24" s="59" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="25" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A25" s="44"/>
       <c r="B25" s="44"/>
       <c r="C25" s="44"/>
@@ -4329,8 +4408,11 @@
         <v>19</v>
       </c>
       <c r="AF25" s="5"/>
-    </row>
-    <row r="26" spans="1:36" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="AG25" s="59" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="26" spans="1:37" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A26" s="44"/>
       <c r="B26" s="44"/>
       <c r="C26" s="44"/>
@@ -4397,8 +4479,11 @@
       </c>
       <c r="AE26" s="14"/>
       <c r="AF26" s="7"/>
-    </row>
-    <row r="27" spans="1:36" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="AG26" s="59" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="27" spans="1:37" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A27" s="44"/>
       <c r="B27" s="44"/>
       <c r="C27" s="44"/>
@@ -4457,8 +4542,41 @@
         <v>3</v>
       </c>
       <c r="Z27" s="135"/>
-    </row>
-    <row r="28" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="AA27" s="59" t="s">
+        <v>3</v>
+      </c>
+      <c r="AB27" s="59" t="s">
+        <v>3</v>
+      </c>
+      <c r="AC27" s="59" t="s">
+        <v>3</v>
+      </c>
+      <c r="AD27" s="59" t="s">
+        <v>3</v>
+      </c>
+      <c r="AE27" s="59" t="s">
+        <v>3</v>
+      </c>
+      <c r="AF27" s="59" t="s">
+        <v>3</v>
+      </c>
+      <c r="AG27" s="59" t="s">
+        <v>3</v>
+      </c>
+      <c r="AH27" s="59" t="s">
+        <v>3</v>
+      </c>
+      <c r="AI27" s="59" t="s">
+        <v>3</v>
+      </c>
+      <c r="AJ27" s="59" t="s">
+        <v>3</v>
+      </c>
+      <c r="AK27" s="59" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="28" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A28" s="44"/>
       <c r="B28" s="44"/>
       <c r="C28" s="44"/>
@@ -4519,8 +4637,11 @@
       <c r="AJ28" s="146" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="29" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="AK28" s="59" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="29" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A29" s="44"/>
       <c r="B29" s="44"/>
       <c r="C29" s="44"/>
@@ -4593,8 +4714,11 @@
       <c r="AJ29" s="110" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="30" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="AK29" s="59" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="30" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A30" s="44"/>
       <c r="B30" s="44"/>
       <c r="C30" s="44"/>
@@ -4663,8 +4787,11 @@
       <c r="AJ30" s="110" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="31" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="AK30" s="59" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="31" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A31" s="44"/>
       <c r="B31" s="44"/>
       <c r="C31" s="44"/>
@@ -4737,8 +4864,11 @@
       <c r="AJ31" s="110" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="32" spans="1:36" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="AK31" s="59" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="32" spans="1:37" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A32" s="44"/>
       <c r="B32" s="44"/>
       <c r="C32" s="44"/>
@@ -4820,7 +4950,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="33" spans="1:36" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:37" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A33" s="44"/>
       <c r="B33" s="44"/>
       <c r="C33" s="44"/>
@@ -4901,8 +5031,11 @@
       <c r="AJ33" s="110" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="34" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="AK33" s="59" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="34" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A34" s="44"/>
       <c r="B34" s="44"/>
       <c r="C34" s="44"/>
@@ -4958,8 +5091,11 @@
       <c r="AJ34" s="110" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="35" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="AK34" s="59" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="35" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A35" s="44"/>
       <c r="B35" s="44"/>
       <c r="C35" s="44"/>
@@ -4984,6 +5120,9 @@
       </c>
       <c r="W35" s="131"/>
       <c r="X35" s="131"/>
+      <c r="Y35" s="59" t="s">
+        <v>3</v>
+      </c>
       <c r="Z35" s="10"/>
       <c r="AA35" s="109" t="s">
         <v>19</v>
@@ -5013,8 +5152,14 @@
       <c r="AJ35" s="110" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="36" spans="1:36" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="AK35" s="59" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="36" spans="1:37" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="Y36" s="59" t="s">
+        <v>3</v>
+      </c>
       <c r="Z36" s="13"/>
       <c r="AA36" s="14"/>
       <c r="AB36" s="14"/>
@@ -5032,10 +5177,51 @@
       <c r="AJ36" s="112" t="s">
         <v>19</v>
       </c>
+      <c r="AK36" s="59" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="37" spans="1:37" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="Y37" s="59" t="s">
+        <v>3</v>
+      </c>
+      <c r="Z37" s="59" t="s">
+        <v>3</v>
+      </c>
+      <c r="AA37" s="59" t="s">
+        <v>3</v>
+      </c>
+      <c r="AB37" s="59" t="s">
+        <v>3</v>
+      </c>
+      <c r="AC37" s="59" t="s">
+        <v>3</v>
+      </c>
+      <c r="AD37" s="136" t="s">
+        <v>27</v>
+      </c>
+      <c r="AE37" s="137"/>
+      <c r="AF37" s="138"/>
+      <c r="AG37" s="59" t="s">
+        <v>3</v>
+      </c>
+      <c r="AH37" s="59" t="s">
+        <v>3</v>
+      </c>
+      <c r="AI37" s="59" t="s">
+        <v>3</v>
+      </c>
+      <c r="AJ37" s="59" t="s">
+        <v>3</v>
+      </c>
+      <c r="AK37" s="59" t="s">
+        <v>3</v>
+      </c>
     </row>
   </sheetData>
-  <mergeCells count="8">
+  <mergeCells count="9">
     <mergeCell ref="AB21:AD21"/>
+    <mergeCell ref="AD37:AF37"/>
     <mergeCell ref="V35:X35"/>
     <mergeCell ref="O1:Q1"/>
     <mergeCell ref="F16:H16"/>
@@ -5053,8 +5239,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="F2:Q20"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="L17" sqref="L17"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="O7" sqref="O7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5169,7 +5355,9 @@
       <c r="J8" s="140">
         <v>10</v>
       </c>
-      <c r="K8" s="121"/>
+      <c r="K8" s="140">
+        <v>11</v>
+      </c>
       <c r="L8" s="121"/>
       <c r="M8" s="121"/>
       <c r="N8" s="121"/>

</xml_diff>

<commit_message>
Implémentation niveau 11 buggé. TO DO: corriger le bug
</commit_message>
<xml_diff>
--- a/Niveaux.xlsx
+++ b/Niveaux.xlsx
@@ -4,20 +4,21 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="150" windowWidth="24915" windowHeight="12075" activeTab="3"/>
+    <workbookView xWindow="120" yWindow="150" windowWidth="24915" windowHeight="12075" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Niveau 1-5" sheetId="1" r:id="rId1"/>
     <sheet name="Niveau 6-10" sheetId="2" r:id="rId2"/>
     <sheet name="Tous_les_niveaux" sheetId="3" r:id="rId3"/>
     <sheet name="Carte des niveaux" sheetId="4" r:id="rId4"/>
+    <sheet name="Feuil2" sheetId="7" r:id="rId5"/>
   </sheets>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="927" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="978" uniqueCount="58">
   <si>
     <t>J</t>
   </si>
@@ -119,6 +120,78 @@
   </si>
   <si>
     <t>8 par 11</t>
+  </si>
+  <si>
+    <t>Statistiques du projet</t>
+  </si>
+  <si>
+    <t>Nombres de lignes de code</t>
+  </si>
+  <si>
+    <t>Classes =&gt;</t>
+  </si>
+  <si>
+    <t>Affichage</t>
+  </si>
+  <si>
+    <t>Bloc</t>
+  </si>
+  <si>
+    <t>Bouton</t>
+  </si>
+  <si>
+    <t>DangerElement</t>
+  </si>
+  <si>
+    <t>Déplacement</t>
+  </si>
+  <si>
+    <t>DonnéesMenu</t>
+  </si>
+  <si>
+    <t>DonneesNiveau</t>
+  </si>
+  <si>
+    <t>DonneesPubliques</t>
+  </si>
+  <si>
+    <t>Fonctions</t>
+  </si>
+  <si>
+    <t>Initialisations</t>
+  </si>
+  <si>
+    <t>Manivelle</t>
+  </si>
+  <si>
+    <t>Map</t>
+  </si>
+  <si>
+    <t>MapElement</t>
+  </si>
+  <si>
+    <t>Menu</t>
+  </si>
+  <si>
+    <t>MessageElement</t>
+  </si>
+  <si>
+    <t>Mur</t>
+  </si>
+  <si>
+    <t>Niveau</t>
+  </si>
+  <si>
+    <t>Porte</t>
+  </si>
+  <si>
+    <t>Program</t>
+  </si>
+  <si>
+    <t>SortieElement</t>
+  </si>
+  <si>
+    <t>Total</t>
   </si>
 </sst>
 </file>
@@ -524,7 +597,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="153">
+  <cellXfs count="161">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
@@ -960,6 +1033,26 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1263,8 +1356,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="C1:J46"/>
   <sheetViews>
-    <sheetView topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="I38" sqref="I38:I39"/>
+    <sheetView topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1283,7 +1376,9 @@
         <v>6</v>
       </c>
       <c r="D2" s="8"/>
-      <c r="E2" s="8"/>
+      <c r="E2" s="68" t="s">
+        <v>2</v>
+      </c>
       <c r="F2" s="8"/>
       <c r="G2" s="9"/>
       <c r="I2" s="85" t="s">
@@ -2960,10 +3055,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AK37"/>
+  <dimension ref="A1:AU37"/>
   <sheetViews>
-    <sheetView topLeftCell="U10" workbookViewId="0">
-      <selection activeCell="AI41" sqref="AI41"/>
+    <sheetView tabSelected="1" topLeftCell="AD10" workbookViewId="0">
+      <selection activeCell="AR44" sqref="AR44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3785,7 +3880,7 @@
       </c>
       <c r="AH16" s="143"/>
     </row>
-    <row r="17" spans="1:37" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:47" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="44"/>
       <c r="B17" s="44"/>
       <c r="C17" s="44"/>
@@ -3848,7 +3943,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="18" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A18" s="44"/>
       <c r="B18" s="44"/>
       <c r="C18" s="44"/>
@@ -3907,7 +4002,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="19" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A19" s="44"/>
       <c r="B19" s="44"/>
       <c r="C19" s="44"/>
@@ -3966,7 +4061,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="20" spans="1:37" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:47" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="44"/>
       <c r="B20" s="44"/>
       <c r="C20" s="44"/>
@@ -4047,7 +4142,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="21" spans="1:37" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:47" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="44"/>
       <c r="B21" s="44"/>
       <c r="C21" s="44"/>
@@ -4120,7 +4215,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="22" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A22" s="44"/>
       <c r="B22" s="44"/>
       <c r="C22" s="44"/>
@@ -4191,7 +4286,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="23" spans="1:37" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:47" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="44"/>
       <c r="B23" s="44"/>
       <c r="C23" s="44"/>
@@ -4260,7 +4355,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="24" spans="1:37" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:47" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A24" s="44"/>
       <c r="B24" s="44"/>
       <c r="C24" s="44"/>
@@ -4339,7 +4434,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="25" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A25" s="44"/>
       <c r="B25" s="44"/>
       <c r="C25" s="44"/>
@@ -4412,7 +4507,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="26" spans="1:37" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:47" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A26" s="44"/>
       <c r="B26" s="44"/>
       <c r="C26" s="44"/>
@@ -4483,7 +4578,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="27" spans="1:37" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:47" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A27" s="44"/>
       <c r="B27" s="44"/>
       <c r="C27" s="44"/>
@@ -4576,7 +4671,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="28" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A28" s="44"/>
       <c r="B28" s="44"/>
       <c r="C28" s="44"/>
@@ -4641,7 +4736,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="29" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:47" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A29" s="44"/>
       <c r="B29" s="44"/>
       <c r="C29" s="44"/>
@@ -4717,8 +4812,38 @@
       <c r="AK29" s="59" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="30" spans="1:37" x14ac:dyDescent="0.25">
+      <c r="AL29" s="59" t="s">
+        <v>3</v>
+      </c>
+      <c r="AM29" s="59" t="s">
+        <v>3</v>
+      </c>
+      <c r="AN29" s="59" t="s">
+        <v>3</v>
+      </c>
+      <c r="AO29" s="59" t="s">
+        <v>3</v>
+      </c>
+      <c r="AP29" s="59" t="s">
+        <v>3</v>
+      </c>
+      <c r="AQ29" s="59" t="s">
+        <v>3</v>
+      </c>
+      <c r="AR29" s="59" t="s">
+        <v>3</v>
+      </c>
+      <c r="AS29" s="59" t="s">
+        <v>3</v>
+      </c>
+      <c r="AT29" s="59" t="s">
+        <v>3</v>
+      </c>
+      <c r="AU29" s="59" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="30" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A30" s="44"/>
       <c r="B30" s="44"/>
       <c r="C30" s="44"/>
@@ -4790,8 +4915,20 @@
       <c r="AK30" s="59" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="31" spans="1:37" x14ac:dyDescent="0.25">
+      <c r="AL30" s="115"/>
+      <c r="AM30" s="8"/>
+      <c r="AN30" s="8"/>
+      <c r="AO30" s="8"/>
+      <c r="AP30" s="8"/>
+      <c r="AQ30" s="8"/>
+      <c r="AR30" s="8"/>
+      <c r="AS30" s="8"/>
+      <c r="AT30" s="9"/>
+      <c r="AU30" s="59" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="31" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A31" s="44"/>
       <c r="B31" s="44"/>
       <c r="C31" s="44"/>
@@ -4867,8 +5004,20 @@
       <c r="AK31" s="59" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="32" spans="1:37" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="AL31" s="10"/>
+      <c r="AM31" s="11"/>
+      <c r="AN31" s="11"/>
+      <c r="AO31" s="11"/>
+      <c r="AP31" s="11"/>
+      <c r="AQ31" s="11"/>
+      <c r="AR31" s="11"/>
+      <c r="AS31" s="11"/>
+      <c r="AT31" s="12"/>
+      <c r="AU31" s="59" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="32" spans="1:47" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A32" s="44"/>
       <c r="B32" s="44"/>
       <c r="C32" s="44"/>
@@ -4946,11 +5095,26 @@
       <c r="AI32" s="109" t="s">
         <v>19</v>
       </c>
-      <c r="AJ32" s="147" t="s">
+      <c r="AJ32" s="159" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="33" spans="1:37" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="AK32" s="135"/>
+      <c r="AL32" s="104" t="s">
+        <v>0</v>
+      </c>
+      <c r="AM32" s="11"/>
+      <c r="AN32" s="11"/>
+      <c r="AO32" s="11"/>
+      <c r="AP32" s="11"/>
+      <c r="AQ32" s="11"/>
+      <c r="AR32" s="11"/>
+      <c r="AS32" s="11"/>
+      <c r="AT32" s="12"/>
+      <c r="AU32" s="59" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="33" spans="1:47" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A33" s="44"/>
       <c r="B33" s="44"/>
       <c r="C33" s="44"/>
@@ -5034,8 +5198,20 @@
       <c r="AK33" s="59" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="34" spans="1:37" x14ac:dyDescent="0.25">
+      <c r="AL33" s="10"/>
+      <c r="AM33" s="11"/>
+      <c r="AN33" s="11"/>
+      <c r="AO33" s="11"/>
+      <c r="AP33" s="11"/>
+      <c r="AQ33" s="11"/>
+      <c r="AR33" s="11"/>
+      <c r="AS33" s="11"/>
+      <c r="AT33" s="12"/>
+      <c r="AU33" s="59" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="34" spans="1:47" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A34" s="44"/>
       <c r="B34" s="44"/>
       <c r="C34" s="44"/>
@@ -5094,8 +5270,22 @@
       <c r="AK34" s="59" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="35" spans="1:37" x14ac:dyDescent="0.25">
+      <c r="AL34" s="13"/>
+      <c r="AM34" s="14"/>
+      <c r="AN34" s="14"/>
+      <c r="AO34" s="14"/>
+      <c r="AP34" s="14"/>
+      <c r="AQ34" s="14"/>
+      <c r="AR34" s="14"/>
+      <c r="AS34" s="14"/>
+      <c r="AT34" s="160" t="s">
+        <v>6</v>
+      </c>
+      <c r="AU34" s="59" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="35" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A35" s="44"/>
       <c r="B35" s="44"/>
       <c r="C35" s="44"/>
@@ -5155,8 +5345,35 @@
       <c r="AK35" s="59" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="36" spans="1:37" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="AL35" s="59" t="s">
+        <v>3</v>
+      </c>
+      <c r="AM35" s="59" t="s">
+        <v>3</v>
+      </c>
+      <c r="AN35" s="59" t="s">
+        <v>3</v>
+      </c>
+      <c r="AO35" s="59" t="s">
+        <v>3</v>
+      </c>
+      <c r="AP35" s="59" t="s">
+        <v>3</v>
+      </c>
+      <c r="AQ35" s="59" t="s">
+        <v>3</v>
+      </c>
+      <c r="AR35" s="59" t="s">
+        <v>3</v>
+      </c>
+      <c r="AS35" s="59" t="s">
+        <v>3</v>
+      </c>
+      <c r="AU35" s="59" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="36" spans="1:47" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="Y36" s="59" t="s">
         <v>3</v>
       </c>
@@ -5181,7 +5398,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="37" spans="1:37" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:47" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="Y37" s="59" t="s">
         <v>3</v>
       </c>
@@ -5239,7 +5456,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="F2:Q20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="O7" sqref="O7"/>
     </sheetView>
   </sheetViews>
@@ -5536,4 +5753,185 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:V4"/>
+  <sheetViews>
+    <sheetView topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="B10" sqref="B10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="25.5703125" customWidth="1"/>
+    <col min="5" max="5" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="15.140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="17.85546875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="13" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="16.28515625" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="13.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="153" t="s">
+        <v>34</v>
+      </c>
+      <c r="B1" s="154"/>
+      <c r="C1" s="154"/>
+      <c r="D1" s="155"/>
+    </row>
+    <row r="2" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A2" s="157"/>
+      <c r="B2" s="157"/>
+      <c r="C2" s="157"/>
+      <c r="D2" s="157"/>
+    </row>
+    <row r="3" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A3" s="156" t="s">
+        <v>36</v>
+      </c>
+      <c r="B3" s="156" t="s">
+        <v>37</v>
+      </c>
+      <c r="C3" s="156" t="s">
+        <v>38</v>
+      </c>
+      <c r="D3" s="156" t="s">
+        <v>39</v>
+      </c>
+      <c r="E3" s="156" t="s">
+        <v>40</v>
+      </c>
+      <c r="F3" s="156" t="s">
+        <v>41</v>
+      </c>
+      <c r="G3" s="156" t="s">
+        <v>42</v>
+      </c>
+      <c r="H3" s="156" t="s">
+        <v>43</v>
+      </c>
+      <c r="I3" s="156" t="s">
+        <v>44</v>
+      </c>
+      <c r="J3" s="156" t="s">
+        <v>45</v>
+      </c>
+      <c r="K3" s="156" t="s">
+        <v>46</v>
+      </c>
+      <c r="L3" s="156" t="s">
+        <v>47</v>
+      </c>
+      <c r="M3" s="156" t="s">
+        <v>48</v>
+      </c>
+      <c r="N3" s="156" t="s">
+        <v>49</v>
+      </c>
+      <c r="O3" s="156" t="s">
+        <v>50</v>
+      </c>
+      <c r="P3" s="156" t="s">
+        <v>51</v>
+      </c>
+      <c r="Q3" s="156" t="s">
+        <v>52</v>
+      </c>
+      <c r="R3" s="156" t="s">
+        <v>53</v>
+      </c>
+      <c r="S3" s="156" t="s">
+        <v>54</v>
+      </c>
+      <c r="T3" s="156" t="s">
+        <v>55</v>
+      </c>
+      <c r="U3" s="156" t="s">
+        <v>56</v>
+      </c>
+      <c r="V3" s="156" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="4" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A4" s="156" t="s">
+        <v>35</v>
+      </c>
+      <c r="B4" s="156">
+        <v>522</v>
+      </c>
+      <c r="C4" s="156">
+        <v>54</v>
+      </c>
+      <c r="D4" s="156">
+        <v>82</v>
+      </c>
+      <c r="E4" s="156">
+        <v>28</v>
+      </c>
+      <c r="F4" s="156">
+        <v>347</v>
+      </c>
+      <c r="G4" s="156">
+        <v>342</v>
+      </c>
+      <c r="H4" s="156">
+        <v>352</v>
+      </c>
+      <c r="I4" s="156">
+        <v>39</v>
+      </c>
+      <c r="J4" s="156">
+        <v>600</v>
+      </c>
+      <c r="K4" s="156">
+        <v>927</v>
+      </c>
+      <c r="L4" s="156">
+        <v>115</v>
+      </c>
+      <c r="M4" s="156">
+        <v>92</v>
+      </c>
+      <c r="N4" s="156">
+        <v>137</v>
+      </c>
+      <c r="O4" s="156">
+        <v>96</v>
+      </c>
+      <c r="P4" s="156">
+        <v>97</v>
+      </c>
+      <c r="Q4" s="156">
+        <v>71</v>
+      </c>
+      <c r="R4" s="156">
+        <v>248</v>
+      </c>
+      <c r="S4" s="156">
+        <v>144</v>
+      </c>
+      <c r="T4" s="156">
+        <v>33</v>
+      </c>
+      <c r="U4" s="156">
+        <v>40</v>
+      </c>
+      <c r="V4" s="158">
+        <f>SUM(B4:U4)</f>
+        <v>4366</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:D1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Fin du niveau 12
</commit_message>
<xml_diff>
--- a/Niveaux.xlsx
+++ b/Niveaux.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="150" windowWidth="24915" windowHeight="12075" activeTab="4"/>
+    <workbookView xWindow="120" yWindow="150" windowWidth="24915" windowHeight="12075" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Niveau 1-5" sheetId="1" r:id="rId1"/>
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1229" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1339" uniqueCount="70">
   <si>
     <t>J</t>
   </si>
@@ -211,12 +211,30 @@
   <si>
     <t xml:space="preserve"> </t>
   </si>
+  <si>
+    <t>B1</t>
+  </si>
+  <si>
+    <t>B2</t>
+  </si>
+  <si>
+    <t>B3</t>
+  </si>
+  <si>
+    <t>P4</t>
+  </si>
+  <si>
+    <t>B4</t>
+  </si>
+  <si>
+    <t>b4</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="12" x14ac:knownFonts="1">
+  <fonts count="14" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -306,6 +324,22 @@
     <font>
       <sz val="11"/>
       <color rgb="FFC00000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF0070C0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="9" tint="-0.499984740745262"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -615,7 +649,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="162">
+  <cellXfs count="174">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
@@ -964,46 +998,10 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1029,28 +1027,10 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1062,6 +1042,54 @@
     <xf numFmtId="0" fontId="5" fillId="6" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1071,8 +1099,50 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1384,13 +1454,13 @@
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="3:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C1" s="122" t="s">
+      <c r="C1" s="141" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="123"/>
-      <c r="E1" s="123"/>
-      <c r="F1" s="123"/>
-      <c r="G1" s="124"/>
+      <c r="D1" s="142"/>
+      <c r="E1" s="142"/>
+      <c r="F1" s="142"/>
+      <c r="G1" s="143"/>
     </row>
     <row r="2" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C2" s="35" t="s">
@@ -1461,13 +1531,13 @@
     </row>
     <row r="8" spans="3:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="9" spans="3:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C9" s="122" t="s">
+      <c r="C9" s="141" t="s">
         <v>4</v>
       </c>
-      <c r="D9" s="123"/>
-      <c r="E9" s="123"/>
-      <c r="F9" s="123"/>
-      <c r="G9" s="124"/>
+      <c r="D9" s="142"/>
+      <c r="E9" s="142"/>
+      <c r="F9" s="142"/>
+      <c r="G9" s="143"/>
     </row>
     <row r="10" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C10" s="34" t="s">
@@ -1538,14 +1608,14 @@
     </row>
     <row r="16" spans="3:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="17" spans="3:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C17" s="125" t="s">
+      <c r="C17" s="144" t="s">
         <v>7</v>
       </c>
-      <c r="D17" s="126"/>
-      <c r="E17" s="126"/>
-      <c r="F17" s="126"/>
-      <c r="G17" s="126"/>
-      <c r="H17" s="127"/>
+      <c r="D17" s="145"/>
+      <c r="E17" s="145"/>
+      <c r="F17" s="145"/>
+      <c r="G17" s="145"/>
+      <c r="H17" s="146"/>
     </row>
     <row r="18" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C18" s="21"/>
@@ -1651,13 +1721,13 @@
     </row>
     <row r="25" spans="3:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="26" spans="3:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C26" s="122" t="s">
+      <c r="C26" s="141" t="s">
         <v>10</v>
       </c>
-      <c r="D26" s="123"/>
-      <c r="E26" s="123"/>
-      <c r="F26" s="123"/>
-      <c r="G26" s="124"/>
+      <c r="D26" s="142"/>
+      <c r="E26" s="142"/>
+      <c r="F26" s="142"/>
+      <c r="G26" s="143"/>
     </row>
     <row r="27" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C27" s="63" t="s">
@@ -1763,13 +1833,13 @@
     </row>
     <row r="36" spans="3:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="37" spans="3:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C37" s="122" t="s">
+      <c r="C37" s="141" t="s">
         <v>11</v>
       </c>
-      <c r="D37" s="123"/>
-      <c r="E37" s="123"/>
-      <c r="F37" s="123"/>
-      <c r="G37" s="124"/>
+      <c r="D37" s="142"/>
+      <c r="E37" s="142"/>
+      <c r="F37" s="142"/>
+      <c r="G37" s="143"/>
     </row>
     <row r="38" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C38" s="83" t="s">
@@ -1907,17 +1977,17 @@
   <sheetData>
     <row r="2" spans="3:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="3" spans="3:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C3" s="122" t="s">
+      <c r="C3" s="141" t="s">
         <v>17</v>
       </c>
-      <c r="D3" s="123"/>
-      <c r="E3" s="123"/>
-      <c r="F3" s="123"/>
-      <c r="G3" s="123"/>
-      <c r="H3" s="123"/>
-      <c r="I3" s="123"/>
-      <c r="J3" s="123"/>
-      <c r="K3" s="124"/>
+      <c r="D3" s="142"/>
+      <c r="E3" s="142"/>
+      <c r="F3" s="142"/>
+      <c r="G3" s="142"/>
+      <c r="H3" s="142"/>
+      <c r="I3" s="142"/>
+      <c r="J3" s="142"/>
+      <c r="K3" s="143"/>
     </row>
     <row r="4" spans="3:13" x14ac:dyDescent="0.25">
       <c r="C4" s="87" t="s">
@@ -2115,11 +2185,11 @@
     </row>
     <row r="13" spans="3:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="14" spans="3:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C14" s="128" t="s">
+      <c r="C14" s="147" t="s">
         <v>20</v>
       </c>
-      <c r="D14" s="129"/>
-      <c r="E14" s="130"/>
+      <c r="D14" s="148"/>
+      <c r="E14" s="149"/>
     </row>
     <row r="15" spans="3:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C15" s="107" t="s">
@@ -2231,15 +2301,15 @@
     </row>
     <row r="28" spans="3:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="29" spans="3:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C29" s="128" t="s">
+      <c r="C29" s="147" t="s">
         <v>22</v>
       </c>
-      <c r="D29" s="129"/>
-      <c r="E29" s="129"/>
-      <c r="F29" s="129"/>
-      <c r="G29" s="129"/>
-      <c r="H29" s="129"/>
-      <c r="I29" s="130"/>
+      <c r="D29" s="148"/>
+      <c r="E29" s="148"/>
+      <c r="F29" s="148"/>
+      <c r="G29" s="148"/>
+      <c r="H29" s="148"/>
+      <c r="I29" s="149"/>
     </row>
     <row r="30" spans="3:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C30" s="115"/>
@@ -2389,18 +2459,18 @@
     </row>
     <row r="40" spans="3:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="41" spans="3:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C41" s="122" t="s">
+      <c r="C41" s="141" t="s">
         <v>25</v>
       </c>
-      <c r="D41" s="123"/>
-      <c r="E41" s="123"/>
-      <c r="F41" s="123"/>
-      <c r="G41" s="123"/>
-      <c r="H41" s="123"/>
-      <c r="I41" s="124"/>
+      <c r="D41" s="142"/>
+      <c r="E41" s="142"/>
+      <c r="F41" s="142"/>
+      <c r="G41" s="142"/>
+      <c r="H41" s="142"/>
+      <c r="I41" s="143"/>
     </row>
     <row r="42" spans="3:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C42" s="136" t="s">
+      <c r="C42" s="124" t="s">
         <v>0</v>
       </c>
       <c r="D42" s="117" t="s">
@@ -2412,7 +2482,7 @@
       <c r="H42" s="117" t="s">
         <v>19</v>
       </c>
-      <c r="I42" s="138" t="s">
+      <c r="I42" s="126" t="s">
         <v>24</v>
       </c>
     </row>
@@ -2484,18 +2554,18 @@
     </row>
     <row r="48" spans="3:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="49" spans="3:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C49" s="122" t="s">
+      <c r="C49" s="141" t="s">
         <v>26</v>
       </c>
-      <c r="D49" s="123"/>
-      <c r="E49" s="123"/>
-      <c r="F49" s="123"/>
-      <c r="G49" s="123"/>
-      <c r="H49" s="123"/>
-      <c r="I49" s="124"/>
+      <c r="D49" s="142"/>
+      <c r="E49" s="142"/>
+      <c r="F49" s="142"/>
+      <c r="G49" s="142"/>
+      <c r="H49" s="142"/>
+      <c r="I49" s="143"/>
     </row>
     <row r="50" spans="3:15" x14ac:dyDescent="0.25">
-      <c r="C50" s="136" t="s">
+      <c r="C50" s="124" t="s">
         <v>0</v>
       </c>
       <c r="D50" s="117" t="s">
@@ -2507,7 +2577,7 @@
       <c r="H50" s="117" t="s">
         <v>19</v>
       </c>
-      <c r="I50" s="138" t="s">
+      <c r="I50" s="126" t="s">
         <v>24</v>
       </c>
     </row>
@@ -2573,22 +2643,22 @@
     </row>
     <row r="56" spans="3:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="57" spans="3:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C57" s="128" t="s">
+      <c r="C57" s="147" t="s">
         <v>27</v>
       </c>
-      <c r="D57" s="129"/>
-      <c r="E57" s="129"/>
-      <c r="F57" s="129"/>
-      <c r="G57" s="129"/>
-      <c r="H57" s="129"/>
-      <c r="I57" s="129"/>
-      <c r="J57" s="129"/>
-      <c r="K57" s="129"/>
-      <c r="L57" s="129"/>
-      <c r="M57" s="130"/>
+      <c r="D57" s="148"/>
+      <c r="E57" s="148"/>
+      <c r="F57" s="148"/>
+      <c r="G57" s="148"/>
+      <c r="H57" s="148"/>
+      <c r="I57" s="148"/>
+      <c r="J57" s="148"/>
+      <c r="K57" s="148"/>
+      <c r="L57" s="148"/>
+      <c r="M57" s="149"/>
     </row>
     <row r="58" spans="3:15" x14ac:dyDescent="0.25">
-      <c r="C58" s="136" t="s">
+      <c r="C58" s="124" t="s">
         <v>0</v>
       </c>
       <c r="D58" s="117" t="s">
@@ -2604,7 +2674,7 @@
       <c r="L58" s="117" t="s">
         <v>19</v>
       </c>
-      <c r="M58" s="143" t="s">
+      <c r="M58" s="131" t="s">
         <v>19</v>
       </c>
     </row>
@@ -2710,18 +2780,18 @@
       <c r="J62" s="109" t="s">
         <v>19</v>
       </c>
-      <c r="K62" s="142" t="s">
+      <c r="K62" s="130" t="s">
         <v>2</v>
       </c>
       <c r="L62" s="109" t="s">
         <v>19</v>
       </c>
-      <c r="M62" s="144" t="s">
+      <c r="M62" s="132" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="63" spans="3:15" x14ac:dyDescent="0.25">
-      <c r="C63" s="141" t="s">
+      <c r="C63" s="129" t="s">
         <v>2</v>
       </c>
       <c r="D63" s="109" t="s">
@@ -2821,28 +2891,28 @@
       </c>
     </row>
     <row r="67" spans="3:13" x14ac:dyDescent="0.25">
-      <c r="H67" s="149"/>
+      <c r="H67" s="134"/>
     </row>
     <row r="68" spans="3:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="H68" s="149"/>
+      <c r="H68" s="134"/>
     </row>
     <row r="69" spans="3:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C69" s="145" t="s">
+      <c r="C69" s="150" t="s">
         <v>28</v>
       </c>
-      <c r="D69" s="146"/>
-      <c r="E69" s="146"/>
-      <c r="F69" s="146"/>
-      <c r="G69" s="146"/>
-      <c r="H69" s="146"/>
-      <c r="I69" s="146"/>
-      <c r="J69" s="146"/>
-      <c r="K69" s="146"/>
-      <c r="L69" s="146"/>
-      <c r="M69" s="147"/>
+      <c r="D69" s="151"/>
+      <c r="E69" s="151"/>
+      <c r="F69" s="151"/>
+      <c r="G69" s="151"/>
+      <c r="H69" s="151"/>
+      <c r="I69" s="151"/>
+      <c r="J69" s="151"/>
+      <c r="K69" s="151"/>
+      <c r="L69" s="151"/>
+      <c r="M69" s="152"/>
     </row>
     <row r="70" spans="3:13" x14ac:dyDescent="0.25">
-      <c r="C70" s="136" t="s">
+      <c r="C70" s="124" t="s">
         <v>0</v>
       </c>
       <c r="D70" s="117" t="s">
@@ -2864,7 +2934,7 @@
       <c r="J70" s="8"/>
       <c r="K70" s="2"/>
       <c r="L70" s="117"/>
-      <c r="M70" s="143" t="s">
+      <c r="M70" s="131" t="s">
         <v>19</v>
       </c>
     </row>
@@ -2958,18 +3028,18 @@
       <c r="J74" s="109" t="s">
         <v>19</v>
       </c>
-      <c r="K74" s="142" t="s">
+      <c r="K74" s="130" t="s">
         <v>2</v>
       </c>
       <c r="L74" s="11" t="s">
         <v>32</v>
       </c>
-      <c r="M74" s="144" t="s">
+      <c r="M74" s="132" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="75" spans="3:13" x14ac:dyDescent="0.25">
-      <c r="C75" s="141" t="s">
+      <c r="C75" s="129" t="s">
         <v>2</v>
       </c>
       <c r="D75" s="109" t="s">
@@ -3053,7 +3123,7 @@
         <v>19</v>
       </c>
       <c r="K78" s="6"/>
-      <c r="L78" s="148" t="s">
+      <c r="L78" s="133" t="s">
         <v>31</v>
       </c>
       <c r="M78" s="112" t="s">
@@ -3076,25 +3146,25 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AU37"/>
+  <dimension ref="A1:AU54"/>
   <sheetViews>
-    <sheetView topLeftCell="AB16" workbookViewId="0">
-      <selection activeCell="AL34" sqref="AL34"/>
+    <sheetView tabSelected="1" topLeftCell="AB22" workbookViewId="0">
+      <selection activeCell="AS42" sqref="AS42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:34" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="O1" s="128" t="s">
+      <c r="O1" s="147" t="s">
         <v>4</v>
       </c>
-      <c r="P1" s="129"/>
-      <c r="Q1" s="130"/>
-      <c r="U1" s="128" t="s">
+      <c r="P1" s="148"/>
+      <c r="Q1" s="149"/>
+      <c r="U1" s="147" t="s">
         <v>1</v>
       </c>
-      <c r="V1" s="129"/>
-      <c r="W1" s="130"/>
+      <c r="V1" s="148"/>
+      <c r="W1" s="149"/>
     </row>
     <row r="2" spans="1:34" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="E2" s="59" t="s">
@@ -3439,11 +3509,11 @@
       <c r="I7" s="59" t="s">
         <v>3</v>
       </c>
-      <c r="J7" s="122" t="s">
+      <c r="J7" s="141" t="s">
         <v>7</v>
       </c>
-      <c r="K7" s="123"/>
-      <c r="L7" s="124"/>
+      <c r="K7" s="142"/>
+      <c r="L7" s="143"/>
       <c r="M7" s="58" t="s">
         <v>3</v>
       </c>
@@ -3814,11 +3884,11 @@
       <c r="U12" s="59" t="s">
         <v>3</v>
       </c>
-      <c r="V12" s="133" t="s">
+      <c r="V12" s="153" t="s">
         <v>22</v>
       </c>
-      <c r="W12" s="134"/>
-      <c r="X12" s="135"/>
+      <c r="W12" s="154"/>
+      <c r="X12" s="155"/>
       <c r="Y12" s="59" t="s">
         <v>3</v>
       </c>
@@ -4036,11 +4106,11 @@
       <c r="E16" s="59" t="s">
         <v>3</v>
       </c>
-      <c r="F16" s="122" t="s">
+      <c r="F16" s="141" t="s">
         <v>11</v>
       </c>
-      <c r="G16" s="123"/>
-      <c r="H16" s="124"/>
+      <c r="G16" s="142"/>
+      <c r="H16" s="143"/>
       <c r="I16" s="59" t="s">
         <v>3</v>
       </c>
@@ -4094,7 +4164,7 @@
       <c r="AA16" s="59" t="s">
         <v>3</v>
       </c>
-      <c r="AH16" s="140"/>
+      <c r="AH16" s="128"/>
     </row>
     <row r="17" spans="1:47" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="44"/>
@@ -4333,7 +4403,7 @@
       <c r="Y20" s="120" t="s">
         <v>2</v>
       </c>
-      <c r="Z20" s="131" t="s">
+      <c r="Z20" s="122" t="s">
         <v>6</v>
       </c>
       <c r="AA20" s="59" t="s">
@@ -4454,15 +4524,15 @@
       <c r="Y21" s="59" t="s">
         <v>3</v>
       </c>
-      <c r="Z21" s="132"/>
+      <c r="Z21" s="123"/>
       <c r="AA21" s="59" t="s">
         <v>3</v>
       </c>
-      <c r="AB21" s="122" t="s">
+      <c r="AB21" s="141" t="s">
         <v>25</v>
       </c>
-      <c r="AC21" s="123"/>
-      <c r="AD21" s="124"/>
+      <c r="AC21" s="142"/>
+      <c r="AD21" s="143"/>
       <c r="AE21" s="59" t="s">
         <v>3</v>
       </c>
@@ -4567,7 +4637,7 @@
       <c r="Y22" s="59" t="s">
         <v>3</v>
       </c>
-      <c r="Z22" s="136" t="s">
+      <c r="Z22" s="124" t="s">
         <v>0</v>
       </c>
       <c r="AA22" s="117" t="s">
@@ -4579,7 +4649,7 @@
       <c r="AE22" s="117" t="s">
         <v>19</v>
       </c>
-      <c r="AF22" s="138" t="s">
+      <c r="AF22" s="126" t="s">
         <v>24</v>
       </c>
       <c r="AG22" s="59" t="s">
@@ -5027,7 +5097,7 @@
       <c r="Y26" s="59" t="s">
         <v>3</v>
       </c>
-      <c r="Z26" s="139" t="s">
+      <c r="Z26" s="127" t="s">
         <v>6</v>
       </c>
       <c r="AA26" s="14"/>
@@ -5146,7 +5216,7 @@
       <c r="Y27" s="59" t="s">
         <v>3</v>
       </c>
-      <c r="Z27" s="132"/>
+      <c r="Z27" s="123"/>
       <c r="AA27" s="59" t="s">
         <v>3</v>
       </c>
@@ -5265,7 +5335,7 @@
       <c r="Y28" s="59" t="s">
         <v>3</v>
       </c>
-      <c r="Z28" s="136" t="s">
+      <c r="Z28" s="124" t="s">
         <v>0</v>
       </c>
       <c r="AA28" s="117" t="s">
@@ -5281,7 +5351,7 @@
       <c r="AI28" s="117" t="s">
         <v>19</v>
       </c>
-      <c r="AJ28" s="143" t="s">
+      <c r="AJ28" s="131" t="s">
         <v>19</v>
       </c>
       <c r="AK28" s="59" t="s">
@@ -5415,11 +5485,11 @@
       <c r="AN29" s="59" t="s">
         <v>3</v>
       </c>
-      <c r="AO29" s="133" t="s">
+      <c r="AO29" s="153" t="s">
         <v>60</v>
       </c>
-      <c r="AP29" s="134"/>
-      <c r="AQ29" s="135"/>
+      <c r="AP29" s="154"/>
+      <c r="AQ29" s="155"/>
       <c r="AR29" s="59" t="s">
         <v>3</v>
       </c>
@@ -5693,16 +5763,16 @@
       <c r="AG32" s="109" t="s">
         <v>19</v>
       </c>
-      <c r="AH32" s="142" t="s">
+      <c r="AH32" s="130" t="s">
         <v>2</v>
       </c>
       <c r="AI32" s="109" t="s">
         <v>19</v>
       </c>
-      <c r="AJ32" s="156" t="s">
+      <c r="AJ32" s="138" t="s">
         <v>6</v>
       </c>
-      <c r="AK32" s="132"/>
+      <c r="AK32" s="123"/>
       <c r="AL32" s="104" t="s">
         <v>0</v>
       </c>
@@ -5747,11 +5817,11 @@
       <c r="N33" s="59" t="s">
         <v>3</v>
       </c>
-      <c r="O33" s="158" t="s">
+      <c r="O33" s="156" t="s">
         <v>17</v>
       </c>
-      <c r="P33" s="159"/>
-      <c r="Q33" s="160"/>
+      <c r="P33" s="157"/>
+      <c r="Q33" s="158"/>
       <c r="R33" s="59" t="s">
         <v>3</v>
       </c>
@@ -5774,7 +5844,7 @@
       <c r="Y33" s="59" t="s">
         <v>3</v>
       </c>
-      <c r="Z33" s="141" t="s">
+      <c r="Z33" s="129" t="s">
         <v>2</v>
       </c>
       <c r="AA33" s="109" t="s">
@@ -5867,11 +5937,11 @@
       <c r="U34" s="59" t="s">
         <v>3</v>
       </c>
-      <c r="V34" s="122" t="s">
+      <c r="V34" s="141" t="s">
         <v>20</v>
       </c>
-      <c r="W34" s="123"/>
-      <c r="X34" s="124"/>
+      <c r="W34" s="142"/>
+      <c r="X34" s="143"/>
       <c r="Y34" s="59" t="s">
         <v>3</v>
       </c>
@@ -5897,32 +5967,32 @@
       <c r="AK34" s="59" t="s">
         <v>3</v>
       </c>
-      <c r="AL34" s="161" t="s">
+      <c r="AL34" s="140" t="s">
         <v>2</v>
       </c>
       <c r="AM34" s="14" t="s">
         <v>32</v>
       </c>
-      <c r="AN34" s="148" t="s">
+      <c r="AN34" s="133" t="s">
         <v>33</v>
       </c>
       <c r="AO34" s="14"/>
       <c r="AP34" s="14"/>
-      <c r="AQ34" s="148" t="s">
+      <c r="AQ34" s="133" t="s">
         <v>62</v>
       </c>
       <c r="AR34" s="14"/>
       <c r="AS34" s="14" t="s">
         <v>61</v>
       </c>
-      <c r="AT34" s="157" t="s">
+      <c r="AT34" s="139" t="s">
         <v>6</v>
       </c>
       <c r="AU34" s="59" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="35" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:47" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A35" s="44"/>
       <c r="B35" s="44"/>
       <c r="C35" s="44"/>
@@ -6013,7 +6083,7 @@
       <c r="AS35" s="59" t="s">
         <v>3</v>
       </c>
-      <c r="AT35" s="132"/>
+      <c r="AT35" s="123"/>
       <c r="AU35" s="59" t="s">
         <v>3</v>
       </c>
@@ -6054,7 +6124,23 @@
       <c r="AK36" s="59" t="s">
         <v>3</v>
       </c>
-      <c r="AT36" s="132"/>
+      <c r="AL36" s="115"/>
+      <c r="AM36" s="8"/>
+      <c r="AN36" s="8"/>
+      <c r="AO36" s="8"/>
+      <c r="AP36" s="68" t="s">
+        <v>2</v>
+      </c>
+      <c r="AQ36" s="117" t="s">
+        <v>19</v>
+      </c>
+      <c r="AR36" s="117" t="s">
+        <v>19</v>
+      </c>
+      <c r="AS36" s="8"/>
+      <c r="AT36" s="167" t="s">
+        <v>0</v>
+      </c>
     </row>
     <row r="37" spans="1:47" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="U37" s="59" t="s">
@@ -6084,11 +6170,11 @@
       <c r="AC37" s="59" t="s">
         <v>3</v>
       </c>
-      <c r="AD37" s="133" t="s">
+      <c r="AD37" s="153" t="s">
         <v>27</v>
       </c>
-      <c r="AE37" s="134"/>
-      <c r="AF37" s="135"/>
+      <c r="AE37" s="154"/>
+      <c r="AF37" s="155"/>
       <c r="AG37" s="59" t="s">
         <v>3</v>
       </c>
@@ -6103,20 +6189,463 @@
       </c>
       <c r="AK37" s="59" t="s">
         <v>3</v>
+      </c>
+      <c r="AL37" s="10"/>
+      <c r="AM37" s="11"/>
+      <c r="AN37" s="11"/>
+      <c r="AO37" s="11"/>
+      <c r="AP37" s="11"/>
+      <c r="AQ37" s="65" t="s">
+        <v>33</v>
+      </c>
+      <c r="AR37" s="109" t="s">
+        <v>19</v>
+      </c>
+      <c r="AS37" s="11"/>
+      <c r="AT37" s="69" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="38" spans="1:47" x14ac:dyDescent="0.25">
+      <c r="AG38" s="59" t="s">
+        <v>3</v>
+      </c>
+      <c r="AH38" s="59" t="s">
+        <v>3</v>
+      </c>
+      <c r="AI38" s="59" t="s">
+        <v>3</v>
+      </c>
+      <c r="AJ38" s="59" t="s">
+        <v>3</v>
+      </c>
+      <c r="AK38" s="59" t="s">
+        <v>3</v>
+      </c>
+      <c r="AL38" s="10"/>
+      <c r="AM38" s="11"/>
+      <c r="AN38" s="11"/>
+      <c r="AO38" s="109" t="s">
+        <v>19</v>
+      </c>
+      <c r="AP38" s="109" t="s">
+        <v>19</v>
+      </c>
+      <c r="AQ38" s="109" t="s">
+        <v>19</v>
+      </c>
+      <c r="AR38" s="109" t="s">
+        <v>19</v>
+      </c>
+      <c r="AS38" s="11"/>
+      <c r="AT38" s="12"/>
+    </row>
+    <row r="39" spans="1:47" x14ac:dyDescent="0.25">
+      <c r="AG39" s="59" t="s">
+        <v>3</v>
+      </c>
+      <c r="AH39" s="59" t="s">
+        <v>3</v>
+      </c>
+      <c r="AI39" s="59" t="s">
+        <v>3</v>
+      </c>
+      <c r="AJ39" s="59" t="s">
+        <v>3</v>
+      </c>
+      <c r="AK39" s="59" t="s">
+        <v>3</v>
+      </c>
+      <c r="AL39" s="70" t="s">
+        <v>2</v>
+      </c>
+      <c r="AM39" s="109" t="s">
+        <v>19</v>
+      </c>
+      <c r="AN39" s="11"/>
+      <c r="AO39" s="109" t="s">
+        <v>19</v>
+      </c>
+      <c r="AP39" s="11"/>
+      <c r="AQ39" s="11"/>
+      <c r="AR39" s="65" t="s">
+        <v>64</v>
+      </c>
+      <c r="AS39" s="11"/>
+      <c r="AT39" s="12"/>
+    </row>
+    <row r="40" spans="1:47" x14ac:dyDescent="0.25">
+      <c r="AG40" s="59" t="s">
+        <v>3</v>
+      </c>
+      <c r="AH40" s="59" t="s">
+        <v>3</v>
+      </c>
+      <c r="AI40" s="59" t="s">
+        <v>3</v>
+      </c>
+      <c r="AJ40" s="59" t="s">
+        <v>3</v>
+      </c>
+      <c r="AK40" s="59" t="s">
+        <v>3</v>
+      </c>
+      <c r="AL40" s="10"/>
+      <c r="AM40" s="109" t="s">
+        <v>19</v>
+      </c>
+      <c r="AN40" s="11"/>
+      <c r="AO40" s="109" t="s">
+        <v>19</v>
+      </c>
+      <c r="AP40" s="11"/>
+      <c r="AQ40" s="11"/>
+      <c r="AR40" s="65" t="s">
+        <v>65</v>
+      </c>
+      <c r="AS40" s="11"/>
+      <c r="AT40" s="12"/>
+    </row>
+    <row r="41" spans="1:47" x14ac:dyDescent="0.25">
+      <c r="AG41" s="59" t="s">
+        <v>3</v>
+      </c>
+      <c r="AH41" s="59" t="s">
+        <v>3</v>
+      </c>
+      <c r="AI41" s="59" t="s">
+        <v>3</v>
+      </c>
+      <c r="AJ41" s="59" t="s">
+        <v>3</v>
+      </c>
+      <c r="AK41" s="59" t="s">
+        <v>3</v>
+      </c>
+      <c r="AL41" s="10"/>
+      <c r="AM41" s="11"/>
+      <c r="AN41" s="11"/>
+      <c r="AO41" s="11"/>
+      <c r="AP41" s="11"/>
+      <c r="AQ41" s="11"/>
+      <c r="AR41" s="109" t="s">
+        <v>19</v>
+      </c>
+      <c r="AS41" s="11"/>
+      <c r="AT41" s="12"/>
+    </row>
+    <row r="42" spans="1:47" x14ac:dyDescent="0.25">
+      <c r="AG42" s="59" t="s">
+        <v>3</v>
+      </c>
+      <c r="AH42" s="59" t="s">
+        <v>3</v>
+      </c>
+      <c r="AI42" s="59" t="s">
+        <v>3</v>
+      </c>
+      <c r="AJ42" s="59" t="s">
+        <v>3</v>
+      </c>
+      <c r="AK42" s="59" t="s">
+        <v>3</v>
+      </c>
+      <c r="AL42" s="108" t="s">
+        <v>19</v>
+      </c>
+      <c r="AM42" s="109" t="s">
+        <v>19</v>
+      </c>
+      <c r="AN42" s="11"/>
+      <c r="AO42" s="109" t="s">
+        <v>19</v>
+      </c>
+      <c r="AP42" s="11"/>
+      <c r="AQ42" s="11"/>
+      <c r="AR42" s="109" t="s">
+        <v>19</v>
+      </c>
+      <c r="AS42" s="11"/>
+      <c r="AT42" s="12"/>
+    </row>
+    <row r="43" spans="1:47" x14ac:dyDescent="0.25">
+      <c r="AG43" s="59" t="s">
+        <v>3</v>
+      </c>
+      <c r="AH43" s="59" t="s">
+        <v>3</v>
+      </c>
+      <c r="AI43" s="59" t="s">
+        <v>3</v>
+      </c>
+      <c r="AJ43" s="59" t="s">
+        <v>3</v>
+      </c>
+      <c r="AK43" s="59" t="s">
+        <v>3</v>
+      </c>
+      <c r="AL43" s="10"/>
+      <c r="AM43" s="11"/>
+      <c r="AN43" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="AO43" s="109" t="s">
+        <v>19</v>
+      </c>
+      <c r="AP43" s="11"/>
+      <c r="AQ43" s="11"/>
+      <c r="AR43" s="109" t="s">
+        <v>19</v>
+      </c>
+      <c r="AS43" s="65" t="s">
+        <v>30</v>
+      </c>
+      <c r="AT43" s="12"/>
+    </row>
+    <row r="44" spans="1:47" x14ac:dyDescent="0.25">
+      <c r="AG44" s="59" t="s">
+        <v>3</v>
+      </c>
+      <c r="AH44" s="59" t="s">
+        <v>3</v>
+      </c>
+      <c r="AI44" s="59" t="s">
+        <v>3</v>
+      </c>
+      <c r="AJ44" s="59" t="s">
+        <v>3</v>
+      </c>
+      <c r="AK44" s="59" t="s">
+        <v>3</v>
+      </c>
+      <c r="AL44" s="162"/>
+      <c r="AM44" s="168" t="s">
+        <v>19</v>
+      </c>
+      <c r="AN44" s="163"/>
+      <c r="AO44" s="168" t="s">
+        <v>19</v>
+      </c>
+      <c r="AP44" s="163" t="s">
+        <v>32</v>
+      </c>
+      <c r="AQ44" s="168" t="s">
+        <v>19</v>
+      </c>
+      <c r="AR44" s="168" t="s">
+        <v>19</v>
+      </c>
+      <c r="AS44" s="168" t="s">
+        <v>19</v>
+      </c>
+      <c r="AT44" s="164" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="45" spans="1:47" x14ac:dyDescent="0.25">
+      <c r="AL45" s="162"/>
+      <c r="AM45" s="168" t="s">
+        <v>19</v>
+      </c>
+      <c r="AN45" s="163"/>
+      <c r="AO45" s="168" t="s">
+        <v>19</v>
+      </c>
+      <c r="AP45" s="171" t="s">
+        <v>66</v>
+      </c>
+      <c r="AQ45" s="163"/>
+      <c r="AR45" s="171" t="s">
+        <v>62</v>
+      </c>
+      <c r="AS45" s="168" t="s">
+        <v>19</v>
+      </c>
+      <c r="AT45" s="164"/>
+    </row>
+    <row r="46" spans="1:47" x14ac:dyDescent="0.25">
+      <c r="AL46" s="162"/>
+      <c r="AM46" s="163"/>
+      <c r="AN46" s="163"/>
+      <c r="AO46" s="168" t="s">
+        <v>19</v>
+      </c>
+      <c r="AP46" s="163"/>
+      <c r="AQ46" s="168" t="s">
+        <v>19</v>
+      </c>
+      <c r="AR46" s="163"/>
+      <c r="AS46" s="168" t="s">
+        <v>19</v>
+      </c>
+      <c r="AT46" s="164"/>
+    </row>
+    <row r="47" spans="1:47" x14ac:dyDescent="0.25">
+      <c r="AL47" s="169" t="s">
+        <v>19</v>
+      </c>
+      <c r="AM47" s="168" t="s">
+        <v>19</v>
+      </c>
+      <c r="AN47" s="168" t="s">
+        <v>19</v>
+      </c>
+      <c r="AO47" s="168" t="s">
+        <v>19</v>
+      </c>
+      <c r="AP47" s="163"/>
+      <c r="AQ47" s="168" t="s">
+        <v>19</v>
+      </c>
+      <c r="AR47" s="163"/>
+      <c r="AS47" s="168" t="s">
+        <v>19</v>
+      </c>
+      <c r="AT47" s="164"/>
+    </row>
+    <row r="48" spans="1:47" x14ac:dyDescent="0.25">
+      <c r="AL48" s="162"/>
+      <c r="AM48" s="163"/>
+      <c r="AN48" s="163"/>
+      <c r="AO48" s="163"/>
+      <c r="AP48" s="163"/>
+      <c r="AQ48" s="163"/>
+      <c r="AR48" s="163"/>
+      <c r="AS48" s="168" t="s">
+        <v>19</v>
+      </c>
+      <c r="AT48" s="173" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="49" spans="38:46" x14ac:dyDescent="0.25">
+      <c r="AL49" s="162"/>
+      <c r="AM49" s="163"/>
+      <c r="AN49" s="163"/>
+      <c r="AO49" s="168" t="s">
+        <v>19</v>
+      </c>
+      <c r="AP49" s="168" t="s">
+        <v>19</v>
+      </c>
+      <c r="AQ49" s="168" t="s">
+        <v>19</v>
+      </c>
+      <c r="AR49" s="163" t="s">
+        <v>67</v>
+      </c>
+      <c r="AS49" s="168" t="s">
+        <v>19</v>
+      </c>
+      <c r="AT49" s="164"/>
+    </row>
+    <row r="50" spans="38:46" x14ac:dyDescent="0.25">
+      <c r="AL50" s="162"/>
+      <c r="AM50" s="163"/>
+      <c r="AN50" s="171" t="s">
+        <v>68</v>
+      </c>
+      <c r="AO50" s="163"/>
+      <c r="AP50" s="163"/>
+      <c r="AQ50" s="163"/>
+      <c r="AR50" s="163"/>
+      <c r="AS50" s="168" t="s">
+        <v>19</v>
+      </c>
+      <c r="AT50" s="173" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="51" spans="38:46" x14ac:dyDescent="0.25">
+      <c r="AL51" s="162"/>
+      <c r="AM51" s="163"/>
+      <c r="AN51" s="168" t="s">
+        <v>19</v>
+      </c>
+      <c r="AO51" s="130" t="s">
+        <v>2</v>
+      </c>
+      <c r="AP51" s="168" t="s">
+        <v>19</v>
+      </c>
+      <c r="AQ51" s="168" t="s">
+        <v>19</v>
+      </c>
+      <c r="AR51" s="168" t="s">
+        <v>19</v>
+      </c>
+      <c r="AS51" s="168" t="s">
+        <v>19</v>
+      </c>
+      <c r="AT51" s="164"/>
+    </row>
+    <row r="52" spans="38:46" x14ac:dyDescent="0.25">
+      <c r="AL52" s="162"/>
+      <c r="AM52" s="163"/>
+      <c r="AN52" s="168" t="s">
+        <v>19</v>
+      </c>
+      <c r="AO52" s="163"/>
+      <c r="AP52" s="163"/>
+      <c r="AQ52" s="163"/>
+      <c r="AR52" s="163"/>
+      <c r="AS52" s="168" t="s">
+        <v>19</v>
+      </c>
+      <c r="AT52" s="173" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="53" spans="38:46" x14ac:dyDescent="0.25">
+      <c r="AL53" s="162"/>
+      <c r="AM53" s="163"/>
+      <c r="AN53" s="168" t="s">
+        <v>19</v>
+      </c>
+      <c r="AO53" s="168" t="s">
+        <v>19</v>
+      </c>
+      <c r="AP53" s="168" t="s">
+        <v>19</v>
+      </c>
+      <c r="AQ53" s="168" t="s">
+        <v>19</v>
+      </c>
+      <c r="AR53" s="163"/>
+      <c r="AS53" s="168" t="s">
+        <v>19</v>
+      </c>
+      <c r="AT53" s="164"/>
+    </row>
+    <row r="54" spans="38:46" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="AL54" s="165"/>
+      <c r="AM54" s="166"/>
+      <c r="AN54" s="166"/>
+      <c r="AO54" s="166"/>
+      <c r="AP54" s="166"/>
+      <c r="AQ54" s="166"/>
+      <c r="AR54" s="172" t="s">
+        <v>69</v>
+      </c>
+      <c r="AS54" s="168" t="s">
+        <v>19</v>
+      </c>
+      <c r="AT54" s="170" t="s">
+        <v>6</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="F16:H16"/>
+    <mergeCell ref="J7:L7"/>
+    <mergeCell ref="O33:Q33"/>
+    <mergeCell ref="U1:W1"/>
+    <mergeCell ref="V12:X12"/>
     <mergeCell ref="AB21:AD21"/>
     <mergeCell ref="AD37:AF37"/>
     <mergeCell ref="AO29:AQ29"/>
     <mergeCell ref="V34:X34"/>
     <mergeCell ref="O1:Q1"/>
-    <mergeCell ref="F16:H16"/>
-    <mergeCell ref="J7:L7"/>
-    <mergeCell ref="O33:Q33"/>
-    <mergeCell ref="U1:W1"/>
-    <mergeCell ref="V12:X12"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -6128,7 +6657,7 @@
   <dimension ref="F2:Q20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="O7" sqref="O7"/>
+      <selection activeCell="K9" sqref="K9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6164,10 +6693,10 @@
     <row r="4" spans="6:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="F4" s="121"/>
       <c r="G4" s="121"/>
-      <c r="H4" s="137">
+      <c r="H4" s="125">
         <v>2</v>
       </c>
-      <c r="I4" s="137">
+      <c r="I4" s="125">
         <v>1</v>
       </c>
       <c r="J4" s="121"/>
@@ -6182,7 +6711,7 @@
     <row r="5" spans="6:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="F5" s="121"/>
       <c r="G5" s="121"/>
-      <c r="H5" s="137">
+      <c r="H5" s="125">
         <v>3</v>
       </c>
       <c r="I5" s="121"/>
@@ -6198,10 +6727,10 @@
     <row r="6" spans="6:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="F6" s="121"/>
       <c r="G6" s="121"/>
-      <c r="H6" s="137">
+      <c r="H6" s="125">
         <v>4</v>
       </c>
-      <c r="I6" s="137">
+      <c r="I6" s="125">
         <v>8</v>
       </c>
       <c r="J6" s="121"/>
@@ -6215,16 +6744,16 @@
     </row>
     <row r="7" spans="6:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="F7" s="121"/>
-      <c r="G7" s="137">
+      <c r="G7" s="125">
         <v>5</v>
       </c>
-      <c r="H7" s="137">
+      <c r="H7" s="125">
         <v>6</v>
       </c>
-      <c r="I7" s="137">
+      <c r="I7" s="125">
         <v>7</v>
       </c>
-      <c r="J7" s="137">
+      <c r="J7" s="125">
         <v>9</v>
       </c>
       <c r="K7" s="121"/>
@@ -6240,10 +6769,10 @@
       <c r="G8" s="121"/>
       <c r="H8" s="121"/>
       <c r="I8" s="121"/>
-      <c r="J8" s="137">
+      <c r="J8" s="125">
         <v>10</v>
       </c>
-      <c r="K8" s="137">
+      <c r="K8" s="125">
         <v>11</v>
       </c>
       <c r="L8" s="121"/>
@@ -6253,13 +6782,15 @@
       <c r="P8" s="121"/>
       <c r="Q8" s="121"/>
     </row>
-    <row r="9" spans="6:17" x14ac:dyDescent="0.25">
+    <row r="9" spans="6:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="F9" s="121"/>
       <c r="G9" s="121"/>
       <c r="H9" s="121"/>
       <c r="I9" s="121"/>
       <c r="J9" s="121"/>
-      <c r="K9" s="121"/>
+      <c r="K9" s="125">
+        <v>12</v>
+      </c>
       <c r="L9" s="121"/>
       <c r="M9" s="121"/>
       <c r="N9" s="121"/>
@@ -6430,7 +6961,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:V10"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+    <sheetView topLeftCell="E1" workbookViewId="0">
       <selection activeCell="J10" sqref="J10"/>
     </sheetView>
   </sheetViews>
@@ -6449,152 +6980,152 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="150" t="s">
+      <c r="A1" s="159" t="s">
         <v>36</v>
       </c>
-      <c r="B1" s="151"/>
-      <c r="C1" s="151"/>
-      <c r="D1" s="152"/>
+      <c r="B1" s="160"/>
+      <c r="C1" s="160"/>
+      <c r="D1" s="161"/>
     </row>
     <row r="2" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A2" s="154"/>
-      <c r="B2" s="154"/>
-      <c r="C2" s="154"/>
-      <c r="D2" s="154"/>
+      <c r="A2" s="136"/>
+      <c r="B2" s="136"/>
+      <c r="C2" s="136"/>
+      <c r="D2" s="136"/>
     </row>
     <row r="3" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A3" s="153" t="s">
+      <c r="A3" s="135" t="s">
         <v>38</v>
       </c>
-      <c r="B3" s="153" t="s">
+      <c r="B3" s="135" t="s">
         <v>39</v>
       </c>
-      <c r="C3" s="153" t="s">
+      <c r="C3" s="135" t="s">
         <v>40</v>
       </c>
-      <c r="D3" s="153" t="s">
+      <c r="D3" s="135" t="s">
         <v>41</v>
       </c>
-      <c r="E3" s="153" t="s">
+      <c r="E3" s="135" t="s">
         <v>42</v>
       </c>
-      <c r="F3" s="153" t="s">
+      <c r="F3" s="135" t="s">
         <v>43</v>
       </c>
-      <c r="G3" s="153" t="s">
+      <c r="G3" s="135" t="s">
         <v>44</v>
       </c>
-      <c r="H3" s="153" t="s">
+      <c r="H3" s="135" t="s">
         <v>45</v>
       </c>
-      <c r="I3" s="153" t="s">
+      <c r="I3" s="135" t="s">
         <v>46</v>
       </c>
-      <c r="J3" s="153" t="s">
+      <c r="J3" s="135" t="s">
         <v>47</v>
       </c>
-      <c r="K3" s="153" t="s">
+      <c r="K3" s="135" t="s">
         <v>48</v>
       </c>
-      <c r="L3" s="153" t="s">
+      <c r="L3" s="135" t="s">
         <v>49</v>
       </c>
-      <c r="M3" s="153" t="s">
+      <c r="M3" s="135" t="s">
         <v>50</v>
       </c>
-      <c r="N3" s="153" t="s">
+      <c r="N3" s="135" t="s">
         <v>51</v>
       </c>
-      <c r="O3" s="153" t="s">
+      <c r="O3" s="135" t="s">
         <v>52</v>
       </c>
-      <c r="P3" s="153" t="s">
+      <c r="P3" s="135" t="s">
         <v>53</v>
       </c>
-      <c r="Q3" s="153" t="s">
+      <c r="Q3" s="135" t="s">
         <v>54</v>
       </c>
-      <c r="R3" s="153" t="s">
+      <c r="R3" s="135" t="s">
         <v>55</v>
       </c>
-      <c r="S3" s="153" t="s">
+      <c r="S3" s="135" t="s">
         <v>56</v>
       </c>
-      <c r="T3" s="153" t="s">
+      <c r="T3" s="135" t="s">
         <v>57</v>
       </c>
-      <c r="U3" s="153" t="s">
+      <c r="U3" s="135" t="s">
         <v>58</v>
       </c>
-      <c r="V3" s="153" t="s">
+      <c r="V3" s="135" t="s">
         <v>59</v>
       </c>
     </row>
     <row r="4" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A4" s="153" t="s">
+      <c r="A4" s="135" t="s">
         <v>37</v>
       </c>
-      <c r="B4" s="153">
+      <c r="B4" s="135">
         <v>522</v>
       </c>
-      <c r="C4" s="153">
+      <c r="C4" s="135">
         <v>54</v>
       </c>
-      <c r="D4" s="153">
+      <c r="D4" s="135">
         <v>82</v>
       </c>
-      <c r="E4" s="153">
+      <c r="E4" s="135">
         <v>28</v>
       </c>
-      <c r="F4" s="153">
+      <c r="F4" s="135">
         <v>347</v>
       </c>
-      <c r="G4" s="153">
+      <c r="G4" s="135">
         <v>342</v>
       </c>
-      <c r="H4" s="153">
+      <c r="H4" s="135">
         <v>352</v>
       </c>
-      <c r="I4" s="153">
+      <c r="I4" s="135">
         <v>39</v>
       </c>
-      <c r="J4" s="153">
+      <c r="J4" s="135">
         <v>600</v>
       </c>
-      <c r="K4" s="153">
+      <c r="K4" s="135">
         <v>927</v>
       </c>
-      <c r="L4" s="153">
+      <c r="L4" s="135">
         <v>115</v>
       </c>
-      <c r="M4" s="153">
+      <c r="M4" s="135">
         <v>92</v>
       </c>
-      <c r="N4" s="153">
+      <c r="N4" s="135">
         <v>137</v>
       </c>
-      <c r="O4" s="153">
+      <c r="O4" s="135">
         <v>96</v>
       </c>
-      <c r="P4" s="153">
+      <c r="P4" s="135">
         <v>97</v>
       </c>
-      <c r="Q4" s="153">
+      <c r="Q4" s="135">
         <v>71</v>
       </c>
-      <c r="R4" s="153">
+      <c r="R4" s="135">
         <v>248</v>
       </c>
-      <c r="S4" s="153">
+      <c r="S4" s="135">
         <v>144</v>
       </c>
-      <c r="T4" s="153">
+      <c r="T4" s="135">
         <v>33</v>
       </c>
-      <c r="U4" s="153">
+      <c r="U4" s="135">
         <v>40</v>
       </c>
-      <c r="V4" s="155">
+      <c r="V4" s="137">
         <f>SUM(B4:U4)</f>
         <v>4366</v>
       </c>

</xml_diff>